<commit_message>
Remove BM_update from ywesee. Use drug information from Packungen.xlsx
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package.xlsx
+++ b/spec/data/swissmedic_package.xlsx
@@ -11,21 +11,21 @@
     <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$19</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">{#name?}</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">{#name?}</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_1" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Sheet1!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Sheet1!#REF!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_1" vbProcedure="false">Sheet1!#REF!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$19</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">sheet1!#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">sheet1!#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">sheet1!#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_1" vbProcedure="false">sheet1!#ref!</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="108">
   <si>
     <t>Zugelassene Packungen / Conditionnements autorisés</t>
   </si>
@@ -36,7 +36,7 @@
     <r>
       <t>* Die Gültigkeitsdauer entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten. Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen / 
   La durée de validité correspond aux données figurant sur le certificat d'autorisation. Les autorisations provisoires, sans report de la date d'expiration, restent réservées. Tous les médicaments énumérés dans la liste sont autorisés au moment de la mise à jour de la liste. 
-** </t>
+**</t>
     </r>
     <r>
       <rPr>
@@ -55,18 +55,16 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t> (Kategorien der Kontrollmassnahmen, denen die Betäubungsmittel unterstellt sind) / Tableaux (catégories de mesures de contrôle auxquelles sont soumis les stupéfiants)
+      <t>(Kategorien der Kontrollmassnahmen, denen die Betäubungsmittel unterstellt sind) / Tableaux (catégories de mesures de contrôle auxquelles sont soumis les stupéfiants)
 a: Unterstehen allen Kontrollmassnahmen (s. auch Anhang a der BetmVV-EDI) / Soumis à toutes les mesures de contrôle (voir aussi le tableau a de l'OTStup-DFI)
 b: Unterstehen nicht allen Kontrollmassnahmen (s. auch Anhang b der BetmVV-EDI) / Soustraits partiellement au contrôle (voir aussi le tableau b de l'OTStup-DFI)
 c: Unterstehen nicht allen Kontrollmassnahmen; in kleinen Mengen ohne Verschreibung erhältlich (s. auch Verzeichnis c der BetmVV-EDI) / Soustraits partiellement au contrôle; pouvant être obtenus en petites quantités sans ordonnance (voir aussi le tableau c de l'OTStup-DFI)
-d: Zugelassene Arzneimittel, die kontrollierte Substanzen des Verzeichnisses d gemäss BetmVV-EDI enthalten / Médicaments autorisés contenant des substances soumises à contrôle figurant dans le tableau d de l'OTStup-DFI
-</t>
+d: Zugelassene Arzneimittel, die kontrollierte Substanzen des Verzeichnisses d gemäss BetmVV-EDI enthalten / Médicaments autorisés contenant des substances soumises à contrôle figurant dans le tableau d de l'OTStup-DFI</t>
     </r>
   </si>
   <si>
     <t>Zulassungs-nummer
-Numéro d'autorisation
-</t>
+Numéro d'autorisation</t>
   </si>
   <si>
     <t>Dosisstärke-nummer
@@ -86,7 +84,7 @@
   </si>
   <si>
     <t>IT-Nummer
-N° IT </t>
+N° IT</t>
   </si>
   <si>
     <t>ATC-Code
@@ -334,6 +332,75 @@
   </si>
   <si>
     <t>Venenmittel für den äusserlichen Gebrauch</t>
+  </si>
+  <si>
+    <t>Insulin Lilly Humalog Flacon, solution injectable</t>
+  </si>
+  <si>
+    <t>Eli Lilly (Suisse) SA</t>
+  </si>
+  <si>
+    <t>Biotechnologika</t>
+  </si>
+  <si>
+    <t>07.06.1.</t>
+  </si>
+  <si>
+    <t>A10AB04</t>
+  </si>
+  <si>
+    <t>1 x 10 ml</t>
+  </si>
+  <si>
+    <t>Flasche(n)</t>
+  </si>
+  <si>
+    <t>insulinum lisprum</t>
+  </si>
+  <si>
+    <t>insulinum lisprum 100 U.I., glycerolum, zincum, natrii phosphates, conserv.: metacresolum 3.15 mg, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Diabète sucré</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Insulinanalog: schnell wirkend</t>
+  </si>
+  <si>
+    <t>Diaphin 10 g i.v., Injektionspräparat</t>
+  </si>
+  <si>
+    <t>DiaMo Narcotics GmbH</t>
+  </si>
+  <si>
+    <t>01.01.3.</t>
+  </si>
+  <si>
+    <t>N07BC06</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>Ampulle(n)</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>diamorphinum</t>
+  </si>
+  <si>
+    <t>diamorphini hydrochloridum monohydricum 10 g corresp. diamorphinum 8.71 g pro vitro.</t>
+  </si>
+  <si>
+    <t>Ergänzung der Behandlung von schwer heroinabhängigen Personen</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -451,7 +518,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -479,8 +546,12 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="48">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -497,7 +568,7 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -517,7 +588,7 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -525,83 +596,71 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -621,20 +680,44 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -661,12 +744,8 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
@@ -674,6 +753,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Standard 2" xfId="20" builtinId="54" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Standard 2" xfId="21" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -683,15 +763,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>38520</xdr:colOff>
+      <xdr:colOff>65520</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>989280</xdr:colOff>
+      <xdr:colOff>1015920</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>29520</xdr:rowOff>
+      <xdr:rowOff>29160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -704,8 +784,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="38520" y="360"/>
-          <a:ext cx="1693440" cy="562320"/>
+          <a:off x="65520" y="360"/>
+          <a:ext cx="1693080" cy="561960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -725,10 +805,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:20"/>
+  <dimension ref="1:22"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A20" activeCellId="0" sqref="20:20"/>
+      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="21:22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -772,35 +852,35 @@
       </c>
       <c r="Q1" s="13"/>
       <c r="R1" s="13"/>
-      <c r="S1" s="14"/>
-      <c r="T1" s="14"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="13"/>
       <c r="U1" s="4"/>
       <c r="V1" s="4"/>
       <c r="W1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17"/>
-      <c r="E2" s="18"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="23" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="18"/>
+      <c r="G2" s="19"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="19"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="22" t="s">
         <v>1</v>
       </c>
       <c r="P2" s="0"/>
       <c r="Q2" s="13"/>
       <c r="R2" s="13"/>
-      <c r="S2" s="14"/>
-      <c r="T2" s="14"/>
+      <c r="S2" s="13"/>
+      <c r="T2" s="13"/>
       <c r="U2" s="4"/>
       <c r="V2" s="4"/>
       <c r="W2" s="4"/>
@@ -1807,26 +1887,26 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24"/>
-      <c r="B3" s="24"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="27"/>
-      <c r="G3" s="27"/>
-      <c r="H3" s="28"/>
-      <c r="I3" s="28"/>
-      <c r="J3" s="28"/>
-      <c r="K3" s="24"/>
-      <c r="L3" s="24"/>
-      <c r="M3" s="24"/>
-      <c r="N3" s="24"/>
-      <c r="O3" s="29"/>
-      <c r="P3" s="30"/>
+      <c r="A3" s="23"/>
+      <c r="B3" s="23"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="24"/>
+      <c r="E3" s="25"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+      <c r="I3" s="27"/>
+      <c r="J3" s="27"/>
+      <c r="K3" s="23"/>
+      <c r="L3" s="23"/>
+      <c r="M3" s="23"/>
+      <c r="N3" s="23"/>
+      <c r="O3" s="4"/>
+      <c r="P3" s="4"/>
       <c r="Q3" s="13"/>
       <c r="R3" s="13"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="13"/>
       <c r="U3" s="4"/>
       <c r="V3" s="4"/>
       <c r="W3" s="4"/>
@@ -2833,28 +2913,28 @@
       <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="96.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31" t="s">
+      <c r="A4" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="31"/>
-      <c r="C4" s="31"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="31"/>
-      <c r="F4" s="31"/>
-      <c r="G4" s="31"/>
-      <c r="H4" s="31"/>
-      <c r="I4" s="31"/>
-      <c r="J4" s="31"/>
-      <c r="K4" s="31"/>
-      <c r="L4" s="31"/>
-      <c r="M4" s="31"/>
-      <c r="N4" s="31"/>
-      <c r="O4" s="31"/>
-      <c r="P4" s="32"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="29"/>
       <c r="Q4" s="13"/>
       <c r="R4" s="13"/>
-      <c r="S4" s="14"/>
-      <c r="T4" s="14"/>
+      <c r="S4" s="13"/>
+      <c r="T4" s="13"/>
       <c r="U4" s="4"/>
       <c r="V4" s="4"/>
       <c r="W4" s="4"/>
@@ -3860,1020 +3940,1151 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="38" customFormat="true" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="33" t="s">
+    <row r="5" s="35" customFormat="true" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="33" t="s">
+      <c r="B5" s="30" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="34" t="s">
+      <c r="C5" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="34" t="s">
+      <c r="D5" s="31" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="36" t="s">
+      <c r="G5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="37" t="s">
+      <c r="H5" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="37" t="s">
+      <c r="I5" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="37" t="s">
+      <c r="J5" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="33" t="s">
+      <c r="K5" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="33" t="s">
+      <c r="L5" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="33" t="s">
+      <c r="M5" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="33" t="s">
+      <c r="N5" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="36" t="s">
+      <c r="O5" s="33" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="36" t="s">
+      <c r="P5" s="33" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="35" t="s">
+      <c r="Q5" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="35" t="s">
+      <c r="R5" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="S5" s="35" t="s">
+      <c r="S5" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="T5" s="35" t="s">
+      <c r="T5" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="U5" s="36" t="s">
+      <c r="U5" s="33" t="s">
         <v>23</v>
       </c>
-      <c r="V5" s="36" t="s">
+      <c r="V5" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="W5" s="36" t="s">
+      <c r="W5" s="33" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="39" t="n">
+    <row r="6" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="36" t="n">
         <v>277</v>
       </c>
-      <c r="B6" s="40" t="n">
+      <c r="B6" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="41" t="s">
+      <c r="C6" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="41" t="s">
+      <c r="D6" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="41" t="s">
+      <c r="E6" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="40" t="s">
+      <c r="F6" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="40" t="s">
+      <c r="G6" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="42" t="n">
+      <c r="H6" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I6" s="42" t="n">
+      <c r="I6" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J6" s="42" t="n">
+      <c r="J6" s="39" t="n">
         <v>43946</v>
       </c>
-      <c r="K6" s="43" t="n">
+      <c r="K6" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="L6" s="40" t="s">
+      <c r="L6" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="40" t="s">
+      <c r="M6" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="40" t="s">
+      <c r="N6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="40" t="s">
+      <c r="O6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="40" t="s">
+      <c r="P6" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q6" s="41" t="s">
+      <c r="Q6" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="R6" s="41" t="s">
+      <c r="R6" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="41" t="s">
+      <c r="S6" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="T6" s="41"/>
-      <c r="U6" s="40"/>
-      <c r="V6" s="40"/>
-      <c r="W6" s="40"/>
+      <c r="T6" s="38"/>
+      <c r="U6" s="37"/>
+      <c r="V6" s="37"/>
+      <c r="W6" s="37"/>
     </row>
-    <row r="7" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="39" t="n">
+    <row r="7" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="36" t="n">
         <v>277</v>
       </c>
-      <c r="B7" s="40" t="n">
+      <c r="B7" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="41" t="s">
+      <c r="C7" s="38" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="41" t="s">
+      <c r="D7" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="41" t="s">
+      <c r="E7" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F7" s="40" t="s">
+      <c r="F7" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="40" t="s">
+      <c r="G7" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="42" t="n">
+      <c r="H7" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I7" s="42" t="n">
+      <c r="I7" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J7" s="42" t="n">
+      <c r="J7" s="39" t="n">
         <v>43946</v>
       </c>
-      <c r="K7" s="43" t="n">
+      <c r="K7" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="40" t="s">
+      <c r="L7" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="M7" s="40" t="s">
+      <c r="M7" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N7" s="40" t="s">
+      <c r="N7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="40" t="s">
+      <c r="O7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P7" s="40" t="s">
+      <c r="P7" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="41" t="s">
+      <c r="Q7" s="38" t="s">
         <v>34</v>
       </c>
-      <c r="R7" s="41" t="s">
+      <c r="R7" s="38" t="s">
         <v>35</v>
       </c>
-      <c r="S7" s="41" t="s">
+      <c r="S7" s="38" t="s">
         <v>36</v>
       </c>
-      <c r="T7" s="41"/>
-      <c r="U7" s="40"/>
-      <c r="V7" s="40"/>
-      <c r="W7" s="40"/>
+      <c r="T7" s="38"/>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="37"/>
     </row>
-    <row r="8" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="39" t="n">
+    <row r="8" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="36" t="n">
         <v>278</v>
       </c>
-      <c r="B8" s="40" t="n">
+      <c r="B8" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="41" t="s">
+      <c r="C8" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D8" s="41" t="s">
+      <c r="D8" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F8" s="40" t="s">
+      <c r="F8" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G8" s="40" t="s">
+      <c r="G8" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H8" s="42" t="n">
+      <c r="H8" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I8" s="42" t="n">
+      <c r="I8" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J8" s="42" t="n">
+      <c r="J8" s="39" t="n">
         <v>43946</v>
       </c>
-      <c r="K8" s="43" t="n">
+      <c r="K8" s="40" t="n">
         <v>1</v>
       </c>
-      <c r="L8" s="40" t="s">
+      <c r="L8" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="M8" s="40" t="s">
+      <c r="M8" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N8" s="40" t="s">
+      <c r="N8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="40" t="s">
+      <c r="O8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="40" t="s">
+      <c r="P8" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="41" t="s">
+      <c r="Q8" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="41" t="s">
+      <c r="R8" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="S8" s="41" t="s">
+      <c r="S8" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="T8" s="41"/>
-      <c r="U8" s="40"/>
-      <c r="V8" s="40"/>
-      <c r="W8" s="40"/>
+      <c r="T8" s="38"/>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="37"/>
     </row>
-    <row r="9" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="45" t="n">
+    <row r="9" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="41" t="n">
         <v>278</v>
       </c>
-      <c r="B9" s="40" t="n">
+      <c r="B9" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="38" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="41" t="s">
+      <c r="D9" s="38" t="s">
         <v>27</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="38" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="40" t="s">
+      <c r="F9" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="G9" s="40" t="s">
+      <c r="G9" s="37" t="s">
         <v>30</v>
       </c>
-      <c r="H9" s="42" t="n">
+      <c r="H9" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="I9" s="42" t="n">
+      <c r="I9" s="39" t="n">
         <v>40294</v>
       </c>
-      <c r="J9" s="42" t="n">
+      <c r="J9" s="39" t="n">
         <v>43946</v>
       </c>
-      <c r="K9" s="43" t="n">
+      <c r="K9" s="40" t="n">
         <v>2</v>
       </c>
-      <c r="L9" s="40" t="s">
+      <c r="L9" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="M9" s="40" t="s">
+      <c r="M9" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="N9" s="40" t="s">
+      <c r="N9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="40" t="s">
+      <c r="O9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P9" s="40" t="s">
+      <c r="P9" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q9" s="41" t="s">
+      <c r="Q9" s="38" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="41" t="s">
+      <c r="R9" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="S9" s="41" t="s">
+      <c r="S9" s="38" t="s">
         <v>41</v>
       </c>
-      <c r="T9" s="41"/>
-      <c r="U9" s="40"/>
-      <c r="V9" s="40"/>
-      <c r="W9" s="40"/>
+      <c r="T9" s="38"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
     </row>
-    <row r="10" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="39" t="n">
+    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="36" t="n">
         <v>47066</v>
       </c>
-      <c r="B10" s="40" t="n">
+      <c r="B10" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="41" t="s">
+      <c r="D10" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E10" s="41" t="s">
+      <c r="E10" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40" t="s">
+      <c r="F10" s="37"/>
+      <c r="G10" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="H10" s="42" t="n">
+      <c r="H10" s="39" t="n">
         <v>31239</v>
       </c>
-      <c r="I10" s="42" t="n">
+      <c r="I10" s="39" t="n">
         <v>31239</v>
       </c>
-      <c r="J10" s="42" t="n">
+      <c r="J10" s="39" t="n">
         <v>43779</v>
       </c>
-      <c r="K10" s="43" t="n">
+      <c r="K10" s="40" t="n">
         <v>18</v>
       </c>
-      <c r="L10" s="40" t="s">
+      <c r="L10" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="M10" s="40" t="s">
+      <c r="M10" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N10" s="40" t="s">
+      <c r="N10" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="40" t="s">
+      <c r="O10" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P10" s="40" t="s">
+      <c r="P10" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="41" t="s">
+      <c r="Q10" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="R10" s="41" t="s">
+      <c r="R10" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="S10" s="41" t="s">
+      <c r="S10" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="T10" s="41"/>
-      <c r="U10" s="40"/>
-      <c r="V10" s="40"/>
-      <c r="W10" s="40"/>
+      <c r="T10" s="38"/>
+      <c r="U10" s="37"/>
+      <c r="V10" s="37"/>
+      <c r="W10" s="37"/>
     </row>
-    <row r="11" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="39" t="n">
+    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="36" t="n">
         <v>47066</v>
       </c>
-      <c r="B11" s="40" t="n">
+      <c r="B11" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="41" t="s">
+      <c r="C11" s="38" t="s">
         <v>42</v>
       </c>
-      <c r="D11" s="41" t="s">
+      <c r="D11" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40" t="s">
+      <c r="F11" s="37"/>
+      <c r="G11" s="37" t="s">
         <v>45</v>
       </c>
-      <c r="H11" s="42" t="n">
+      <c r="H11" s="39" t="n">
         <v>31239</v>
       </c>
-      <c r="I11" s="42" t="n">
+      <c r="I11" s="39" t="n">
         <v>31239</v>
       </c>
-      <c r="J11" s="42" t="n">
+      <c r="J11" s="39" t="n">
         <v>43779</v>
       </c>
-      <c r="K11" s="43" t="n">
+      <c r="K11" s="40" t="n">
         <v>26</v>
       </c>
-      <c r="L11" s="40" t="s">
+      <c r="L11" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="M11" s="40" t="s">
+      <c r="M11" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N11" s="40" t="s">
+      <c r="N11" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="40" t="s">
+      <c r="O11" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P11" s="40" t="s">
+      <c r="P11" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="41" t="s">
+      <c r="Q11" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="R11" s="41" t="s">
+      <c r="R11" s="38" t="s">
         <v>49</v>
       </c>
-      <c r="S11" s="41" t="s">
+      <c r="S11" s="38" t="s">
         <v>50</v>
       </c>
-      <c r="T11" s="41"/>
-      <c r="U11" s="40"/>
-      <c r="V11" s="40"/>
-      <c r="W11" s="40"/>
+      <c r="T11" s="38"/>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="37"/>
     </row>
-    <row r="12" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="39" t="n">
+    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="36" t="n">
         <v>48624</v>
       </c>
-      <c r="B12" s="40" t="n">
+      <c r="B12" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="41" t="s">
+      <c r="C12" s="38" t="s">
         <v>52</v>
       </c>
-      <c r="D12" s="41" t="s">
+      <c r="D12" s="38" t="s">
         <v>53</v>
       </c>
-      <c r="E12" s="41" t="s">
+      <c r="E12" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F12" s="40" t="s">
+      <c r="F12" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="40" t="s">
+      <c r="G12" s="37" t="s">
         <v>56</v>
       </c>
-      <c r="H12" s="42" t="n">
+      <c r="H12" s="39" t="n">
         <v>31860</v>
       </c>
-      <c r="I12" s="42" t="n">
+      <c r="I12" s="39" t="n">
         <v>36859</v>
       </c>
-      <c r="J12" s="42" t="n">
+      <c r="J12" s="39" t="n">
         <v>42701</v>
       </c>
-      <c r="K12" s="43" t="n">
+      <c r="K12" s="40" t="n">
         <v>22</v>
       </c>
-      <c r="L12" s="40" t="s">
+      <c r="L12" s="37" t="s">
         <v>57</v>
       </c>
-      <c r="M12" s="40" t="s">
+      <c r="M12" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="N12" s="40" t="s">
+      <c r="N12" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="O12" s="40" t="s">
+      <c r="O12" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="P12" s="40" t="s">
+      <c r="P12" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="Q12" s="41" t="s">
+      <c r="Q12" s="38" t="s">
         <v>60</v>
       </c>
-      <c r="R12" s="41" t="s">
+      <c r="R12" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="S12" s="41" t="s">
+      <c r="S12" s="38" t="s">
         <v>62</v>
       </c>
-      <c r="T12" s="41"/>
-      <c r="U12" s="40"/>
-      <c r="V12" s="40"/>
-      <c r="W12" s="40"/>
+      <c r="T12" s="38"/>
+      <c r="U12" s="37"/>
+      <c r="V12" s="37"/>
+      <c r="W12" s="37"/>
     </row>
-    <row r="13" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="39" t="n">
+    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="36" t="n">
         <v>62069</v>
       </c>
-      <c r="B13" s="40" t="n">
+      <c r="B13" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="41" t="s">
+      <c r="C13" s="38" t="s">
         <v>63</v>
       </c>
-      <c r="D13" s="41" t="s">
+      <c r="D13" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E13" s="41" t="s">
+      <c r="E13" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F13" s="40" t="s">
+      <c r="F13" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="40" t="s">
+      <c r="G13" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="42" t="n">
+      <c r="H13" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="I13" s="42" t="n">
+      <c r="I13" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="J13" s="42" t="n">
+      <c r="J13" s="39" t="n">
         <v>42436</v>
       </c>
-      <c r="K13" s="43" t="n">
+      <c r="K13" s="40" t="n">
         <v>8</v>
       </c>
-      <c r="L13" s="40" t="s">
+      <c r="L13" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="M13" s="40" t="s">
+      <c r="M13" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N13" s="40" t="s">
+      <c r="N13" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O13" s="40" t="s">
+      <c r="O13" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P13" s="40" t="s">
+      <c r="P13" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q13" s="41" t="s">
+      <c r="Q13" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="R13" s="41" t="s">
+      <c r="R13" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="S13" s="41" t="s">
+      <c r="S13" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="T13" s="41"/>
-      <c r="U13" s="40"/>
-      <c r="V13" s="40"/>
-      <c r="W13" s="40"/>
+      <c r="T13" s="38"/>
+      <c r="U13" s="37"/>
+      <c r="V13" s="37"/>
+      <c r="W13" s="37"/>
     </row>
-    <row r="14" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="39" t="n">
+    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="36" t="n">
         <v>62069</v>
       </c>
-      <c r="B14" s="40" t="n">
+      <c r="B14" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="41" t="s">
+      <c r="C14" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D14" s="41" t="s">
+      <c r="D14" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E14" s="41" t="s">
+      <c r="E14" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F14" s="40" t="s">
+      <c r="F14" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="G14" s="40" t="s">
+      <c r="G14" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H14" s="42" t="n">
+      <c r="H14" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="I14" s="42" t="n">
+      <c r="I14" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="J14" s="42" t="n">
+      <c r="J14" s="39" t="n">
         <v>42436</v>
       </c>
-      <c r="K14" s="43" t="n">
+      <c r="K14" s="40" t="n">
         <v>9</v>
       </c>
-      <c r="L14" s="40" t="s">
+      <c r="L14" s="37" t="s">
         <v>72</v>
       </c>
-      <c r="M14" s="40" t="s">
+      <c r="M14" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N14" s="40" t="s">
+      <c r="N14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O14" s="40" t="s">
+      <c r="O14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P14" s="40" t="s">
+      <c r="P14" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q14" s="41" t="s">
+      <c r="Q14" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="R14" s="41" t="s">
+      <c r="R14" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="S14" s="41" t="s">
+      <c r="S14" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="T14" s="41"/>
-      <c r="U14" s="40"/>
-      <c r="V14" s="40"/>
-      <c r="W14" s="40"/>
+      <c r="T14" s="38"/>
+      <c r="U14" s="37"/>
+      <c r="V14" s="37"/>
+      <c r="W14" s="37"/>
     </row>
-    <row r="15" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="39" t="n">
+    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="36" t="n">
         <v>62069</v>
       </c>
-      <c r="B15" s="40" t="n">
+      <c r="B15" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="41" t="s">
+      <c r="C15" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="41" t="s">
+      <c r="D15" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E15" s="41" t="s">
+      <c r="E15" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F15" s="40" t="s">
+      <c r="F15" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="G15" s="40" t="s">
+      <c r="G15" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H15" s="42" t="n">
+      <c r="H15" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="I15" s="42" t="n">
+      <c r="I15" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="J15" s="42" t="n">
+      <c r="J15" s="39" t="n">
         <v>42436</v>
       </c>
-      <c r="K15" s="43" t="n">
+      <c r="K15" s="40" t="n">
         <v>10</v>
       </c>
-      <c r="L15" s="40" t="s">
+      <c r="L15" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="M15" s="40" t="s">
+      <c r="M15" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N15" s="40" t="s">
+      <c r="N15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O15" s="40" t="s">
+      <c r="O15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P15" s="40" t="s">
+      <c r="P15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q15" s="41" t="s">
+      <c r="Q15" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="R15" s="41" t="s">
+      <c r="R15" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="S15" s="41" t="s">
+      <c r="S15" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="T15" s="41"/>
-      <c r="U15" s="40"/>
-      <c r="V15" s="40"/>
-      <c r="W15" s="40"/>
+      <c r="T15" s="38"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="37"/>
     </row>
-    <row r="16" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="39" t="n">
+    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="36" t="n">
         <v>62069</v>
       </c>
-      <c r="B16" s="40" t="n">
+      <c r="B16" s="37" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="41" t="s">
+      <c r="C16" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="41" t="s">
+      <c r="D16" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E16" s="41" t="s">
+      <c r="E16" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F16" s="40" t="s">
+      <c r="F16" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="G16" s="40" t="s">
+      <c r="G16" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H16" s="42" t="n">
+      <c r="H16" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="I16" s="42" t="n">
+      <c r="I16" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="J16" s="42" t="n">
+      <c r="J16" s="39" t="n">
         <v>42436</v>
       </c>
-      <c r="K16" s="43" t="n">
+      <c r="K16" s="40" t="n">
         <v>11</v>
       </c>
-      <c r="L16" s="40" t="s">
+      <c r="L16" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="M16" s="40" t="s">
+      <c r="M16" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N16" s="40" t="s">
+      <c r="N16" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O16" s="40" t="s">
+      <c r="O16" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P16" s="40" t="s">
+      <c r="P16" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q16" s="41" t="s">
+      <c r="Q16" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="R16" s="41" t="s">
+      <c r="R16" s="38" t="s">
         <v>73</v>
       </c>
-      <c r="S16" s="41" t="s">
+      <c r="S16" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="T16" s="41"/>
-      <c r="U16" s="40"/>
-      <c r="V16" s="40"/>
-      <c r="W16" s="40"/>
+      <c r="T16" s="38"/>
+      <c r="U16" s="37"/>
+      <c r="V16" s="37"/>
+      <c r="W16" s="37"/>
     </row>
-    <row r="17" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="39" t="n">
+    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="36" t="n">
         <v>62069</v>
       </c>
-      <c r="B17" s="40" t="n">
+      <c r="B17" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="41" t="s">
+      <c r="C17" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="D17" s="41" t="s">
+      <c r="D17" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E17" s="41" t="s">
+      <c r="E17" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F17" s="40" t="s">
+      <c r="F17" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="G17" s="40" t="s">
+      <c r="G17" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H17" s="42" t="n">
+      <c r="H17" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="I17" s="42" t="n">
+      <c r="I17" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="J17" s="42" t="n">
+      <c r="J17" s="39" t="n">
         <v>42436</v>
       </c>
-      <c r="K17" s="43" t="n">
+      <c r="K17" s="40" t="n">
         <v>12</v>
       </c>
-      <c r="L17" s="40" t="s">
+      <c r="L17" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="M17" s="40" t="s">
+      <c r="M17" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N17" s="40" t="s">
+      <c r="N17" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O17" s="40" t="s">
+      <c r="O17" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P17" s="40" t="s">
+      <c r="P17" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q17" s="41" t="s">
+      <c r="Q17" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="R17" s="41" t="s">
+      <c r="R17" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="S17" s="41" t="s">
+      <c r="S17" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="T17" s="41"/>
-      <c r="U17" s="40"/>
-      <c r="V17" s="40"/>
-      <c r="W17" s="40"/>
+      <c r="T17" s="38"/>
+      <c r="U17" s="37"/>
+      <c r="V17" s="37"/>
+      <c r="W17" s="37"/>
     </row>
-    <row r="18" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="39" t="n">
+    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="36" t="n">
         <v>62069</v>
       </c>
-      <c r="B18" s="40" t="n">
+      <c r="B18" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="41" t="s">
+      <c r="C18" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="D18" s="41" t="s">
+      <c r="D18" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E18" s="41" t="s">
+      <c r="E18" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F18" s="40" t="s">
+      <c r="F18" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="40" t="s">
+      <c r="G18" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H18" s="42" t="n">
+      <c r="H18" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="I18" s="42" t="n">
+      <c r="I18" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="J18" s="42" t="n">
+      <c r="J18" s="39" t="n">
         <v>42436</v>
       </c>
-      <c r="K18" s="43" t="n">
+      <c r="K18" s="40" t="n">
         <v>13</v>
       </c>
-      <c r="L18" s="40" t="s">
+      <c r="L18" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="M18" s="40" t="s">
+      <c r="M18" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N18" s="40" t="s">
+      <c r="N18" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O18" s="40" t="s">
+      <c r="O18" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P18" s="40" t="s">
+      <c r="P18" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q18" s="41" t="s">
+      <c r="Q18" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="R18" s="41" t="s">
+      <c r="R18" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="S18" s="41" t="s">
+      <c r="S18" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="T18" s="41"/>
-      <c r="U18" s="40"/>
-      <c r="V18" s="40"/>
-      <c r="W18" s="40"/>
+      <c r="T18" s="38"/>
+      <c r="U18" s="37"/>
+      <c r="V18" s="37"/>
+      <c r="W18" s="37"/>
     </row>
-    <row r="19" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="39" t="n">
+    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="36" t="n">
         <v>62069</v>
       </c>
-      <c r="B19" s="40" t="n">
+      <c r="B19" s="37" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="41" t="s">
+      <c r="C19" s="38" t="s">
         <v>75</v>
       </c>
-      <c r="D19" s="41" t="s">
+      <c r="D19" s="38" t="s">
         <v>64</v>
       </c>
-      <c r="E19" s="41" t="s">
+      <c r="E19" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F19" s="40" t="s">
+      <c r="F19" s="37" t="s">
         <v>65</v>
       </c>
-      <c r="G19" s="40" t="s">
+      <c r="G19" s="37" t="s">
         <v>66</v>
       </c>
-      <c r="H19" s="42" t="n">
+      <c r="H19" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="I19" s="42" t="n">
+      <c r="I19" s="39" t="n">
         <v>40610</v>
       </c>
-      <c r="J19" s="42" t="n">
+      <c r="J19" s="39" t="n">
         <v>42436</v>
       </c>
-      <c r="K19" s="43" t="n">
+      <c r="K19" s="40" t="n">
         <v>14</v>
       </c>
-      <c r="L19" s="40" t="s">
+      <c r="L19" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="M19" s="40" t="s">
+      <c r="M19" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="N19" s="40" t="s">
+      <c r="N19" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="O19" s="40" t="s">
+      <c r="O19" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="P19" s="40" t="s">
+      <c r="P19" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="Q19" s="41" t="s">
+      <c r="Q19" s="38" t="s">
         <v>68</v>
       </c>
-      <c r="R19" s="41" t="s">
+      <c r="R19" s="38" t="s">
         <v>76</v>
       </c>
-      <c r="S19" s="41" t="s">
+      <c r="S19" s="38" t="s">
         <v>70</v>
       </c>
-      <c r="T19" s="41"/>
-      <c r="U19" s="40"/>
-      <c r="V19" s="40"/>
-      <c r="W19" s="40"/>
+      <c r="T19" s="38"/>
+      <c r="U19" s="37"/>
+      <c r="V19" s="37"/>
+      <c r="W19" s="37"/>
     </row>
-    <row r="20" s="44" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="39" t="n">
+    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="36" t="n">
         <v>16105</v>
       </c>
-      <c r="B20" s="40" t="n">
+      <c r="B20" s="37" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="41" t="s">
+      <c r="C20" s="38" t="s">
         <v>77</v>
       </c>
-      <c r="D20" s="41" t="s">
+      <c r="D20" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="40" t="s">
+      <c r="F20" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="G20" s="40" t="s">
+      <c r="G20" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="H20" s="42" t="n">
+      <c r="H20" s="39" t="n">
         <v>18872</v>
       </c>
-      <c r="I20" s="42" t="n">
+      <c r="I20" s="39" t="n">
         <v>18872</v>
       </c>
-      <c r="J20" s="42" t="n">
+      <c r="J20" s="39" t="n">
         <v>43162</v>
       </c>
-      <c r="K20" s="43" t="n">
+      <c r="K20" s="40" t="n">
         <v>58</v>
       </c>
-      <c r="L20" s="40" t="s">
+      <c r="L20" s="37" t="s">
         <v>81</v>
       </c>
-      <c r="M20" s="40" t="s">
+      <c r="M20" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="N20" s="40" t="s">
+      <c r="N20" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="O20" s="40" t="s">
+      <c r="O20" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="P20" s="40" t="s">
+      <c r="P20" s="37" t="s">
         <v>59</v>
       </c>
-      <c r="Q20" s="41" t="s">
+      <c r="Q20" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="R20" s="41" t="s">
+      <c r="R20" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="S20" s="41" t="s">
+      <c r="S20" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="T20" s="41"/>
-      <c r="U20" s="40"/>
-      <c r="V20" s="40"/>
-      <c r="W20" s="40"/>
+      <c r="T20" s="38"/>
+      <c r="U20" s="37"/>
+      <c r="V20" s="37"/>
+      <c r="W20" s="37"/>
+    </row>
+    <row r="21" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="42" t="n">
+        <v>53290</v>
+      </c>
+      <c r="B21" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="C21" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D21" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="E21" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="F21" s="43" t="s">
+        <v>88</v>
+      </c>
+      <c r="G21" s="43" t="s">
+        <v>89</v>
+      </c>
+      <c r="H21" s="45" t="n">
+        <v>35026</v>
+      </c>
+      <c r="I21" s="45" t="n">
+        <v>35026</v>
+      </c>
+      <c r="J21" s="45" t="n">
+        <v>43002</v>
+      </c>
+      <c r="K21" s="46" t="n">
+        <v>19</v>
+      </c>
+      <c r="L21" s="43" t="s">
+        <v>90</v>
+      </c>
+      <c r="M21" s="43" t="s">
+        <v>91</v>
+      </c>
+      <c r="N21" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="O21" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="P21" s="43" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q21" s="44" t="s">
+        <v>92</v>
+      </c>
+      <c r="R21" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="S21" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="T21" s="44"/>
+      <c r="U21" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="V21" s="43" t="s">
+        <v>96</v>
+      </c>
+      <c r="W21" s="43"/>
+    </row>
+    <row r="22" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="42" t="n">
+        <v>55561</v>
+      </c>
+      <c r="B22" s="43" t="n">
+        <v>2</v>
+      </c>
+      <c r="C22" s="44" t="s">
+        <v>97</v>
+      </c>
+      <c r="D22" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="E22" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="F22" s="43" t="s">
+        <v>99</v>
+      </c>
+      <c r="G22" s="43" t="s">
+        <v>100</v>
+      </c>
+      <c r="H22" s="45" t="n">
+        <v>37232</v>
+      </c>
+      <c r="I22" s="45" t="n">
+        <v>37232</v>
+      </c>
+      <c r="J22" s="45" t="n">
+        <v>43732</v>
+      </c>
+      <c r="K22" s="46" t="n">
+        <v>4</v>
+      </c>
+      <c r="L22" s="43" t="s">
+        <v>101</v>
+      </c>
+      <c r="M22" s="43" t="s">
+        <v>102</v>
+      </c>
+      <c r="N22" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="O22" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="P22" s="43" t="s">
+        <v>103</v>
+      </c>
+      <c r="Q22" s="44" t="s">
+        <v>104</v>
+      </c>
+      <c r="R22" s="44" t="s">
+        <v>105</v>
+      </c>
+      <c r="S22" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="T22" s="44"/>
+      <c r="U22" s="43"/>
+      <c r="V22" s="43"/>
+      <c r="W22" s="43" t="s">
+        <v>107</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A4:R19"/>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>

</xml_diff>

<commit_message>
Fixed QTY in XSD. Generate COOL & ORPH
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package.xlsx
+++ b/spec/data/swissmedic_package.xlsx
@@ -5,38 +5,32 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="601" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Zugelassene Packungen" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">{#name?}</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0" vbProcedure="false">{#name?}</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_1" vbProcedure="false">Sheet1!$3:$4</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Sheet1!$A$4:$R$19</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">sheet1!#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">sheet1!#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0_0_0" vbProcedure="false">sheet1!#ref!</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_1" vbProcedure="false">sheet1!#ref!</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="217">
   <si>
     <t>Zugelassene Packungen / Conditionnements autorisés</t>
   </si>
   <si>
-    <t>Stand / Etat au: 30.06.2015</t>
+    <t>Stand / Etat au: 31.10.2015</t>
   </si>
   <si>
     <r>
       <t>* Die Gültigkeitsdauer entspricht den Angaben auf der Zulassungsbescheinigung. Provisorische Zulassungen, ohne Erneuerung des Gültigkeitsdatums, sind vorbehalten. Alle in der Liste aufgeführten Arzneimittel sind zum Zeitpunkt der Aktualisierung der Liste zugelassen / 
   La durée de validité correspond aux données figurant sur le certificat d'autorisation. Les autorisations provisoires, sans report de la date d'expiration, restent réservées. Tous les médicaments énumérés dans la liste sont autorisés au moment de la mise à jour de la liste. 
-**</t>
+** </t>
     </r>
     <r>
       <rPr>
@@ -55,16 +49,18 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t>(Kategorien der Kontrollmassnahmen, denen die Betäubungsmittel unterstellt sind) / Tableaux (catégories de mesures de contrôle auxquelles sont soumis les stupéfiants)
+      <t> (Kategorien der Kontrollmassnahmen, denen die Betäubungsmittel unterstellt sind) / Tableaux (catégories de mesures de contrôle auxquelles sont soumis les stupéfiants)
 a: Unterstehen allen Kontrollmassnahmen (s. auch Anhang a der BetmVV-EDI) / Soumis à toutes les mesures de contrôle (voir aussi le tableau a de l'OTStup-DFI)
 b: Unterstehen nicht allen Kontrollmassnahmen (s. auch Anhang b der BetmVV-EDI) / Soustraits partiellement au contrôle (voir aussi le tableau b de l'OTStup-DFI)
 c: Unterstehen nicht allen Kontrollmassnahmen; in kleinen Mengen ohne Verschreibung erhältlich (s. auch Verzeichnis c der BetmVV-EDI) / Soustraits partiellement au contrôle; pouvant être obtenus en petites quantités sans ordonnance (voir aussi le tableau c de l'OTStup-DFI)
-d: Zugelassene Arzneimittel, die kontrollierte Substanzen des Verzeichnisses d gemäss BetmVV-EDI enthalten / Médicaments autorisés contenant des substances soumises à contrôle figurant dans le tableau d de l'OTStup-DFI</t>
+d: Zugelassene Arzneimittel, die kontrollierte Substanzen des Verzeichnisses d gemäss BetmVV-EDI enthalten / Médicaments autorisés contenant des substances soumises à contrôle figurant dans le tableau d de l'OTStup-DFI
+f:  Zugelassene Arzneimittel, die kontrollierte Substanzen des Verzeichnisses f gemäss BetmVV-EDI enthalten / médicaments autorisés contenant des substances soumises à contrôle figurant dans le tableau f de l'OTStup-DFI</t>
     </r>
   </si>
   <si>
     <t>Zulassungs-nummer
-Numéro d'autorisation</t>
+Numéro d'autorisation
+</t>
   </si>
   <si>
     <t>Dosisstärke-nummer
@@ -84,7 +80,7 @@
   </si>
   <si>
     <t>IT-Nummer
-N° IT</t>
+N° IT </t>
   </si>
   <si>
     <t>ATC-Code
@@ -189,83 +185,509 @@
 Possibilités d'emploi voir information professionnelle</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
-    <t>Colon Sérocytol, suppositoire</t>
-  </si>
-  <si>
-    <t>globulina equina (immunisé avec tissu intestinal porcin)</t>
-  </si>
-  <si>
-    <t>globulina equina (immunisé avec tissu intestinal porcin) 8 mg, propylenglycolum, conserv.: E 216, E 218, excipiens pro suppositorio.</t>
-  </si>
-  <si>
-    <t>Traitement immunomodulant  selon le Dr Thomas
-Possibilités d'emploi voir information professionnelle</t>
-  </si>
-  <si>
-    <t>Caniphedrin 20mg ad us.vet., Tabletten</t>
+    <t>Hirudoid, Creme</t>
+  </si>
+  <si>
+    <t>Medinova AG</t>
+  </si>
+  <si>
+    <t>Synthetika human</t>
+  </si>
+  <si>
+    <t>02.08.2.</t>
+  </si>
+  <si>
+    <t>C05BA</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>heparinoidum (chondroitini polysulfas)</t>
+  </si>
+  <si>
+    <t>heparinoidum (chondroitini polysulfas) 3 mg alcoholes adipis lanae, aromatica, conserv.: E 218, E 216, excipiens ad unguentum pro 1 g.</t>
+  </si>
+  <si>
+    <t>Venenmittel für den äusserlichen Gebrauch</t>
+  </si>
+  <si>
+    <t>W-Tropfen</t>
+  </si>
+  <si>
+    <t>Iromedica AG</t>
+  </si>
+  <si>
+    <t>10.07.0.</t>
+  </si>
+  <si>
+    <t>D11AF</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>ml</t>
+  </si>
+  <si>
+    <t>acidum lacticum, acidum salicylicum</t>
+  </si>
+  <si>
+    <t>acidum lacticum 40.915 mg, acidum salicylicum 100.2 mg, excipiens ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Hühneraugen, Hornhaut, Warzen</t>
+  </si>
+  <si>
+    <t>Ancopir, Injektionslösung</t>
+  </si>
+  <si>
+    <t>Dr. Grossmann AG, Pharmaca</t>
+  </si>
+  <si>
+    <t>07.02.4.</t>
+  </si>
+  <si>
+    <t>A11DB</t>
+  </si>
+  <si>
+    <t>5 x 2 ml</t>
+  </si>
+  <si>
+    <t>Ampulle(n)</t>
+  </si>
+  <si>
+    <t>thiamini hydrochloridum, pyridoxini hydrochloridum, cyanocobalaminum, lidocaini hydrochloridum</t>
+  </si>
+  <si>
+    <t>thiamini hydrochloridum 200 mg, pyridoxini hydrochloridum 50 mg, cyanocobalaminum 1 mg, lidocaini hydrochloridum 10 mg, sorbitolum, conserv.: E 218 1.6 mg, aqua ad iniectabilia q.s. ad solutionem pro 2 ml.</t>
+  </si>
+  <si>
+    <t>Vitamin B1, B6, B12-Präparat</t>
+  </si>
+  <si>
+    <t>Lidocain 1% Streuli, Injektionslösung (Ampullen)</t>
   </si>
   <si>
     <t>Streuli Pharma AG</t>
   </si>
   <si>
-    <t>Tierarzneimittel</t>
-  </si>
-  <si>
-    <t>QG04BX90</t>
-  </si>
-  <si>
-    <t>100</t>
+    <t>01.02.2.</t>
+  </si>
+  <si>
+    <t>N01BB02</t>
+  </si>
+  <si>
+    <t>10 x  2</t>
+  </si>
+  <si>
+    <t>lidocaini hydrochloridum</t>
+  </si>
+  <si>
+    <t>lidocaini hydrochloridum 10 mg, natrii chloridum, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Lokalanaestheticum</t>
+  </si>
+  <si>
+    <t>Ferro-Gradumet, compresse a rilascio prolungato</t>
+  </si>
+  <si>
+    <t>FARMACEUTICA TEOFARMA SUISSE SA</t>
+  </si>
+  <si>
+    <t>06.07.1.</t>
+  </si>
+  <si>
+    <t>B03AA07</t>
+  </si>
+  <si>
+    <t>30</t>
   </si>
   <si>
     <t>Tablette(n)</t>
   </si>
   <si>
-    <t>ephedrini hydrochloridum</t>
-  </si>
-  <si>
-    <t>ephedrini hydrochloridum 20 mg, excipiens pro compresso.</t>
-  </si>
-  <si>
-    <t>Zur Behandlung der Harninkontinenz bei Hunden</t>
-  </si>
-  <si>
-    <t>500</t>
-  </si>
-  <si>
-    <t>Viscotears Tropfgel, Augengel</t>
-  </si>
-  <si>
-    <t>Alcon Switzerland SA</t>
-  </si>
-  <si>
-    <t>Synthetika human</t>
-  </si>
-  <si>
-    <t>11.08.2.</t>
-  </si>
-  <si>
-    <t>S01XA20</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>carbomerum 980</t>
-  </si>
-  <si>
-    <t>carbomerum 980 2 mg, conserv.: cetrimidum, excipiens ad gelatum pro 1 g.</t>
-  </si>
-  <si>
-    <t>Tränenflüssigkeitsersatz</t>
+    <t>C</t>
+  </si>
+  <si>
+    <t>ferrum(II)</t>
+  </si>
+  <si>
+    <t>ferrum(II) 105 mg ut ferrosi sulfas dessiccatus, arom.: saccharinum natricum, color.: E 127, excipiens pro compresso.</t>
+  </si>
+  <si>
+    <t>Anemia da carenza di ferro con carenza di ferro accertata</t>
+  </si>
+  <si>
+    <t>Lansoyl, gelée</t>
+  </si>
+  <si>
+    <t>Actipharm SA</t>
+  </si>
+  <si>
+    <t>04.08.11</t>
+  </si>
+  <si>
+    <t>A06AA01</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>paraffinum liquidum</t>
+  </si>
+  <si>
+    <t>paraffinum liquidum 782.3 mg, saccharum, arom.: vanillinum, ethylvanillinum et alia, color.: E 124, excipiens ad gelatum pro 1 g.</t>
+  </si>
+  <si>
+    <t>Laxatif</t>
+  </si>
+  <si>
+    <t>Kendural, compresse a rilascio prolungato</t>
+  </si>
+  <si>
+    <t>B03AE10</t>
+  </si>
+  <si>
+    <t>ferrum(II), acidum ascorbicum</t>
+  </si>
+  <si>
+    <t>ferrum(II) 105 mg ut ferrosi sulfas dessiccatus, acidum ascorbicum 500 mg ut natrii ascorbas, color.: E 124, excipiens pro compresso obducto.</t>
+  </si>
+  <si>
+    <t>Kamillin Medipharm, Bad</t>
+  </si>
+  <si>
+    <t>Phytotherapeutika</t>
+  </si>
+  <si>
+    <t>10.08.0.</t>
+  </si>
+  <si>
+    <t>D03AX</t>
+  </si>
+  <si>
+    <t>10 x 40</t>
+  </si>
+  <si>
+    <t>matricariae extractum isopropanolicum liquidum</t>
+  </si>
+  <si>
+    <t>matricariae extractum isopropanolicum liquidum 98.9 g corresp. levomenolum 10-50 mg, ratio: 1:2-2.8, excipiens ad solutionem pro 100 g.</t>
+  </si>
+  <si>
+    <t>Bei Hauterkrankungen</t>
+  </si>
+  <si>
+    <t>Rocephin 500 mg i.v., Trockenampullen + Solvens</t>
+  </si>
+  <si>
+    <t>Roche Pharma (Schweiz) AG</t>
+  </si>
+  <si>
+    <t>08.01.3.</t>
+  </si>
+  <si>
+    <t>J01DD04</t>
+  </si>
+  <si>
+    <t>5 + 5</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>ceftriaxonum</t>
+  </si>
+  <si>
+    <t>Praeparatio sicca: ceftriaxonum 500 mg ut ceftriaxonum natricum pro vitro.
+Solvens: aqua ad iniectabilia 5 ml.</t>
+  </si>
+  <si>
+    <t>Infektionskrankheiten</t>
+  </si>
+  <si>
+    <t>Magnesiumchlorid 0,5 molar B. Braun, Zusatzampulle für              Infusionslösungen</t>
+  </si>
+  <si>
+    <t>B. Braun Medical AG</t>
+  </si>
+  <si>
+    <t>05.03.2.</t>
+  </si>
+  <si>
+    <t>B05XA11</t>
+  </si>
+  <si>
+    <t>5 x 10 mL</t>
+  </si>
+  <si>
+    <t>magnesium, chloridum</t>
+  </si>
+  <si>
+    <t>magnesium 500 mmol, chloridum 1000 mmol, aqua ad iniectabilia q.s. ad solutionem pro 1000 ml.</t>
+  </si>
+  <si>
+    <t>Magnesiummangel</t>
+  </si>
+  <si>
+    <t>Insulin Lilly Humalog Flacon, solution injectable</t>
+  </si>
+  <si>
+    <t>Eli Lilly (Suisse) SA</t>
+  </si>
+  <si>
+    <t>Biotechnologika</t>
+  </si>
+  <si>
+    <t>07.06.1.</t>
+  </si>
+  <si>
+    <t>A10AB04</t>
+  </si>
+  <si>
+    <t>1 x 10 ml</t>
+  </si>
+  <si>
+    <t>Flasche(n)</t>
+  </si>
+  <si>
+    <t>insulinum lisprum</t>
+  </si>
+  <si>
+    <t>insulinum lisprum 100 U.I., glycerolum, zincum, natrii phosphates, conserv.: metacresolum 3.15 mg, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Diabète sucré</t>
+  </si>
+  <si>
+    <t>X</t>
+  </si>
+  <si>
+    <t>Insulinanalog: schnell wirkend</t>
+  </si>
+  <si>
+    <t>3TC 150 mg, Filmtabletten</t>
+  </si>
+  <si>
+    <t>ViiV Healthcare GmbH</t>
+  </si>
+  <si>
+    <t>08.03.0.</t>
+  </si>
+  <si>
+    <t>J05AF05</t>
+  </si>
+  <si>
+    <t>60</t>
+  </si>
+  <si>
+    <t>lamivudinum</t>
+  </si>
+  <si>
+    <t>lamivudinum 150 mg, excipiens pro compresso obducto.</t>
+  </si>
+  <si>
+    <t>HIV-Infektionen</t>
+  </si>
+  <si>
+    <t>Naropin 0,2 %, Infusionslösung / Injektionslösung</t>
+  </si>
+  <si>
+    <t>AstraZeneca AG</t>
+  </si>
+  <si>
+    <t>N01BB09</t>
+  </si>
+  <si>
+    <t>5 x 10</t>
+  </si>
+  <si>
+    <t>ropivacainum</t>
+  </si>
+  <si>
+    <t>ropivacaini hydrochloridum 2 mg, natrii chloridum, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
+  </si>
+  <si>
+    <t>Lokalanästhetikum</t>
+  </si>
+  <si>
+    <t>Zyvoxid 600 mg, Filmtabletten</t>
+  </si>
+  <si>
+    <t>Pfizer AG</t>
+  </si>
+  <si>
+    <t>08.01.9.</t>
+  </si>
+  <si>
+    <t>J01XX08</t>
+  </si>
+  <si>
+    <t>linezolidum</t>
+  </si>
+  <si>
+    <t>linezolidum 600 mg, excipiens pro compresso obducto.</t>
+  </si>
+  <si>
+    <t>Diaphin 10 g i.v., Injektionspräparat</t>
+  </si>
+  <si>
+    <t>DiaMo Narcotics GmbH</t>
+  </si>
+  <si>
+    <t>01.01.3.</t>
+  </si>
+  <si>
+    <t>N07BC06</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>diamorphinum</t>
+  </si>
+  <si>
+    <t>diamorphini hydrochloridum monohydricum 10 g corresp. diamorphinum 8.71 g pro vitro.</t>
+  </si>
+  <si>
+    <t>Ergänzung der Behandlung von schwer heroinabhängigen Personen</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>Nutriflex Lipid plus, Infusionsemulsion, 1250ml</t>
+  </si>
+  <si>
+    <t>07.01.2.</t>
+  </si>
+  <si>
+    <t>B05BA10</t>
+  </si>
+  <si>
+    <t>5 x 1250</t>
+  </si>
+  <si>
+    <t>glucosum anhydricum, natrii dihydrogenophosphas dihydricus, zinci acetas dihydricus, isoleucinum, leucinum, lysinum anhydricum, methioninum, phenylalaninum, threoninum, tryptophanum, valinum, argininum, histidinum, alaninum, acidum asparticum, acidum glutamicum, glycinum, prolinum, serinum, natrii hydroxidum, natrii chloridum, natrii acetas trihydricus, kalii acetas, magnesii acetas tetrahydricus, calcii chloridum dihydricum, aminoacida, nitrogenia, carbohydrata, materia crassa, natrium, kalium, magnesium, calcium, zincum, chloridum, phosphas, acetas, sojae oleum, triglycerida saturata media</t>
+  </si>
+  <si>
+    <t>I) Glucoselösung: glucosum anhydricum 150 g ut glucosum monohydricum, natrii dihydrogenophosphas dihydricus 2.34 g, zinci acetas dihydricus 6.58 mg, aqua ad iniectabilia q.s. ad solutionem pro 500 ml.
+II) Fettemulsion: sojae oleum 25 g, triglycerida saturata media 25 g, lecithinum ex ovo, glycerolum, natrii oleas, aqua ad iniectabilia q.s. ad emulsionem pro 250 ml.
+III) Aminosäurenlösung: isoleucinum 2.82 g, leucinum 3.76 g, lysinum anhydricum 2.73 g ut lysinum monohydricum, methioninum 2.35 g, phenylalaninum 4.21 g, threoninum 2.18 g, tryptophanum 680 mg, valinum 3.12 g, argininum 3.24 g, histidinum 1.5 g ut histidini hydrochloridum monohydricum, alaninum 5.82 g, acidum asparticum 1.8 g, acidum glutamicum 4.21 g, glycinum 1.98 g, prolinum 4.08 g, serinum 3.6 g, natrii hydroxidum 0.976 g, natrii chloridum 0.503 g, natrii acetas trihydricus 0.277 g, kalii acetas 3.434 g, magnesii acetas tetrahydricus 0.858 g, calcii chloridum dihydricum 0.588 g, aqua ad iniectabilia q.s. ad solutionem pro 500 ml.
+.
+I) et II) et III) corresp.: aminoacida 38.4 g/l, nitrogenia 5.44 g/l, carbohydrata 120 g/l, materia crassa 40 g/l, natrium 40 mmol/l, kalium 28 mmol/l, magnesium 3.2 mmol/l, calcium 3.2 mmol/l, zincum 0.024 mmol/l, chloridum 36 mmol/l, phosphas 12 mmol/l, acetas 36 mmol/l, in emulsione recenter mixta 1000 ml.
+Corresp. 4240 kJ pro 1 l.</t>
+  </si>
+  <si>
+    <t>Parenterale Ernährung</t>
+  </si>
+  <si>
+    <t>Caverject DC 10, Injektionspräparat</t>
+  </si>
+  <si>
+    <t>05.99.0.</t>
+  </si>
+  <si>
+    <t>G04BE01</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Spritze(n)</t>
+  </si>
+  <si>
+    <t>alprostadilum</t>
+  </si>
+  <si>
+    <t>Praeparatio cryodesiccata: alprostadilum 10 µg, alfadexum, lactosum anhydricum, natrii citras dihydricus, acidum hydrochloridum aut natrii hydroxidum, pro vitro.
+Solvens: conserv.: alcohol benzylicus 4.45 mg, aqua ad iniectabilia q.s. ad solutionem pro 0.5 ml.</t>
+  </si>
+  <si>
+    <t>Erektile Dysfunktion</t>
+  </si>
+  <si>
+    <t>Apligraf</t>
+  </si>
+  <si>
+    <t>Organogenesis Switzerland GmbH</t>
+  </si>
+  <si>
+    <t>Transplantat: Gewebeprodukt</t>
+  </si>
+  <si>
+    <t>10.06.0.</t>
+  </si>
+  <si>
+    <t>75 mm</t>
+  </si>
+  <si>
+    <t>Scheibe(n)/disque(s)</t>
+  </si>
+  <si>
+    <t>Wundbehandlung (Hautäquivalent)</t>
+  </si>
+  <si>
+    <t>Behandlung von chronischen venösen Beinulzera sowie von diabetischen Fussulzera 
+Behandlung von Muco-Gingivalen Läsionen (Anwendung nur nach  Herstellung  mit Rinderhypophysenextrakt aus einem Land Kategorie A)</t>
+  </si>
+  <si>
+    <t>Agrippal, Injektionssuspension</t>
+  </si>
+  <si>
+    <t>Novartis Pharma Schweiz AG</t>
+  </si>
+  <si>
+    <t>Impfstoffe</t>
+  </si>
+  <si>
+    <t>08.08.</t>
+  </si>
+  <si>
+    <t>J07BB02</t>
+  </si>
+  <si>
+    <t>1 x 0.5 ml</t>
+  </si>
+  <si>
+    <t>Fertigspritze(n)</t>
+  </si>
+  <si>
+    <t>haemagglutininum influenzae A (H1N1), neuraminidasum inactivatum (Virus-Stamm A/California/7/2009 (H1N1)-like: reassortant virus NYMC X-181), haemagglutininum influenzae A (H3N2), haemagglutininum influenzae B</t>
+  </si>
+  <si>
+    <t>haemagglutininum influenzae A (H1N1) 15 µg et neuraminidasum inactivatum (Virus-Stamm A/California/7/2009 (H1N1)-like: reassortant virus NYMC X-181), haemagglutininum influenzae A (H3N2) 15 µg et neuraminidasum inactivatum (Virus-Stamm A/Switzerland/9715293/2013 (H3N2)-like: reassortant virus NIB-88), haemagglutininum influenzae B 15 µg et neuraminidasum inactivatum (Virus-Stamm B/Phuket/3073/2013-like: B/Brisbane/9/2014), natrii chloridum, kalii chloridum, kalii dihydrogenophosphas, dinatrii phosphas dihydricus, magnesii chloridum hexahydricum, calcii chloridum dihydricum, aqua ad iniectabilia q.s. ad suspensionem pro 0.5 ml.</t>
+  </si>
+  <si>
+    <t>aktive Immunisierung gegen Influenza, bei Kindern und Erwachsenen</t>
+  </si>
+  <si>
+    <t>Nutriflex Omega special, Infusionsemulsion 625 ml</t>
+  </si>
+  <si>
+    <t>5 x 625 ml</t>
+  </si>
+  <si>
+    <t>Beutel</t>
+  </si>
+  <si>
+    <t>glucosum anhydricum, natrii dihydrogenophosphas dihydricus, zinci acetas dihydricus, isoleucinum, leucinum, lysinum anhydricum, methioninum, phenylalaninum, threoninum, tryptophanum, valinum, argininum, histidinum, alaninum, acidum asparticum, acidum glutamicum, glycinum, prolinum, serinum, natrii hydroxidum, natrii chloridum, natrii acetas trihydricus, kalii acetas, magnesii acetas tetrahydricus, calcii chloridum dihydricum, aminoacida, nitrogenia, carbohydrata, materia crassa, natrium, kalium, magnesium, calcium, zincum, chloridum, phosphas, acetas, sojae oleum, triglycerida saturata media, omega-3 acidorum triglycerida</t>
+  </si>
+  <si>
+    <t>I) Glucoselösung: glucosum anhydricum 90 g ut glucosum monohydricum, natrii dihydrogenophosphas dihydricus 1.56 g, zinci acetas dihydricus 4.39 mg, aqua ad iniectabilia q.s. ad solutionem pro 250 ml.
+II) Fettemulsion: sojae oleum 10 g, triglycerida saturata media 12.5 g, omega-3 acidorum triglycerida 2.5 g, glycerolum, lecithinum ex ovo, natrii oleas, antiox.: E 307 25 mg, aqua ad iniectabilia q.s. ad emulsionem pro 125 ml.
+III) Aminosäurenlösung: isoleucinum 2.06 g, leucinum 2.74 g, lysinum anhydricum 1.99 g ut lysini hydrochloridum, methioninum 1.71 g, phenylalaninum 3.08 g, threoninum 1.59 g, tryptophanum 500 mg, valinum 2.26 g, argininum 2.37 g, histidinum 1.1 g ut histidini hydrochloridum monohydricum, alaninum 4.25 g, acidum asparticum 1.32 g, acidum glutamicum 3.07 g, glycinum 1.45 g, prolinum 2.98 g, serinum 2.63 g, natrii hydroxidum 732 mg, natrii chloridum 237 mg, natrii acetas trihydricus 157 mg, kalii acetas 2.306 g, magnesii acetas tetrahydricus 569 mg, calcii chloridum dihydricum 390 mg, aqua ad iniectabilia q.s. ad solutionem pro 250 ml.
+.
+I) et II) et III) corresp.: aminoacida 57.44 g/l, nitrogenia 8 g/l, carbohydrata 144 g/l, materia crassa 40 g/l, natrium 53.6 mmol/l, kalium 37.6 mmol/l, magnesium 4.24 mmol/l, calcium 4.24 mmol/l, zincum 0.032 mmol/l, chloridum 48 mmol/l, phosphas 16 mmol/l, acetas 48 mmol/l, in emulsione recenter mixta 1000 ml.
+Corresp. 4941 kJ pro 1 l.</t>
   </si>
   <si>
     <t>Levetiracetam Desitin 250 mg, Minipacks mit Mini-Filmtabletten</t>
@@ -280,9 +702,6 @@
     <t>N03AX14</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
     <t>levetiracetamum</t>
   </si>
   <si>
@@ -292,115 +711,31 @@
     <t>Antiepileptikum</t>
   </si>
   <si>
-    <t>Levetiracetam Desitin 500 mg, Minipacks mit Mini-Filmtabletten</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>levetiracetamum 500 mg, excipiens pro compressi obducti pro charta.</t>
-  </si>
-  <si>
-    <t>200</t>
-  </si>
-  <si>
-    <t>Levetiracetam Desitin 1000 mg, Minipacks mit Mini-Filmtabletten</t>
-  </si>
-  <si>
-    <t>levetiracetamum 1000 mg, excipiens pro compressi obducti pro charta.</t>
-  </si>
-  <si>
-    <t>Hirudoid, Creme</t>
-  </si>
-  <si>
-    <t>Medinova AG</t>
-  </si>
-  <si>
-    <t>02.08.2.</t>
-  </si>
-  <si>
-    <t>C05BA</t>
-  </si>
-  <si>
-    <t>40</t>
-  </si>
-  <si>
-    <t>heparinoidum (chondroitini polysulfas)</t>
-  </si>
-  <si>
-    <t>heparinoidum (chondroitini polysulfas) 3 mg alcoholes adipis lanae, aromatica, conserv.: E 218, E 216, excipiens ad unguentum pro 1 g.</t>
-  </si>
-  <si>
-    <t>Venenmittel für den äusserlichen Gebrauch</t>
-  </si>
-  <si>
-    <t>Insulin Lilly Humalog Flacon, solution injectable</t>
-  </si>
-  <si>
-    <t>Eli Lilly (Suisse) SA</t>
-  </si>
-  <si>
-    <t>Biotechnologika</t>
-  </si>
-  <si>
-    <t>07.06.1.</t>
-  </si>
-  <si>
-    <t>A10AB04</t>
-  </si>
-  <si>
-    <t>1 x 10 ml</t>
-  </si>
-  <si>
-    <t>Flasche(n)</t>
-  </si>
-  <si>
-    <t>insulinum lisprum</t>
-  </si>
-  <si>
-    <t>insulinum lisprum 100 U.I., glycerolum, zincum, natrii phosphates, conserv.: metacresolum 3.15 mg, aqua ad iniectabilia q.s. ad solutionem pro 1 ml.</t>
-  </si>
-  <si>
-    <t>Diabète sucré</t>
-  </si>
-  <si>
-    <t>X</t>
-  </si>
-  <si>
-    <t>Insulinanalog: schnell wirkend</t>
-  </si>
-  <si>
-    <t>Diaphin 10 g i.v., Injektionspräparat</t>
-  </si>
-  <si>
-    <t>DiaMo Narcotics GmbH</t>
-  </si>
-  <si>
-    <t>01.01.3.</t>
-  </si>
-  <si>
-    <t>N07BC06</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Ampulle(n)</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>diamorphinum</t>
-  </si>
-  <si>
-    <t>diamorphini hydrochloridum monohydricum 10 g corresp. diamorphinum 8.71 g pro vitro.</t>
-  </si>
-  <si>
-    <t>Ergänzung der Behandlung von schwer heroinabhängigen Personen</t>
-  </si>
-  <si>
-    <t>d</t>
+    <t>Adcetris, Pulver zur Herstellung einer Infusionslösung</t>
+  </si>
+  <si>
+    <t>Takeda Pharma AG</t>
+  </si>
+  <si>
+    <t>07.16.1.</t>
+  </si>
+  <si>
+    <t>L01XC12</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Durchstechflasche(n)</t>
+  </si>
+  <si>
+    <t>brentuximabum vedotinum</t>
+  </si>
+  <si>
+    <t>Praeparatio cryodesiccata: brentuximabum vedotinum 50 mg, acidum citricum monohydricum, natrii citras dihydricus, trehalosum dihydricum, polysorbatum 80, pro vitro.</t>
+  </si>
+  <si>
+    <t>Behandlung des anaplatischen grosszelligen Lymphoms; Behandlung des Hodgkin-Lymphoms</t>
   </si>
 </sst>
 </file>
@@ -409,15 +744,15 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YY;@"/>
-    <numFmt numFmtId="166" formatCode="00000"/>
+    <numFmt numFmtId="165" formatCode="00000"/>
+    <numFmt numFmtId="166" formatCode="DD/MM/YY;@"/>
     <numFmt numFmtId="167" formatCode="000"/>
   </numFmts>
   <fonts count="12">
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="ARIAL"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -518,9 +853,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="22">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
@@ -546,29 +881,41 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+  </cellStyleXfs>
+  <cellXfs count="48">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="48">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -588,79 +935,91 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -680,15 +1039,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -696,31 +1055,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -732,7 +1067,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -740,12 +1075,8 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
@@ -753,7 +1084,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
     <cellStyle name="Standard 2" xfId="20" builtinId="54" customBuiltin="true"/>
-    <cellStyle name="Excel Built-in Standard 2" xfId="21" builtinId="54" customBuiltin="true"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -763,15 +1093,15 @@
   <xdr:twoCellAnchor editAs="absolute">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>65520</xdr:colOff>
+      <xdr:colOff>36360</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>360</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>1015920</xdr:colOff>
+      <xdr:colOff>446040</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>29160</xdr:rowOff>
+      <xdr:rowOff>38520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -784,8 +1114,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="65520" y="360"/>
-          <a:ext cx="1693080" cy="561960"/>
+          <a:off x="36360" y="360"/>
+          <a:ext cx="1686600" cy="571320"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -805,86 +1135,95 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:22"/>
+  <dimension ref="1:28"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A21" activeCellId="0" sqref="21:22"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="6.06632653061225"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="4.46428571428571"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="2" width="57.4336734693878"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="35.0510204081633"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.65816326530612"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8163265306122"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="25.5408163265306"/>
-    <col collapsed="false" hidden="false" max="10" min="8" style="1" width="11.25"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="4.9030612244898"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.2397959183673"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="3" width="31.8826530612245"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="2" width="5.91326530612245"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="2" width="56.1275510204082"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="33.1785714285714"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="2" width="36.7908163265306"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="2" width="59.1428571428571"/>
-    <col collapsed="false" hidden="false" max="1025" min="19" style="2" width="6.91836734693878"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="9.09767441860465"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="2" width="7.4"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="3" width="33.8976744186046"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="3" width="22.9953488372093"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="3" width="15.8976744186047"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="2" width="7.90232558139535"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="2" width="8.09767441860465"/>
+    <col collapsed="false" hidden="false" max="9" min="8" style="4" width="10.2"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="4" width="10.0976744186047"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="4" width="9.1953488372093"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="2" width="11"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="2" width="11.4046511627907"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="5" width="10.4046511627907"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="6" width="10.4046511627907"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="2" width="10.4046511627907"/>
+    <col collapsed="false" hidden="false" max="18" min="17" style="3" width="22.093023255814"/>
+    <col collapsed="false" hidden="false" max="20" min="19" style="3" width="26.4"/>
+    <col collapsed="false" hidden="false" max="22" min="21" style="2" width="16.0976744186047"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="2" width="14.093023255814"/>
+    <col collapsed="false" hidden="false" max="27" min="25" style="7" width="7.2046511627907"/>
+    <col collapsed="false" hidden="false" max="28" min="28" style="7" width="8.4"/>
+    <col collapsed="false" hidden="false" max="29" min="29" style="7" width="7.2046511627907"/>
+    <col collapsed="false" hidden="false" max="30" min="30" style="7" width="14.2"/>
+    <col collapsed="false" hidden="false" max="31" min="31" style="7" width="7.2046511627907"/>
+    <col collapsed="false" hidden="false" max="1025" min="32" style="7" width="5.9953488372093"/>
   </cols>
   <sheetData>
-    <row r="1" s="12" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4"/>
-      <c r="B1" s="5"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="4"/>
-      <c r="L1" s="4"/>
-      <c r="M1" s="5"/>
-      <c r="N1" s="4"/>
-      <c r="O1" s="11" t="s">
+    <row r="1" s="16" customFormat="true" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="8"/>
+      <c r="O1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="4"/>
-      <c r="V1" s="4"/>
-      <c r="W1" s="4"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="14"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="17"/>
-      <c r="F2" s="18"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="15"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="22" t="s">
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="24"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="24"/>
+      <c r="O2" s="27" t="s">
         <v>1</v>
       </c>
       <c r="P2" s="0"/>
-      <c r="Q2" s="13"/>
-      <c r="R2" s="13"/>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
-      <c r="U2" s="4"/>
-      <c r="V2" s="4"/>
-      <c r="W2" s="4"/>
-      <c r="X2" s="0"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="17"/>
+      <c r="S2" s="18"/>
+      <c r="T2" s="18"/>
+      <c r="U2" s="8"/>
+      <c r="V2" s="8"/>
+      <c r="W2" s="8"/>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
       <c r="AA2" s="0"/>
@@ -1887,30 +2226,29 @@
       <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="10.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="23"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="24"/>
-      <c r="D3" s="24"/>
-      <c r="E3" s="25"/>
-      <c r="F3" s="26"/>
-      <c r="G3" s="26"/>
-      <c r="H3" s="27"/>
-      <c r="I3" s="27"/>
-      <c r="J3" s="27"/>
-      <c r="K3" s="23"/>
-      <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-      <c r="N3" s="23"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-      <c r="Q3" s="13"/>
-      <c r="R3" s="13"/>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="4"/>
-      <c r="V3" s="4"/>
-      <c r="W3" s="4"/>
-      <c r="X3" s="0"/>
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="33"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="17"/>
+      <c r="R3" s="17"/>
+      <c r="S3" s="18"/>
+      <c r="T3" s="18"/>
+      <c r="U3" s="8"/>
+      <c r="V3" s="8"/>
+      <c r="W3" s="8"/>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
       <c r="AA3" s="0"/>
@@ -2912,33 +3250,32 @@
       <c r="AMI3" s="0"/>
       <c r="AMJ3" s="0"/>
     </row>
-    <row r="4" customFormat="false" ht="96.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="28" t="s">
+    <row r="4" customFormat="false" ht="102" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="28"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="28"/>
-      <c r="J4" s="28"/>
-      <c r="K4" s="28"/>
-      <c r="L4" s="28"/>
-      <c r="M4" s="28"/>
-      <c r="N4" s="28"/>
-      <c r="O4" s="28"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="13"/>
-      <c r="R4" s="13"/>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
-      <c r="U4" s="4"/>
-      <c r="V4" s="4"/>
-      <c r="W4" s="4"/>
-      <c r="X4" s="0"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
+      <c r="M4" s="35"/>
+      <c r="N4" s="35"/>
+      <c r="O4" s="35"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="17"/>
+      <c r="R4" s="17"/>
+      <c r="S4" s="18"/>
+      <c r="T4" s="18"/>
+      <c r="U4" s="8"/>
+      <c r="V4" s="8"/>
+      <c r="W4" s="8"/>
       <c r="Y4" s="0"/>
       <c r="Z4" s="0"/>
       <c r="AA4" s="0"/>
@@ -3940,1160 +4277,1540 @@
       <c r="AMI4" s="0"/>
       <c r="AMJ4" s="0"/>
     </row>
-    <row r="5" s="35" customFormat="true" ht="117.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="30" t="s">
+    <row r="5" s="42" customFormat="true" ht="61.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="37" t="s">
         <v>3</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="37" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="31" t="s">
+      <c r="C5" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="31" t="s">
+      <c r="D5" s="38" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="32" t="s">
+      <c r="E5" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="33" t="s">
+      <c r="F5" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="33" t="s">
+      <c r="G5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="H5" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="I5" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="J5" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="30" t="s">
+      <c r="K5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="L5" s="30" t="s">
+      <c r="L5" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="M5" s="30" t="s">
+      <c r="M5" s="37" t="s">
         <v>15</v>
       </c>
-      <c r="N5" s="30" t="s">
+      <c r="N5" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="O5" s="33" t="s">
+      <c r="O5" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="P5" s="33" t="s">
+      <c r="P5" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="39" t="s">
         <v>19</v>
       </c>
-      <c r="R5" s="32" t="s">
+      <c r="R5" s="39" t="s">
         <v>20</v>
       </c>
-      <c r="S5" s="32" t="s">
+      <c r="S5" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="T5" s="32" t="s">
+      <c r="T5" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="U5" s="33" t="s">
+      <c r="U5" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="V5" s="33" t="s">
+      <c r="V5" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="W5" s="33" t="s">
+      <c r="W5" s="40" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="n">
+    <row r="6" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="43" t="n">
         <v>277</v>
       </c>
-      <c r="B6" s="37" t="n">
+      <c r="B6" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="C6" s="45" t="s">
         <v>26</v>
       </c>
-      <c r="D6" s="38" t="s">
+      <c r="D6" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="38" t="s">
+      <c r="E6" s="45" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="37" t="s">
+      <c r="F6" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="G6" s="37" t="s">
+      <c r="G6" s="44" t="s">
         <v>30</v>
       </c>
-      <c r="H6" s="39" t="n">
+      <c r="H6" s="46" t="n">
         <v>40294</v>
       </c>
-      <c r="I6" s="39" t="n">
+      <c r="I6" s="46" t="n">
         <v>40294</v>
       </c>
-      <c r="J6" s="39" t="n">
+      <c r="J6" s="46" t="n">
         <v>43946</v>
       </c>
-      <c r="K6" s="40" t="n">
+      <c r="K6" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="L6" s="37" t="s">
+      <c r="L6" s="44" t="s">
         <v>31</v>
       </c>
-      <c r="M6" s="37" t="s">
+      <c r="M6" s="44" t="s">
         <v>32</v>
       </c>
-      <c r="N6" s="37" t="s">
+      <c r="N6" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="O6" s="37" t="s">
+      <c r="O6" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="P6" s="37" t="s">
+      <c r="P6" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="Q6" s="38" t="s">
+      <c r="Q6" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="R6" s="38" t="s">
+      <c r="R6" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="S6" s="38" t="s">
+      <c r="S6" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="T6" s="38"/>
-      <c r="U6" s="37"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
+      <c r="T6" s="45"/>
+      <c r="U6" s="44"/>
+      <c r="V6" s="44"/>
+      <c r="W6" s="44"/>
     </row>
-    <row r="7" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36" t="n">
-        <v>277</v>
-      </c>
-      <c r="B7" s="37" t="n">
+    <row r="7" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="43" t="n">
+        <v>16105</v>
+      </c>
+      <c r="B7" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="38" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="E7" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F7" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="G7" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" s="39" t="n">
-        <v>40294</v>
-      </c>
-      <c r="I7" s="39" t="n">
-        <v>40294</v>
-      </c>
-      <c r="J7" s="39" t="n">
-        <v>43946</v>
-      </c>
-      <c r="K7" s="40" t="n">
+      <c r="C7" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="44" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="44" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" s="46" t="n">
+        <v>18872</v>
+      </c>
+      <c r="I7" s="46" t="n">
+        <v>18872</v>
+      </c>
+      <c r="J7" s="46" t="n">
+        <v>43162</v>
+      </c>
+      <c r="K7" s="47" t="n">
+        <v>58</v>
+      </c>
+      <c r="L7" s="44" t="s">
+        <v>42</v>
+      </c>
+      <c r="M7" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="N7" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="O7" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="P7" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q7" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="R7" s="45" t="s">
+        <v>46</v>
+      </c>
+      <c r="S7" s="45" t="s">
+        <v>47</v>
+      </c>
+      <c r="T7" s="45"/>
+      <c r="U7" s="44"/>
+      <c r="V7" s="44"/>
+      <c r="W7" s="44"/>
+    </row>
+    <row r="8" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="43" t="n">
+        <v>16598</v>
+      </c>
+      <c r="B8" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="44" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="44" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" s="46" t="n">
+        <v>18833</v>
+      </c>
+      <c r="I8" s="46" t="n">
+        <v>18833</v>
+      </c>
+      <c r="J8" s="46" t="n">
+        <v>43085</v>
+      </c>
+      <c r="K8" s="47" t="n">
+        <v>11</v>
+      </c>
+      <c r="L8" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="M8" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="N8" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="O8" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="P8" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q8" s="45" t="s">
+        <v>54</v>
+      </c>
+      <c r="R8" s="45" t="s">
+        <v>55</v>
+      </c>
+      <c r="S8" s="45" t="s">
+        <v>56</v>
+      </c>
+      <c r="T8" s="45"/>
+      <c r="U8" s="44"/>
+      <c r="V8" s="44"/>
+      <c r="W8" s="44"/>
+    </row>
+    <row r="9" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="43" t="n">
+        <v>28486</v>
+      </c>
+      <c r="B9" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="45" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="45" t="s">
+        <v>58</v>
+      </c>
+      <c r="E9" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F9" s="44" t="s">
+        <v>59</v>
+      </c>
+      <c r="G9" s="44" t="s">
+        <v>60</v>
+      </c>
+      <c r="H9" s="46" t="n">
+        <v>22699</v>
+      </c>
+      <c r="I9" s="46" t="n">
+        <v>22699</v>
+      </c>
+      <c r="J9" s="46" t="n">
+        <v>42513</v>
+      </c>
+      <c r="K9" s="47" t="n">
+        <v>14</v>
+      </c>
+      <c r="L9" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="M9" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="N9" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="O9" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="P9" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q9" s="45" t="s">
+        <v>63</v>
+      </c>
+      <c r="R9" s="45" t="s">
+        <v>64</v>
+      </c>
+      <c r="S9" s="45" t="s">
+        <v>65</v>
+      </c>
+      <c r="T9" s="45"/>
+      <c r="U9" s="44"/>
+      <c r="V9" s="44"/>
+      <c r="W9" s="44"/>
+    </row>
+    <row r="10" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="43" t="n">
+        <v>30015</v>
+      </c>
+      <c r="B10" s="44" t="n">
         <v>2</v>
       </c>
-      <c r="L7" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="M7" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="N7" s="37" t="s">
+      <c r="C10" s="45" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F10" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G10" s="44" t="s">
+        <v>69</v>
+      </c>
+      <c r="H10" s="46" t="n">
+        <v>23410</v>
+      </c>
+      <c r="I10" s="46" t="n">
+        <v>23410</v>
+      </c>
+      <c r="J10" s="46" t="n">
+        <v>43552</v>
+      </c>
+      <c r="K10" s="47" t="n">
+        <v>10</v>
+      </c>
+      <c r="L10" s="44" t="s">
+        <v>70</v>
+      </c>
+      <c r="M10" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="N10" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="O7" s="37" t="s">
+      <c r="O10" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="P7" s="37" t="s">
+      <c r="P10" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="Q7" s="38" t="s">
-        <v>34</v>
-      </c>
-      <c r="R7" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="S7" s="38" t="s">
-        <v>36</v>
-      </c>
-      <c r="T7" s="38"/>
-      <c r="U7" s="37"/>
-      <c r="V7" s="37"/>
-      <c r="W7" s="37"/>
+      <c r="Q10" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="R10" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="S10" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="T10" s="45"/>
+      <c r="U10" s="44"/>
+      <c r="V10" s="44"/>
+      <c r="W10" s="44"/>
     </row>
-    <row r="8" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="n">
-        <v>278</v>
-      </c>
-      <c r="B8" s="37" t="n">
+    <row r="11" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="43" t="n">
+        <v>31644</v>
+      </c>
+      <c r="B11" s="44" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H11" s="46" t="n">
+        <v>24645</v>
+      </c>
+      <c r="I11" s="46" t="n">
+        <v>34421</v>
+      </c>
+      <c r="J11" s="46" t="n">
+        <v>42781</v>
+      </c>
+      <c r="K11" s="47" t="n">
+        <v>11</v>
+      </c>
+      <c r="L11" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="M11" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="N11" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="O11" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="P11" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q11" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="R11" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="S11" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="T11" s="45"/>
+      <c r="U11" s="44"/>
+      <c r="V11" s="44"/>
+      <c r="W11" s="44"/>
+    </row>
+    <row r="12" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="43" t="n">
+        <v>32475</v>
+      </c>
+      <c r="B12" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="E8" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="G8" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" s="39" t="n">
-        <v>40294</v>
-      </c>
-      <c r="I8" s="39" t="n">
-        <v>40294</v>
-      </c>
-      <c r="J8" s="39" t="n">
-        <v>43946</v>
-      </c>
-      <c r="K8" s="40" t="n">
+      <c r="C12" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F12" s="44" t="s">
+        <v>86</v>
+      </c>
+      <c r="G12" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="H12" s="46" t="n">
+        <v>24267</v>
+      </c>
+      <c r="I12" s="46" t="n">
+        <v>24267</v>
+      </c>
+      <c r="J12" s="46" t="n">
+        <v>42480</v>
+      </c>
+      <c r="K12" s="47" t="n">
+        <v>19</v>
+      </c>
+      <c r="L12" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="M12" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="N12" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="O12" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q12" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="R12" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="S12" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="T12" s="45"/>
+      <c r="U12" s="44"/>
+      <c r="V12" s="44"/>
+      <c r="W12" s="44"/>
+    </row>
+    <row r="13" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="43" t="n">
+        <v>35366</v>
+      </c>
+      <c r="B13" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="L8" s="37" t="s">
-        <v>31</v>
-      </c>
-      <c r="M8" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="N8" s="37" t="s">
+      <c r="C13" s="45" t="s">
+        <v>92</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="44" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="44" t="s">
+        <v>93</v>
+      </c>
+      <c r="H13" s="46" t="n">
+        <v>25696</v>
+      </c>
+      <c r="I13" s="46" t="n">
+        <v>25696</v>
+      </c>
+      <c r="J13" s="46" t="n">
+        <v>42781</v>
+      </c>
+      <c r="K13" s="47" t="n">
+        <v>16</v>
+      </c>
+      <c r="L13" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="M13" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="N13" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="O13" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="P13" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q13" s="45" t="s">
+        <v>94</v>
+      </c>
+      <c r="R13" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="S13" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="T13" s="45"/>
+      <c r="U13" s="44"/>
+      <c r="V13" s="44"/>
+      <c r="W13" s="44"/>
+    </row>
+    <row r="14" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="43" t="n">
+        <v>43454</v>
+      </c>
+      <c r="B14" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C14" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="D14" s="45" t="s">
+        <v>49</v>
+      </c>
+      <c r="E14" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="F14" s="44" t="s">
+        <v>98</v>
+      </c>
+      <c r="G14" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="H14" s="46" t="n">
+        <v>29650</v>
+      </c>
+      <c r="I14" s="46" t="n">
+        <v>29650</v>
+      </c>
+      <c r="J14" s="46" t="n">
+        <v>43905</v>
+      </c>
+      <c r="K14" s="47" t="n">
+        <v>99</v>
+      </c>
+      <c r="L14" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="M14" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="N14" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="O14" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="P14" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q14" s="45" t="s">
+        <v>101</v>
+      </c>
+      <c r="R14" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="S14" s="45" t="s">
+        <v>103</v>
+      </c>
+      <c r="T14" s="45"/>
+      <c r="U14" s="44"/>
+      <c r="V14" s="44"/>
+      <c r="W14" s="44"/>
+    </row>
+    <row r="15" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="43" t="n">
+        <v>44625</v>
+      </c>
+      <c r="B15" s="44" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="45" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="E15" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F15" s="44" t="s">
+        <v>106</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>107</v>
+      </c>
+      <c r="H15" s="46" t="n">
+        <v>30098</v>
+      </c>
+      <c r="I15" s="46" t="n">
+        <v>30098</v>
+      </c>
+      <c r="J15" s="46" t="n">
+        <v>42842</v>
+      </c>
+      <c r="K15" s="47" t="n">
+        <v>59</v>
+      </c>
+      <c r="L15" s="44" t="s">
+        <v>108</v>
+      </c>
+      <c r="M15" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="N15" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O15" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P15" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q15" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="R15" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="S15" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="T15" s="45"/>
+      <c r="U15" s="44"/>
+      <c r="V15" s="44"/>
+      <c r="W15" s="44"/>
+    </row>
+    <row r="16" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="43" t="n">
+        <v>45882</v>
+      </c>
+      <c r="B16" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C16" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D16" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" s="44" t="s">
+        <v>115</v>
+      </c>
+      <c r="G16" s="44" t="s">
+        <v>116</v>
+      </c>
+      <c r="H16" s="46" t="n">
+        <v>31180</v>
+      </c>
+      <c r="I16" s="46" t="n">
+        <v>31180</v>
+      </c>
+      <c r="J16" s="46" t="n">
+        <v>43340</v>
+      </c>
+      <c r="K16" s="47" t="n">
+        <v>20</v>
+      </c>
+      <c r="L16" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="M16" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="N16" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="O8" s="37" t="s">
+      <c r="O16" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="P8" s="37" t="s">
+      <c r="P16" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="Q8" s="38" t="s">
+      <c r="Q16" s="45" t="s">
+        <v>118</v>
+      </c>
+      <c r="R16" s="45" t="s">
+        <v>119</v>
+      </c>
+      <c r="S16" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="T16" s="45"/>
+      <c r="U16" s="44"/>
+      <c r="V16" s="44"/>
+      <c r="W16" s="44"/>
+    </row>
+    <row r="17" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="43" t="n">
+        <v>53290</v>
+      </c>
+      <c r="B17" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="D17" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="E17" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="F17" s="44" t="s">
+        <v>124</v>
+      </c>
+      <c r="G17" s="44" t="s">
+        <v>125</v>
+      </c>
+      <c r="H17" s="46" t="n">
+        <v>35026</v>
+      </c>
+      <c r="I17" s="46" t="n">
+        <v>35026</v>
+      </c>
+      <c r="J17" s="46" t="n">
+        <v>43002</v>
+      </c>
+      <c r="K17" s="47" t="n">
+        <v>19</v>
+      </c>
+      <c r="L17" s="44" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" s="44" t="s">
+        <v>127</v>
+      </c>
+      <c r="N17" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="O17" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="P17" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q17" s="45" t="s">
+        <v>128</v>
+      </c>
+      <c r="R17" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="S17" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="T17" s="45"/>
+      <c r="U17" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="V17" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="W17" s="44"/>
+    </row>
+    <row r="18" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="43" t="n">
+        <v>53662</v>
+      </c>
+      <c r="B18" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C18" s="45" t="s">
+        <v>133</v>
+      </c>
+      <c r="D18" s="45" t="s">
+        <v>134</v>
+      </c>
+      <c r="E18" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="R8" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="S8" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="T8" s="38"/>
-      <c r="U8" s="37"/>
-      <c r="V8" s="37"/>
-      <c r="W8" s="37"/>
+      <c r="F18" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="H18" s="46" t="n">
+        <v>35123</v>
+      </c>
+      <c r="I18" s="46" t="n">
+        <v>35123</v>
+      </c>
+      <c r="J18" s="46" t="n">
+        <v>42851</v>
+      </c>
+      <c r="K18" s="47" t="n">
+        <v>13</v>
+      </c>
+      <c r="L18" s="44" t="s">
+        <v>137</v>
+      </c>
+      <c r="M18" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="N18" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O18" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P18" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q18" s="45" t="s">
+        <v>138</v>
+      </c>
+      <c r="R18" s="45" t="s">
+        <v>139</v>
+      </c>
+      <c r="S18" s="45" t="s">
+        <v>140</v>
+      </c>
+      <c r="T18" s="45"/>
+      <c r="U18" s="44"/>
+      <c r="V18" s="44"/>
+      <c r="W18" s="44"/>
     </row>
-    <row r="9" s="12" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="41" t="n">
-        <v>278</v>
-      </c>
-      <c r="B9" s="37" t="n">
+    <row r="19" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="43" t="n">
+        <v>54015</v>
+      </c>
+      <c r="B19" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="38" t="s">
-        <v>38</v>
-      </c>
-      <c r="D9" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="38" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="G9" s="37" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" s="39" t="n">
-        <v>40294</v>
-      </c>
-      <c r="I9" s="39" t="n">
-        <v>40294</v>
-      </c>
-      <c r="J9" s="39" t="n">
-        <v>43946</v>
-      </c>
-      <c r="K9" s="40" t="n">
+      <c r="C19" s="45" t="s">
+        <v>141</v>
+      </c>
+      <c r="D19" s="45" t="s">
+        <v>142</v>
+      </c>
+      <c r="E19" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="G19" s="44" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="46" t="n">
+        <v>35488</v>
+      </c>
+      <c r="I19" s="46" t="n">
+        <v>35488</v>
+      </c>
+      <c r="J19" s="46" t="n">
+        <v>42921</v>
+      </c>
+      <c r="K19" s="47" t="n">
+        <v>11</v>
+      </c>
+      <c r="L19" s="44" t="s">
+        <v>144</v>
+      </c>
+      <c r="M19" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="N19" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="O19" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="P19" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q19" s="45" t="s">
+        <v>145</v>
+      </c>
+      <c r="R19" s="45" t="s">
+        <v>146</v>
+      </c>
+      <c r="S19" s="45" t="s">
+        <v>147</v>
+      </c>
+      <c r="T19" s="45"/>
+      <c r="U19" s="44"/>
+      <c r="V19" s="44"/>
+      <c r="W19" s="44"/>
+    </row>
+    <row r="20" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="43" t="n">
+        <v>55558</v>
+      </c>
+      <c r="B20" s="44" t="n">
         <v>2</v>
       </c>
-      <c r="L9" s="37" t="s">
-        <v>37</v>
-      </c>
-      <c r="M9" s="37" t="s">
-        <v>32</v>
-      </c>
-      <c r="N9" s="37" t="s">
+      <c r="C20" s="45" t="s">
+        <v>148</v>
+      </c>
+      <c r="D20" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="E20" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="G20" s="44" t="s">
+        <v>151</v>
+      </c>
+      <c r="H20" s="46" t="n">
+        <v>37232</v>
+      </c>
+      <c r="I20" s="46" t="n">
+        <v>37232</v>
+      </c>
+      <c r="J20" s="46" t="n">
+        <v>42896</v>
+      </c>
+      <c r="K20" s="47" t="n">
+        <v>5</v>
+      </c>
+      <c r="L20" s="44" t="s">
+        <v>52</v>
+      </c>
+      <c r="M20" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="N20" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O20" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P20" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q20" s="45" t="s">
+        <v>152</v>
+      </c>
+      <c r="R20" s="45" t="s">
+        <v>153</v>
+      </c>
+      <c r="S20" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="T20" s="45"/>
+      <c r="U20" s="44"/>
+      <c r="V20" s="44"/>
+      <c r="W20" s="44"/>
+    </row>
+    <row r="21" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="43" t="n">
+        <v>55561</v>
+      </c>
+      <c r="B21" s="44" t="n">
+        <v>2</v>
+      </c>
+      <c r="C21" s="45" t="s">
+        <v>154</v>
+      </c>
+      <c r="D21" s="45" t="s">
+        <v>155</v>
+      </c>
+      <c r="E21" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F21" s="44" t="s">
+        <v>156</v>
+      </c>
+      <c r="G21" s="44" t="s">
+        <v>157</v>
+      </c>
+      <c r="H21" s="46" t="n">
+        <v>37232</v>
+      </c>
+      <c r="I21" s="46" t="n">
+        <v>37232</v>
+      </c>
+      <c r="J21" s="46" t="n">
+        <v>43732</v>
+      </c>
+      <c r="K21" s="47" t="n">
+        <v>4</v>
+      </c>
+      <c r="L21" s="44" t="s">
+        <v>158</v>
+      </c>
+      <c r="M21" s="44" t="s">
+        <v>62</v>
+      </c>
+      <c r="N21" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O21" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P21" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q21" s="45" t="s">
+        <v>159</v>
+      </c>
+      <c r="R21" s="45" t="s">
+        <v>160</v>
+      </c>
+      <c r="S21" s="45" t="s">
+        <v>161</v>
+      </c>
+      <c r="T21" s="45"/>
+      <c r="U21" s="44"/>
+      <c r="V21" s="44"/>
+      <c r="W21" s="44" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="22" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="43" t="n">
+        <v>55594</v>
+      </c>
+      <c r="B22" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C22" s="45" t="s">
+        <v>163</v>
+      </c>
+      <c r="D22" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E22" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="G22" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="H22" s="46" t="n">
+        <v>37172</v>
+      </c>
+      <c r="I22" s="46" t="n">
+        <v>37172</v>
+      </c>
+      <c r="J22" s="46" t="n">
+        <v>43863</v>
+      </c>
+      <c r="K22" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L22" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="M22" s="44" t="s">
+        <v>53</v>
+      </c>
+      <c r="N22" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="O9" s="37" t="s">
+      <c r="O22" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="P9" s="37" t="s">
+      <c r="P22" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="Q9" s="38" t="s">
+      <c r="Q22" s="45" t="s">
+        <v>167</v>
+      </c>
+      <c r="R22" s="45" t="s">
+        <v>168</v>
+      </c>
+      <c r="S22" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="T22" s="45"/>
+      <c r="U22" s="44"/>
+      <c r="V22" s="44"/>
+      <c r="W22" s="44"/>
+    </row>
+    <row r="23" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="43" t="n">
+        <v>55674</v>
+      </c>
+      <c r="B23" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C23" s="45" t="s">
+        <v>170</v>
+      </c>
+      <c r="D23" s="45" t="s">
+        <v>149</v>
+      </c>
+      <c r="E23" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="R9" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="S9" s="38" t="s">
-        <v>41</v>
-      </c>
-      <c r="T9" s="38"/>
-      <c r="U9" s="37"/>
-      <c r="V9" s="37"/>
-      <c r="W9" s="37"/>
+      <c r="F23" s="44" t="s">
+        <v>171</v>
+      </c>
+      <c r="G23" s="44" t="s">
+        <v>172</v>
+      </c>
+      <c r="H23" s="46" t="n">
+        <v>37321</v>
+      </c>
+      <c r="I23" s="46" t="n">
+        <v>37321</v>
+      </c>
+      <c r="J23" s="46" t="n">
+        <v>42798</v>
+      </c>
+      <c r="K23" s="47" t="n">
+        <v>5</v>
+      </c>
+      <c r="L23" s="44" t="s">
+        <v>173</v>
+      </c>
+      <c r="M23" s="44" t="s">
+        <v>174</v>
+      </c>
+      <c r="N23" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O23" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P23" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q23" s="45" t="s">
+        <v>175</v>
+      </c>
+      <c r="R23" s="45" t="s">
+        <v>176</v>
+      </c>
+      <c r="S23" s="45" t="s">
+        <v>177</v>
+      </c>
+      <c r="T23" s="45"/>
+      <c r="U23" s="44"/>
+      <c r="V23" s="44"/>
+      <c r="W23" s="44"/>
     </row>
-    <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="n">
-        <v>47066</v>
-      </c>
-      <c r="B10" s="37" t="n">
+    <row r="24" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="43" t="n">
+        <v>58943</v>
+      </c>
+      <c r="B24" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="C10" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D10" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="E10" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="F10" s="37"/>
-      <c r="G10" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="H10" s="39" t="n">
-        <v>31239</v>
-      </c>
-      <c r="I10" s="39" t="n">
-        <v>31239</v>
-      </c>
-      <c r="J10" s="39" t="n">
+      <c r="C24" s="45" t="s">
+        <v>178</v>
+      </c>
+      <c r="D24" s="45" t="s">
+        <v>179</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>180</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>181</v>
+      </c>
+      <c r="G24" s="44"/>
+      <c r="H24" s="46" t="n">
+        <v>42110</v>
+      </c>
+      <c r="I24" s="46" t="n">
+        <v>42110</v>
+      </c>
+      <c r="J24" s="46" t="n">
+        <v>43936</v>
+      </c>
+      <c r="K24" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L24" s="44" t="s">
+        <v>182</v>
+      </c>
+      <c r="M24" s="44" t="s">
+        <v>183</v>
+      </c>
+      <c r="N24" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O24" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P24" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="45"/>
+      <c r="S24" s="45" t="s">
+        <v>184</v>
+      </c>
+      <c r="T24" s="45" t="s">
+        <v>185</v>
+      </c>
+      <c r="U24" s="44"/>
+      <c r="V24" s="44"/>
+      <c r="W24" s="44"/>
+    </row>
+    <row r="25" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="43" t="n">
+        <v>59267</v>
+      </c>
+      <c r="B25" s="44" t="n">
+        <v>7</v>
+      </c>
+      <c r="C25" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="D25" s="45" t="s">
+        <v>187</v>
+      </c>
+      <c r="E25" s="45" t="s">
+        <v>188</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>189</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>190</v>
+      </c>
+      <c r="H25" s="46" t="n">
+        <v>40128</v>
+      </c>
+      <c r="I25" s="46" t="n">
+        <v>42257</v>
+      </c>
+      <c r="J25" s="46" t="n">
         <v>43779</v>
       </c>
-      <c r="K10" s="40" t="n">
-        <v>18</v>
-      </c>
-      <c r="L10" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="M10" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="37" t="s">
+      <c r="K25" s="47" t="n">
+        <v>11</v>
+      </c>
+      <c r="L25" s="44" t="s">
+        <v>191</v>
+      </c>
+      <c r="M25" s="44" t="s">
+        <v>192</v>
+      </c>
+      <c r="N25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="O10" s="37" t="s">
+      <c r="O25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="P10" s="37" t="s">
+      <c r="P25" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="Q10" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="R10" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="S10" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="T10" s="38"/>
-      <c r="U10" s="37"/>
-      <c r="V10" s="37"/>
-      <c r="W10" s="37"/>
+      <c r="Q25" s="45" t="s">
+        <v>193</v>
+      </c>
+      <c r="R25" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="S25" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="T25" s="45"/>
+      <c r="U25" s="44"/>
+      <c r="V25" s="44"/>
+      <c r="W25" s="44"/>
     </row>
-    <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="n">
-        <v>47066</v>
-      </c>
-      <c r="B11" s="37" t="n">
+    <row r="26" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="43" t="n">
+        <v>61186</v>
+      </c>
+      <c r="B26" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="C11" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="D11" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="E11" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="F11" s="37"/>
-      <c r="G11" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="H11" s="39" t="n">
-        <v>31239</v>
-      </c>
-      <c r="I11" s="39" t="n">
-        <v>31239</v>
-      </c>
-      <c r="J11" s="39" t="n">
-        <v>43779</v>
-      </c>
-      <c r="K11" s="40" t="n">
-        <v>26</v>
-      </c>
-      <c r="L11" s="37" t="s">
-        <v>51</v>
-      </c>
-      <c r="M11" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N11" s="37" t="s">
+      <c r="C26" s="45" t="s">
+        <v>196</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>114</v>
+      </c>
+      <c r="E26" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>164</v>
+      </c>
+      <c r="G26" s="44" t="s">
+        <v>165</v>
+      </c>
+      <c r="H26" s="46" t="n">
+        <v>40522</v>
+      </c>
+      <c r="I26" s="46" t="n">
+        <v>40522</v>
+      </c>
+      <c r="J26" s="46" t="n">
+        <v>44174</v>
+      </c>
+      <c r="K26" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L26" s="44" t="s">
+        <v>197</v>
+      </c>
+      <c r="M26" s="44" t="s">
+        <v>198</v>
+      </c>
+      <c r="N26" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="O11" s="37" t="s">
+      <c r="O26" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="P11" s="37" t="s">
+      <c r="P26" s="44" t="s">
         <v>33</v>
       </c>
-      <c r="Q11" s="38" t="s">
-        <v>48</v>
-      </c>
-      <c r="R11" s="38" t="s">
-        <v>49</v>
-      </c>
-      <c r="S11" s="38" t="s">
-        <v>50</v>
-      </c>
-      <c r="T11" s="38"/>
-      <c r="U11" s="37"/>
-      <c r="V11" s="37"/>
-      <c r="W11" s="37"/>
+      <c r="Q26" s="45" t="s">
+        <v>199</v>
+      </c>
+      <c r="R26" s="45" t="s">
+        <v>200</v>
+      </c>
+      <c r="S26" s="45" t="s">
+        <v>169</v>
+      </c>
+      <c r="T26" s="45"/>
+      <c r="U26" s="44"/>
+      <c r="V26" s="44"/>
+      <c r="W26" s="44"/>
     </row>
-    <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="n">
-        <v>48624</v>
-      </c>
-      <c r="B12" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="C12" s="38" t="s">
-        <v>52</v>
-      </c>
-      <c r="D12" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="E12" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F12" s="37" t="s">
-        <v>55</v>
-      </c>
-      <c r="G12" s="37" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="39" t="n">
-        <v>31860</v>
-      </c>
-      <c r="I12" s="39" t="n">
-        <v>36859</v>
-      </c>
-      <c r="J12" s="39" t="n">
-        <v>42701</v>
-      </c>
-      <c r="K12" s="40" t="n">
-        <v>22</v>
-      </c>
-      <c r="L12" s="37" t="s">
-        <v>57</v>
-      </c>
-      <c r="M12" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="N12" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="O12" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="P12" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q12" s="38" t="s">
-        <v>60</v>
-      </c>
-      <c r="R12" s="38" t="s">
-        <v>61</v>
-      </c>
-      <c r="S12" s="38" t="s">
-        <v>62</v>
-      </c>
-      <c r="T12" s="38"/>
-      <c r="U12" s="37"/>
-      <c r="V12" s="37"/>
-      <c r="W12" s="37"/>
+    <row r="27" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="43" t="n">
+        <v>62069</v>
+      </c>
+      <c r="B27" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C27" s="45" t="s">
+        <v>201</v>
+      </c>
+      <c r="D27" s="45" t="s">
+        <v>202</v>
+      </c>
+      <c r="E27" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F27" s="44" t="s">
+        <v>203</v>
+      </c>
+      <c r="G27" s="44" t="s">
+        <v>204</v>
+      </c>
+      <c r="H27" s="46" t="n">
+        <v>40610</v>
+      </c>
+      <c r="I27" s="46" t="n">
+        <v>40610</v>
+      </c>
+      <c r="J27" s="46" t="n">
+        <v>44262</v>
+      </c>
+      <c r="K27" s="47" t="n">
+        <v>8</v>
+      </c>
+      <c r="L27" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="M27" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="N27" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="O27" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="P27" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q27" s="45" t="s">
+        <v>205</v>
+      </c>
+      <c r="R27" s="45" t="s">
+        <v>206</v>
+      </c>
+      <c r="S27" s="45" t="s">
+        <v>207</v>
+      </c>
+      <c r="T27" s="45"/>
+      <c r="U27" s="44"/>
+      <c r="V27" s="44"/>
+      <c r="W27" s="44"/>
     </row>
-    <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="n">
-        <v>62069</v>
-      </c>
-      <c r="B13" s="37" t="n">
+    <row r="28" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="43" t="n">
+        <v>62132</v>
+      </c>
+      <c r="B28" s="44" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="38" t="s">
-        <v>63</v>
-      </c>
-      <c r="D13" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E13" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F13" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="G13" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="I13" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="J13" s="39" t="n">
-        <v>42436</v>
-      </c>
-      <c r="K13" s="40" t="n">
-        <v>8</v>
-      </c>
-      <c r="L13" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M13" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N13" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="O13" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P13" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q13" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="R13" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="S13" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="T13" s="38"/>
-      <c r="U13" s="37"/>
-      <c r="V13" s="37"/>
-      <c r="W13" s="37"/>
-    </row>
-    <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36" t="n">
-        <v>62069</v>
-      </c>
-      <c r="B14" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="C14" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D14" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F14" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="G14" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H14" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="I14" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="J14" s="39" t="n">
-        <v>42436</v>
-      </c>
-      <c r="K14" s="40" t="n">
-        <v>9</v>
-      </c>
-      <c r="L14" s="37" t="s">
-        <v>72</v>
-      </c>
-      <c r="M14" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N14" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="O14" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P14" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q14" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="R14" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="S14" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="T14" s="38"/>
-      <c r="U14" s="37"/>
-      <c r="V14" s="37"/>
-      <c r="W14" s="37"/>
-    </row>
-    <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="36" t="n">
-        <v>62069</v>
-      </c>
-      <c r="B15" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="C15" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D15" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E15" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="G15" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H15" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="I15" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="J15" s="39" t="n">
-        <v>42436</v>
-      </c>
-      <c r="K15" s="40" t="n">
-        <v>10</v>
-      </c>
-      <c r="L15" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="M15" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N15" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="O15" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P15" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q15" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="R15" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="S15" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="T15" s="38"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="37"/>
-    </row>
-    <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36" t="n">
-        <v>62069</v>
-      </c>
-      <c r="B16" s="37" t="n">
-        <v>2</v>
-      </c>
-      <c r="C16" s="38" t="s">
-        <v>71</v>
-      </c>
-      <c r="D16" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E16" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F16" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="G16" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H16" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="I16" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="J16" s="39" t="n">
-        <v>42436</v>
-      </c>
-      <c r="K16" s="40" t="n">
-        <v>11</v>
-      </c>
-      <c r="L16" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="M16" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N16" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="O16" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P16" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q16" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="R16" s="38" t="s">
-        <v>73</v>
-      </c>
-      <c r="S16" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="T16" s="38"/>
-      <c r="U16" s="37"/>
-      <c r="V16" s="37"/>
-      <c r="W16" s="37"/>
-    </row>
-    <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="36" t="n">
-        <v>62069</v>
-      </c>
-      <c r="B17" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="C17" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="D17" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E17" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F17" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H17" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="I17" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="J17" s="39" t="n">
-        <v>42436</v>
-      </c>
-      <c r="K17" s="40" t="n">
-        <v>12</v>
-      </c>
-      <c r="L17" s="37" t="s">
-        <v>67</v>
-      </c>
-      <c r="M17" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N17" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="O17" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P17" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q17" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="R17" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="S17" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="T17" s="38"/>
-      <c r="U17" s="37"/>
-      <c r="V17" s="37"/>
-      <c r="W17" s="37"/>
-    </row>
-    <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36" t="n">
-        <v>62069</v>
-      </c>
-      <c r="B18" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="C18" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="D18" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E18" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F18" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="G18" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H18" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="I18" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="J18" s="39" t="n">
-        <v>42436</v>
-      </c>
-      <c r="K18" s="40" t="n">
-        <v>13</v>
-      </c>
-      <c r="L18" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="M18" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N18" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="O18" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P18" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q18" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="R18" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="S18" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="T18" s="38"/>
-      <c r="U18" s="37"/>
-      <c r="V18" s="37"/>
-      <c r="W18" s="37"/>
-    </row>
-    <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="n">
-        <v>62069</v>
-      </c>
-      <c r="B19" s="37" t="n">
-        <v>3</v>
-      </c>
-      <c r="C19" s="38" t="s">
-        <v>75</v>
-      </c>
-      <c r="D19" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="E19" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F19" s="37" t="s">
-        <v>65</v>
-      </c>
-      <c r="G19" s="37" t="s">
-        <v>66</v>
-      </c>
-      <c r="H19" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="I19" s="39" t="n">
-        <v>40610</v>
-      </c>
-      <c r="J19" s="39" t="n">
-        <v>42436</v>
-      </c>
-      <c r="K19" s="40" t="n">
-        <v>14</v>
-      </c>
-      <c r="L19" s="37" t="s">
-        <v>74</v>
-      </c>
-      <c r="M19" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="N19" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="O19" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="P19" s="37" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q19" s="38" t="s">
-        <v>68</v>
-      </c>
-      <c r="R19" s="38" t="s">
-        <v>76</v>
-      </c>
-      <c r="S19" s="38" t="s">
-        <v>70</v>
-      </c>
-      <c r="T19" s="38"/>
-      <c r="U19" s="37"/>
-      <c r="V19" s="37"/>
-      <c r="W19" s="37"/>
-    </row>
-    <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="n">
-        <v>16105</v>
-      </c>
-      <c r="B20" s="37" t="n">
+      <c r="C28" s="45" t="s">
+        <v>208</v>
+      </c>
+      <c r="D28" s="45" t="s">
+        <v>209</v>
+      </c>
+      <c r="E28" s="45" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>210</v>
+      </c>
+      <c r="G28" s="44" t="s">
+        <v>211</v>
+      </c>
+      <c r="H28" s="46" t="n">
+        <v>41337</v>
+      </c>
+      <c r="I28" s="46" t="n">
+        <v>41337</v>
+      </c>
+      <c r="J28" s="46" t="n">
+        <v>43162</v>
+      </c>
+      <c r="K28" s="47" t="n">
         <v>1</v>
       </c>
-      <c r="C20" s="38" t="s">
-        <v>77</v>
-      </c>
-      <c r="D20" s="38" t="s">
-        <v>78</v>
-      </c>
-      <c r="E20" s="38" t="s">
-        <v>54</v>
-      </c>
-      <c r="F20" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="G20" s="37" t="s">
-        <v>80</v>
-      </c>
-      <c r="H20" s="39" t="n">
-        <v>18872</v>
-      </c>
-      <c r="I20" s="39" t="n">
-        <v>18872</v>
-      </c>
-      <c r="J20" s="39" t="n">
-        <v>43162</v>
-      </c>
-      <c r="K20" s="40" t="n">
-        <v>58</v>
-      </c>
-      <c r="L20" s="37" t="s">
-        <v>81</v>
-      </c>
-      <c r="M20" s="37" t="s">
-        <v>58</v>
-      </c>
-      <c r="N20" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="O20" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="P20" s="37" t="s">
-        <v>59</v>
-      </c>
-      <c r="Q20" s="38" t="s">
-        <v>82</v>
-      </c>
-      <c r="R20" s="38" t="s">
-        <v>83</v>
-      </c>
-      <c r="S20" s="38" t="s">
-        <v>84</v>
-      </c>
-      <c r="T20" s="38"/>
-      <c r="U20" s="37"/>
-      <c r="V20" s="37"/>
-      <c r="W20" s="37"/>
-    </row>
-    <row r="21" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="42" t="n">
-        <v>53290</v>
-      </c>
-      <c r="B21" s="43" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D21" s="44" t="s">
-        <v>86</v>
-      </c>
-      <c r="E21" s="44" t="s">
-        <v>87</v>
-      </c>
-      <c r="F21" s="43" t="s">
-        <v>88</v>
-      </c>
-      <c r="G21" s="43" t="s">
-        <v>89</v>
-      </c>
-      <c r="H21" s="45" t="n">
-        <v>35026</v>
-      </c>
-      <c r="I21" s="45" t="n">
-        <v>35026</v>
-      </c>
-      <c r="J21" s="45" t="n">
-        <v>43002</v>
-      </c>
-      <c r="K21" s="46" t="n">
-        <v>19</v>
-      </c>
-      <c r="L21" s="43" t="s">
-        <v>90</v>
-      </c>
-      <c r="M21" s="43" t="s">
-        <v>91</v>
-      </c>
-      <c r="N21" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="O21" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="P21" s="43" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q21" s="44" t="s">
-        <v>92</v>
-      </c>
-      <c r="R21" s="44" t="s">
-        <v>93</v>
-      </c>
-      <c r="S21" s="44" t="s">
-        <v>94</v>
-      </c>
-      <c r="T21" s="44"/>
-      <c r="U21" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="V21" s="43" t="s">
-        <v>96</v>
-      </c>
-      <c r="W21" s="43"/>
-    </row>
-    <row r="22" s="47" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="42" t="n">
-        <v>55561</v>
-      </c>
-      <c r="B22" s="43" t="n">
-        <v>2</v>
-      </c>
-      <c r="C22" s="44" t="s">
-        <v>97</v>
-      </c>
-      <c r="D22" s="44" t="s">
-        <v>98</v>
-      </c>
-      <c r="E22" s="44" t="s">
-        <v>54</v>
-      </c>
-      <c r="F22" s="43" t="s">
-        <v>99</v>
-      </c>
-      <c r="G22" s="43" t="s">
-        <v>100</v>
-      </c>
-      <c r="H22" s="45" t="n">
-        <v>37232</v>
-      </c>
-      <c r="I22" s="45" t="n">
-        <v>37232</v>
-      </c>
-      <c r="J22" s="45" t="n">
-        <v>43732</v>
-      </c>
-      <c r="K22" s="46" t="n">
-        <v>4</v>
-      </c>
-      <c r="L22" s="43" t="s">
-        <v>101</v>
-      </c>
-      <c r="M22" s="43" t="s">
-        <v>102</v>
-      </c>
-      <c r="N22" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="O22" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="P22" s="43" t="s">
-        <v>103</v>
-      </c>
-      <c r="Q22" s="44" t="s">
-        <v>104</v>
-      </c>
-      <c r="R22" s="44" t="s">
-        <v>105</v>
-      </c>
-      <c r="S22" s="44" t="s">
-        <v>106</v>
-      </c>
-      <c r="T22" s="44"/>
-      <c r="U22" s="43"/>
-      <c r="V22" s="43"/>
-      <c r="W22" s="43" t="s">
-        <v>107</v>
-      </c>
+      <c r="L28" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="M28" s="44" t="s">
+        <v>213</v>
+      </c>
+      <c r="N28" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="O28" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="P28" s="44" t="s">
+        <v>109</v>
+      </c>
+      <c r="Q28" s="45" t="s">
+        <v>214</v>
+      </c>
+      <c r="R28" s="45" t="s">
+        <v>215</v>
+      </c>
+      <c r="S28" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="T28" s="45"/>
+      <c r="U28" s="44" t="s">
+        <v>131</v>
+      </c>
+      <c r="V28" s="44"/>
+      <c r="W28" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0" right="0" top="0.279861111111111" bottom="0.490277777777778" header="0.511805555555555" footer="0"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <printOptions headings="false" gridLines="true" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.340277777777778" right="0" top="0.275694444444444" bottom="0.472222222222222" header="0.511805555555555" footer="0.0784722222222222"/>
+  <pageSetup paperSize="8" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="overThenDown" orientation="landscape" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
-    <oddFooter>&amp;CSwissmedic · Hallerstrasse 7 · CH-3000 Bern 9 · www.swissmedic.ch · Tel. +41 31 322 02 11 · Fax +41 31 322 02 12&amp;R&amp;P/&amp;N</oddFooter>
+    <oddFooter>&amp;C&amp;9Swissmedic · Hallerstrasse 7 · CH-3000 Bern 9 · www.swissmedic.ch · Tel. +41 58 462 02 11 · Fax +41 58 462 02 12&amp;R&amp;9&amp;P/&amp;N</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed NINCD for LPPV items
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package.xlsx
+++ b/spec/data/swissmedic_package.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="225">
   <si>
     <t>Zugelassene Packungen / Conditionnements autorisés</t>
   </si>
@@ -185,15 +185,45 @@
 Possibilités d'emploi voir information professionnelle</t>
   </si>
   <si>
+    <t>Zymafluor 0.25 mg, Tabletten</t>
+  </si>
+  <si>
+    <t>MEDA Pharma GmbH</t>
+  </si>
+  <si>
+    <t>Synthetika human</t>
+  </si>
+  <si>
+    <t>13.05.1.</t>
+  </si>
+  <si>
+    <t>A01AA01</t>
+  </si>
+  <si>
+    <t>400</t>
+  </si>
+  <si>
+    <t>Tablette(n)</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>fluoridum</t>
+  </si>
+  <si>
+    <t>fluoridum 0.25 mg ut natrii fluoridum, aromatica, excipiens pro compresso.</t>
+  </si>
+  <si>
+    <t>Kariesprophylaxe</t>
+  </si>
+  <si>
     <t>Hirudoid, Creme</t>
   </si>
   <si>
     <t>Medinova AG</t>
   </si>
   <si>
-    <t>Synthetika human</t>
-  </si>
-  <si>
     <t>02.08.2.</t>
   </si>
   <si>
@@ -309,12 +339,6 @@
   </si>
   <si>
     <t>30</t>
-  </si>
-  <si>
-    <t>Tablette(n)</t>
-  </si>
-  <si>
-    <t>C</t>
   </si>
   <si>
     <t>ferrum(II)</t>
@@ -1135,12 +1159,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:28"/>
+  <dimension ref="1:29"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="7:7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4413,7 +4437,7 @@
     </row>
     <row r="7" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="43" t="n">
-        <v>16105</v>
+        <v>15219</v>
       </c>
       <c r="B7" s="44" t="n">
         <v>1</v>
@@ -4434,16 +4458,16 @@
         <v>41</v>
       </c>
       <c r="H7" s="46" t="n">
-        <v>18872</v>
+        <v>18429</v>
       </c>
       <c r="I7" s="46" t="n">
-        <v>18872</v>
+        <v>18429</v>
       </c>
       <c r="J7" s="46" t="n">
-        <v>43162</v>
+        <v>43100</v>
       </c>
       <c r="K7" s="47" t="n">
-        <v>58</v>
+        <v>68</v>
       </c>
       <c r="L7" s="44" t="s">
         <v>42</v>
@@ -4476,7 +4500,7 @@
     </row>
     <row r="8" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="43" t="n">
-        <v>16598</v>
+        <v>16105</v>
       </c>
       <c r="B8" s="44" t="n">
         <v>1</v>
@@ -4497,16 +4521,16 @@
         <v>51</v>
       </c>
       <c r="H8" s="46" t="n">
-        <v>18833</v>
+        <v>18872</v>
       </c>
       <c r="I8" s="46" t="n">
-        <v>18833</v>
+        <v>18872</v>
       </c>
       <c r="J8" s="46" t="n">
-        <v>43085</v>
+        <v>43162</v>
       </c>
       <c r="K8" s="47" t="n">
-        <v>11</v>
+        <v>58</v>
       </c>
       <c r="L8" s="44" t="s">
         <v>52</v>
@@ -4515,22 +4539,22 @@
         <v>53</v>
       </c>
       <c r="N8" s="44" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="O8" s="44" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="P8" s="44" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="Q8" s="45" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R8" s="45" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="S8" s="45" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="T8" s="45"/>
       <c r="U8" s="44"/>
@@ -4539,61 +4563,61 @@
     </row>
     <row r="9" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="43" t="n">
-        <v>28486</v>
+        <v>16598</v>
       </c>
       <c r="B9" s="44" t="n">
         <v>1</v>
       </c>
       <c r="C9" s="45" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D9" s="45" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="E9" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F9" s="44" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G9" s="44" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="H9" s="46" t="n">
-        <v>22699</v>
+        <v>18833</v>
       </c>
       <c r="I9" s="46" t="n">
-        <v>22699</v>
+        <v>18833</v>
       </c>
       <c r="J9" s="46" t="n">
-        <v>42513</v>
+        <v>43085</v>
       </c>
       <c r="K9" s="47" t="n">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="L9" s="44" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M9" s="44" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N9" s="44" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="O9" s="44" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="P9" s="44" t="s">
-        <v>33</v>
+        <v>54</v>
       </c>
       <c r="Q9" s="45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="R9" s="45" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="S9" s="45" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="T9" s="45"/>
       <c r="U9" s="44"/>
@@ -4602,43 +4626,43 @@
     </row>
     <row r="10" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="43" t="n">
-        <v>30015</v>
+        <v>28486</v>
       </c>
       <c r="B10" s="44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C10" s="45" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D10" s="45" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="E10" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F10" s="44" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="G10" s="44" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H10" s="46" t="n">
-        <v>23410</v>
+        <v>22699</v>
       </c>
       <c r="I10" s="46" t="n">
-        <v>23410</v>
+        <v>22699</v>
       </c>
       <c r="J10" s="46" t="n">
-        <v>43552</v>
+        <v>42513</v>
       </c>
       <c r="K10" s="47" t="n">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="L10" s="44" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="M10" s="44" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="N10" s="44" t="s">
         <v>33</v>
@@ -4650,13 +4674,13 @@
         <v>33</v>
       </c>
       <c r="Q10" s="45" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="R10" s="45" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="S10" s="45" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="T10" s="45"/>
       <c r="U10" s="44"/>
@@ -4665,52 +4689,52 @@
     </row>
     <row r="11" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="43" t="n">
-        <v>31644</v>
+        <v>30015</v>
       </c>
       <c r="B11" s="44" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="45" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="D11" s="45" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="E11" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F11" s="44" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="G11" s="44" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="H11" s="46" t="n">
-        <v>24645</v>
+        <v>23410</v>
       </c>
       <c r="I11" s="46" t="n">
-        <v>34421</v>
+        <v>23410</v>
       </c>
       <c r="J11" s="46" t="n">
-        <v>42781</v>
+        <v>43552</v>
       </c>
       <c r="K11" s="47" t="n">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="L11" s="44" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="M11" s="44" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="N11" s="44" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="O11" s="44" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="P11" s="44" t="s">
-        <v>80</v>
+        <v>33</v>
       </c>
       <c r="Q11" s="45" t="s">
         <v>81</v>
@@ -4728,10 +4752,10 @@
     </row>
     <row r="12" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="43" t="n">
-        <v>32475</v>
+        <v>31644</v>
       </c>
       <c r="B12" s="44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C12" s="45" t="s">
         <v>84</v>
@@ -4749,16 +4773,16 @@
         <v>87</v>
       </c>
       <c r="H12" s="46" t="n">
-        <v>24267</v>
+        <v>24645</v>
       </c>
       <c r="I12" s="46" t="n">
-        <v>24267</v>
+        <v>34421</v>
       </c>
       <c r="J12" s="46" t="n">
-        <v>42480</v>
+        <v>42781</v>
       </c>
       <c r="K12" s="47" t="n">
-        <v>19</v>
+        <v>11</v>
       </c>
       <c r="L12" s="44" t="s">
         <v>88</v>
@@ -4791,7 +4815,7 @@
     </row>
     <row r="13" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="43" t="n">
-        <v>35366</v>
+        <v>32475</v>
       </c>
       <c r="B13" s="44" t="n">
         <v>1</v>
@@ -4800,52 +4824,52 @@
         <v>92</v>
       </c>
       <c r="D13" s="45" t="s">
-        <v>75</v>
+        <v>93</v>
       </c>
       <c r="E13" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F13" s="44" t="s">
-        <v>76</v>
+        <v>94</v>
       </c>
       <c r="G13" s="44" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="H13" s="46" t="n">
-        <v>25696</v>
+        <v>24267</v>
       </c>
       <c r="I13" s="46" t="n">
-        <v>25696</v>
+        <v>24267</v>
       </c>
       <c r="J13" s="46" t="n">
-        <v>42781</v>
+        <v>42480</v>
       </c>
       <c r="K13" s="47" t="n">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="L13" s="44" t="s">
-        <v>78</v>
+        <v>96</v>
       </c>
       <c r="M13" s="44" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="N13" s="44" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="O13" s="44" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="P13" s="44" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
       <c r="Q13" s="45" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="R13" s="45" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="S13" s="45" t="s">
-        <v>83</v>
+        <v>99</v>
       </c>
       <c r="T13" s="45"/>
       <c r="U13" s="44"/>
@@ -4854,43 +4878,43 @@
     </row>
     <row r="14" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="43" t="n">
-        <v>43454</v>
+        <v>35366</v>
       </c>
       <c r="B14" s="44" t="n">
         <v>1</v>
       </c>
       <c r="C14" s="45" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="D14" s="45" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>97</v>
+        <v>39</v>
       </c>
       <c r="F14" s="44" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="G14" s="44" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="H14" s="46" t="n">
-        <v>29650</v>
+        <v>25696</v>
       </c>
       <c r="I14" s="46" t="n">
-        <v>29650</v>
+        <v>25696</v>
       </c>
       <c r="J14" s="46" t="n">
-        <v>43905</v>
+        <v>42781</v>
       </c>
       <c r="K14" s="47" t="n">
-        <v>99</v>
+        <v>16</v>
       </c>
       <c r="L14" s="44" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="M14" s="44" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="N14" s="44" t="s">
         <v>44</v>
@@ -4902,13 +4926,13 @@
         <v>44</v>
       </c>
       <c r="Q14" s="45" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="R14" s="45" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="S14" s="45" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="T14" s="45"/>
       <c r="U14" s="44"/>
@@ -4917,19 +4941,19 @@
     </row>
     <row r="15" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="43" t="n">
-        <v>44625</v>
+        <v>43454</v>
       </c>
       <c r="B15" s="44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C15" s="45" t="s">
         <v>104</v>
       </c>
       <c r="D15" s="45" t="s">
+        <v>59</v>
+      </c>
+      <c r="E15" s="45" t="s">
         <v>105</v>
-      </c>
-      <c r="E15" s="45" t="s">
-        <v>39</v>
       </c>
       <c r="F15" s="44" t="s">
         <v>106</v>
@@ -4938,40 +4962,40 @@
         <v>107</v>
       </c>
       <c r="H15" s="46" t="n">
-        <v>30098</v>
+        <v>29650</v>
       </c>
       <c r="I15" s="46" t="n">
-        <v>30098</v>
+        <v>29650</v>
       </c>
       <c r="J15" s="46" t="n">
-        <v>42842</v>
+        <v>43905</v>
       </c>
       <c r="K15" s="47" t="n">
-        <v>59</v>
+        <v>99</v>
       </c>
       <c r="L15" s="44" t="s">
         <v>108</v>
       </c>
       <c r="M15" s="44" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="N15" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="O15" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="P15" s="44" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q15" s="45" t="s">
         <v>109</v>
       </c>
-      <c r="O15" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="P15" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q15" s="45" t="s">
+      <c r="R15" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="R15" s="45" t="s">
+      <c r="S15" s="45" t="s">
         <v>111</v>
-      </c>
-      <c r="S15" s="45" t="s">
-        <v>112</v>
       </c>
       <c r="T15" s="45"/>
       <c r="U15" s="44"/>
@@ -4980,52 +5004,52 @@
     </row>
     <row r="16" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="43" t="n">
-        <v>45882</v>
+        <v>44625</v>
       </c>
       <c r="B16" s="44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C16" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D16" s="45" t="s">
         <v>113</v>
-      </c>
-      <c r="D16" s="45" t="s">
-        <v>114</v>
       </c>
       <c r="E16" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F16" s="44" t="s">
+        <v>114</v>
+      </c>
+      <c r="G16" s="44" t="s">
         <v>115</v>
       </c>
-      <c r="G16" s="44" t="s">
+      <c r="H16" s="46" t="n">
+        <v>30098</v>
+      </c>
+      <c r="I16" s="46" t="n">
+        <v>30098</v>
+      </c>
+      <c r="J16" s="46" t="n">
+        <v>42842</v>
+      </c>
+      <c r="K16" s="47" t="n">
+        <v>59</v>
+      </c>
+      <c r="L16" s="44" t="s">
         <v>116</v>
       </c>
-      <c r="H16" s="46" t="n">
-        <v>31180</v>
-      </c>
-      <c r="I16" s="46" t="n">
-        <v>31180</v>
-      </c>
-      <c r="J16" s="46" t="n">
-        <v>43340</v>
-      </c>
-      <c r="K16" s="47" t="n">
-        <v>20</v>
-      </c>
-      <c r="L16" s="44" t="s">
+      <c r="M16" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="N16" s="44" t="s">
         <v>117</v>
       </c>
-      <c r="M16" s="44" t="s">
-        <v>62</v>
-      </c>
-      <c r="N16" s="44" t="s">
-        <v>33</v>
-      </c>
       <c r="O16" s="44" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="P16" s="44" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="Q16" s="45" t="s">
         <v>118</v>
@@ -5043,7 +5067,7 @@
     </row>
     <row r="17" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="43" t="n">
-        <v>53290</v>
+        <v>45882</v>
       </c>
       <c r="B17" s="44" t="n">
         <v>1</v>
@@ -5055,31 +5079,31 @@
         <v>122</v>
       </c>
       <c r="E17" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" s="44" t="s">
         <v>123</v>
       </c>
-      <c r="F17" s="44" t="s">
+      <c r="G17" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="G17" s="44" t="s">
+      <c r="H17" s="46" t="n">
+        <v>31180</v>
+      </c>
+      <c r="I17" s="46" t="n">
+        <v>31180</v>
+      </c>
+      <c r="J17" s="46" t="n">
+        <v>43340</v>
+      </c>
+      <c r="K17" s="47" t="n">
+        <v>20</v>
+      </c>
+      <c r="L17" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="H17" s="46" t="n">
-        <v>35026</v>
-      </c>
-      <c r="I17" s="46" t="n">
-        <v>35026</v>
-      </c>
-      <c r="J17" s="46" t="n">
-        <v>43002</v>
-      </c>
-      <c r="K17" s="47" t="n">
-        <v>19</v>
-      </c>
-      <c r="L17" s="44" t="s">
-        <v>126</v>
-      </c>
       <c r="M17" s="44" t="s">
-        <v>127</v>
+        <v>72</v>
       </c>
       <c r="N17" s="44" t="s">
         <v>33</v>
@@ -5091,89 +5115,89 @@
         <v>33</v>
       </c>
       <c r="Q17" s="45" t="s">
+        <v>126</v>
+      </c>
+      <c r="R17" s="45" t="s">
+        <v>127</v>
+      </c>
+      <c r="S17" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="R17" s="45" t="s">
-        <v>129</v>
-      </c>
-      <c r="S17" s="45" t="s">
-        <v>130</v>
-      </c>
       <c r="T17" s="45"/>
-      <c r="U17" s="44" t="s">
-        <v>131</v>
-      </c>
-      <c r="V17" s="44" t="s">
-        <v>132</v>
-      </c>
+      <c r="U17" s="44"/>
+      <c r="V17" s="44"/>
       <c r="W17" s="44"/>
     </row>
     <row r="18" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="43" t="n">
-        <v>53662</v>
+        <v>53290</v>
       </c>
       <c r="B18" s="44" t="n">
         <v>1</v>
       </c>
       <c r="C18" s="45" t="s">
+        <v>129</v>
+      </c>
+      <c r="D18" s="45" t="s">
+        <v>130</v>
+      </c>
+      <c r="E18" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="F18" s="44" t="s">
+        <v>132</v>
+      </c>
+      <c r="G18" s="44" t="s">
         <v>133</v>
       </c>
-      <c r="D18" s="45" t="s">
+      <c r="H18" s="46" t="n">
+        <v>35026</v>
+      </c>
+      <c r="I18" s="46" t="n">
+        <v>35026</v>
+      </c>
+      <c r="J18" s="46" t="n">
+        <v>43002</v>
+      </c>
+      <c r="K18" s="47" t="n">
+        <v>19</v>
+      </c>
+      <c r="L18" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="E18" s="45" t="s">
-        <v>39</v>
-      </c>
-      <c r="F18" s="44" t="s">
+      <c r="M18" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="G18" s="44" t="s">
+      <c r="N18" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="O18" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="P18" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q18" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="H18" s="46" t="n">
-        <v>35123</v>
-      </c>
-      <c r="I18" s="46" t="n">
-        <v>35123</v>
-      </c>
-      <c r="J18" s="46" t="n">
-        <v>42851</v>
-      </c>
-      <c r="K18" s="47" t="n">
-        <v>13</v>
-      </c>
-      <c r="L18" s="44" t="s">
+      <c r="R18" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="M18" s="44" t="s">
-        <v>79</v>
-      </c>
-      <c r="N18" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O18" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="P18" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q18" s="45" t="s">
+      <c r="S18" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="R18" s="45" t="s">
+      <c r="T18" s="45"/>
+      <c r="U18" s="44" t="s">
         <v>139</v>
       </c>
-      <c r="S18" s="45" t="s">
+      <c r="V18" s="44" t="s">
         <v>140</v>
       </c>
-      <c r="T18" s="45"/>
-      <c r="U18" s="44"/>
-      <c r="V18" s="44"/>
       <c r="W18" s="44"/>
     </row>
     <row r="19" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="43" t="n">
-        <v>54015</v>
+        <v>53662</v>
       </c>
       <c r="B19" s="44" t="n">
         <v>1</v>
@@ -5188,46 +5212,46 @@
         <v>39</v>
       </c>
       <c r="F19" s="44" t="s">
-        <v>68</v>
+        <v>143</v>
       </c>
       <c r="G19" s="44" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H19" s="46" t="n">
-        <v>35488</v>
+        <v>35123</v>
       </c>
       <c r="I19" s="46" t="n">
-        <v>35488</v>
+        <v>35123</v>
       </c>
       <c r="J19" s="46" t="n">
-        <v>42921</v>
+        <v>42851</v>
       </c>
       <c r="K19" s="47" t="n">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="L19" s="44" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="M19" s="44" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="N19" s="44" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="O19" s="44" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="P19" s="44" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="Q19" s="45" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="R19" s="45" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="S19" s="45" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="T19" s="45"/>
       <c r="U19" s="44"/>
@@ -5236,61 +5260,61 @@
     </row>
     <row r="20" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="43" t="n">
-        <v>55558</v>
+        <v>54015</v>
       </c>
       <c r="B20" s="44" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C20" s="45" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="D20" s="45" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="E20" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F20" s="44" t="s">
-        <v>150</v>
+        <v>78</v>
       </c>
       <c r="G20" s="44" t="s">
         <v>151</v>
       </c>
       <c r="H20" s="46" t="n">
-        <v>37232</v>
+        <v>35488</v>
       </c>
       <c r="I20" s="46" t="n">
-        <v>37232</v>
+        <v>35488</v>
       </c>
       <c r="J20" s="46" t="n">
-        <v>42896</v>
+        <v>42921</v>
       </c>
       <c r="K20" s="47" t="n">
-        <v>5</v>
+        <v>11</v>
       </c>
       <c r="L20" s="44" t="s">
-        <v>52</v>
+        <v>152</v>
       </c>
       <c r="M20" s="44" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="N20" s="44" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="O20" s="44" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="P20" s="44" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="Q20" s="45" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="R20" s="45" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="S20" s="45" t="s">
-        <v>112</v>
+        <v>155</v>
       </c>
       <c r="T20" s="45"/>
       <c r="U20" s="44"/>
@@ -5299,25 +5323,25 @@
     </row>
     <row r="21" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="43" t="n">
-        <v>55561</v>
+        <v>55558</v>
       </c>
       <c r="B21" s="44" t="n">
         <v>2</v>
       </c>
       <c r="C21" s="45" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D21" s="45" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="E21" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F21" s="44" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="G21" s="44" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="H21" s="46" t="n">
         <v>37232</v>
@@ -5326,54 +5350,52 @@
         <v>37232</v>
       </c>
       <c r="J21" s="46" t="n">
-        <v>43732</v>
+        <v>42896</v>
       </c>
       <c r="K21" s="47" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L21" s="44" t="s">
-        <v>158</v>
+        <v>62</v>
       </c>
       <c r="M21" s="44" t="s">
-        <v>62</v>
+        <v>43</v>
       </c>
       <c r="N21" s="44" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="O21" s="44" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="P21" s="44" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
       <c r="Q21" s="45" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="R21" s="45" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="S21" s="45" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="T21" s="45"/>
       <c r="U21" s="44"/>
       <c r="V21" s="44"/>
-      <c r="W21" s="44" t="s">
-        <v>162</v>
-      </c>
+      <c r="W21" s="44"/>
     </row>
     <row r="22" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="43" t="n">
-        <v>55594</v>
+        <v>55561</v>
       </c>
       <c r="B22" s="44" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C22" s="45" t="s">
+        <v>162</v>
+      </c>
+      <c r="D22" s="45" t="s">
         <v>163</v>
-      </c>
-      <c r="D22" s="45" t="s">
-        <v>114</v>
       </c>
       <c r="E22" s="45" t="s">
         <v>39</v>
@@ -5385,31 +5407,31 @@
         <v>165</v>
       </c>
       <c r="H22" s="46" t="n">
-        <v>37172</v>
+        <v>37232</v>
       </c>
       <c r="I22" s="46" t="n">
-        <v>37172</v>
+        <v>37232</v>
       </c>
       <c r="J22" s="46" t="n">
-        <v>43863</v>
+        <v>43732</v>
       </c>
       <c r="K22" s="47" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="L22" s="44" t="s">
         <v>166</v>
       </c>
       <c r="M22" s="44" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
       <c r="N22" s="44" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="O22" s="44" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="P22" s="44" t="s">
-        <v>33</v>
+        <v>117</v>
       </c>
       <c r="Q22" s="45" t="s">
         <v>167</v>
@@ -5423,56 +5445,58 @@
       <c r="T22" s="45"/>
       <c r="U22" s="44"/>
       <c r="V22" s="44"/>
-      <c r="W22" s="44"/>
+      <c r="W22" s="44" t="s">
+        <v>170</v>
+      </c>
     </row>
     <row r="23" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="43" t="n">
-        <v>55674</v>
+        <v>55594</v>
       </c>
       <c r="B23" s="44" t="n">
         <v>1</v>
       </c>
       <c r="C23" s="45" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="D23" s="45" t="s">
-        <v>149</v>
+        <v>122</v>
       </c>
       <c r="E23" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F23" s="44" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="G23" s="44" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="H23" s="46" t="n">
-        <v>37321</v>
+        <v>37172</v>
       </c>
       <c r="I23" s="46" t="n">
-        <v>37321</v>
+        <v>37172</v>
       </c>
       <c r="J23" s="46" t="n">
-        <v>42798</v>
+        <v>43863</v>
       </c>
       <c r="K23" s="47" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="L23" s="44" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="M23" s="44" t="s">
-        <v>174</v>
+        <v>63</v>
       </c>
       <c r="N23" s="44" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="O23" s="44" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="P23" s="44" t="s">
-        <v>109</v>
+        <v>33</v>
       </c>
       <c r="Q23" s="45" t="s">
         <v>175</v>
@@ -5490,7 +5514,7 @@
     </row>
     <row r="24" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="43" t="n">
-        <v>58943</v>
+        <v>55674</v>
       </c>
       <c r="B24" s="44" t="n">
         <v>1</v>
@@ -5499,60 +5523,64 @@
         <v>178</v>
       </c>
       <c r="D24" s="45" t="s">
+        <v>157</v>
+      </c>
+      <c r="E24" s="45" t="s">
+        <v>39</v>
+      </c>
+      <c r="F24" s="44" t="s">
         <v>179</v>
       </c>
-      <c r="E24" s="45" t="s">
+      <c r="G24" s="44" t="s">
         <v>180</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="H24" s="46" t="n">
+        <v>37321</v>
+      </c>
+      <c r="I24" s="46" t="n">
+        <v>37321</v>
+      </c>
+      <c r="J24" s="46" t="n">
+        <v>42798</v>
+      </c>
+      <c r="K24" s="47" t="n">
+        <v>5</v>
+      </c>
+      <c r="L24" s="44" t="s">
         <v>181</v>
       </c>
-      <c r="G24" s="44"/>
-      <c r="H24" s="46" t="n">
-        <v>42110</v>
-      </c>
-      <c r="I24" s="46" t="n">
-        <v>42110</v>
-      </c>
-      <c r="J24" s="46" t="n">
-        <v>43936</v>
-      </c>
-      <c r="K24" s="47" t="n">
-        <v>1</v>
-      </c>
-      <c r="L24" s="44" t="s">
+      <c r="M24" s="44" t="s">
         <v>182</v>
       </c>
-      <c r="M24" s="44" t="s">
+      <c r="N24" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="O24" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="P24" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q24" s="45" t="s">
         <v>183</v>
       </c>
-      <c r="N24" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O24" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="P24" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q24" s="45"/>
-      <c r="R24" s="45"/>
+      <c r="R24" s="45" t="s">
+        <v>184</v>
+      </c>
       <c r="S24" s="45" t="s">
-        <v>184</v>
-      </c>
-      <c r="T24" s="45" t="s">
         <v>185</v>
       </c>
+      <c r="T24" s="45"/>
       <c r="U24" s="44"/>
       <c r="V24" s="44"/>
       <c r="W24" s="44"/>
     </row>
     <row r="25" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="43" t="n">
-        <v>59267</v>
+        <v>58943</v>
       </c>
       <c r="B25" s="44" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="C25" s="45" t="s">
         <v>186</v>
@@ -5566,89 +5594,85 @@
       <c r="F25" s="44" t="s">
         <v>189</v>
       </c>
-      <c r="G25" s="44" t="s">
+      <c r="G25" s="44"/>
+      <c r="H25" s="46" t="n">
+        <v>42110</v>
+      </c>
+      <c r="I25" s="46" t="n">
+        <v>42110</v>
+      </c>
+      <c r="J25" s="46" t="n">
+        <v>43936</v>
+      </c>
+      <c r="K25" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L25" s="44" t="s">
         <v>190</v>
       </c>
-      <c r="H25" s="46" t="n">
-        <v>40128</v>
-      </c>
-      <c r="I25" s="46" t="n">
-        <v>42257</v>
-      </c>
-      <c r="J25" s="46" t="n">
-        <v>43779</v>
-      </c>
-      <c r="K25" s="47" t="n">
-        <v>11</v>
-      </c>
-      <c r="L25" s="44" t="s">
+      <c r="M25" s="44" t="s">
         <v>191</v>
       </c>
-      <c r="M25" s="44" t="s">
+      <c r="N25" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="O25" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="P25" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q25" s="45"/>
+      <c r="R25" s="45"/>
+      <c r="S25" s="45" t="s">
         <v>192</v>
       </c>
-      <c r="N25" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="O25" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="P25" s="44" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q25" s="45" t="s">
+      <c r="T25" s="45" t="s">
         <v>193</v>
       </c>
-      <c r="R25" s="45" t="s">
-        <v>194</v>
-      </c>
-      <c r="S25" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="T25" s="45"/>
       <c r="U25" s="44"/>
       <c r="V25" s="44"/>
       <c r="W25" s="44"/>
     </row>
     <row r="26" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="43" t="n">
-        <v>61186</v>
+        <v>59267</v>
       </c>
       <c r="B26" s="44" t="n">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="C26" s="45" t="s">
+        <v>194</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>195</v>
+      </c>
+      <c r="E26" s="45" t="s">
         <v>196</v>
       </c>
-      <c r="D26" s="45" t="s">
-        <v>114</v>
-      </c>
-      <c r="E26" s="45" t="s">
-        <v>39</v>
-      </c>
       <c r="F26" s="44" t="s">
-        <v>164</v>
+        <v>197</v>
       </c>
       <c r="G26" s="44" t="s">
-        <v>165</v>
+        <v>198</v>
       </c>
       <c r="H26" s="46" t="n">
-        <v>40522</v>
+        <v>40128</v>
       </c>
       <c r="I26" s="46" t="n">
-        <v>40522</v>
+        <v>42257</v>
       </c>
       <c r="J26" s="46" t="n">
-        <v>44174</v>
+        <v>43779</v>
       </c>
       <c r="K26" s="47" t="n">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="L26" s="44" t="s">
-        <v>197</v>
+        <v>199</v>
       </c>
       <c r="M26" s="44" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="N26" s="44" t="s">
         <v>33</v>
@@ -5660,13 +5684,13 @@
         <v>33</v>
       </c>
       <c r="Q26" s="45" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="R26" s="45" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="S26" s="45" t="s">
-        <v>169</v>
+        <v>203</v>
       </c>
       <c r="T26" s="45"/>
       <c r="U26" s="44"/>
@@ -5675,43 +5699,43 @@
     </row>
     <row r="27" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="43" t="n">
-        <v>62069</v>
+        <v>61186</v>
       </c>
       <c r="B27" s="44" t="n">
         <v>1</v>
       </c>
       <c r="C27" s="45" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="D27" s="45" t="s">
-        <v>202</v>
+        <v>122</v>
       </c>
       <c r="E27" s="45" t="s">
         <v>39</v>
       </c>
       <c r="F27" s="44" t="s">
-        <v>203</v>
+        <v>172</v>
       </c>
       <c r="G27" s="44" t="s">
-        <v>204</v>
+        <v>173</v>
       </c>
       <c r="H27" s="46" t="n">
-        <v>40610</v>
+        <v>40522</v>
       </c>
       <c r="I27" s="46" t="n">
-        <v>40610</v>
+        <v>40522</v>
       </c>
       <c r="J27" s="46" t="n">
-        <v>44262</v>
+        <v>44174</v>
       </c>
       <c r="K27" s="47" t="n">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="L27" s="44" t="s">
-        <v>78</v>
+        <v>205</v>
       </c>
       <c r="M27" s="44" t="s">
-        <v>79</v>
+        <v>206</v>
       </c>
       <c r="N27" s="44" t="s">
         <v>33</v>
@@ -5723,13 +5747,13 @@
         <v>33</v>
       </c>
       <c r="Q27" s="45" t="s">
-        <v>205</v>
+        <v>207</v>
       </c>
       <c r="R27" s="45" t="s">
-        <v>206</v>
+        <v>208</v>
       </c>
       <c r="S27" s="45" t="s">
-        <v>207</v>
+        <v>177</v>
       </c>
       <c r="T27" s="45"/>
       <c r="U27" s="44"/>
@@ -5738,68 +5762,131 @@
     </row>
     <row r="28" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="43" t="n">
-        <v>62132</v>
+        <v>62069</v>
       </c>
       <c r="B28" s="44" t="n">
         <v>1</v>
       </c>
       <c r="C28" s="45" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D28" s="45" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E28" s="45" t="s">
-        <v>123</v>
+        <v>39</v>
       </c>
       <c r="F28" s="44" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="G28" s="44" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="H28" s="46" t="n">
-        <v>41337</v>
+        <v>40610</v>
       </c>
       <c r="I28" s="46" t="n">
-        <v>41337</v>
+        <v>40610</v>
       </c>
       <c r="J28" s="46" t="n">
-        <v>43162</v>
+        <v>44262</v>
       </c>
       <c r="K28" s="47" t="n">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="L28" s="44" t="s">
-        <v>212</v>
+        <v>88</v>
       </c>
       <c r="M28" s="44" t="s">
+        <v>43</v>
+      </c>
+      <c r="N28" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="O28" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="P28" s="44" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q28" s="45" t="s">
         <v>213</v>
       </c>
-      <c r="N28" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="O28" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="P28" s="44" t="s">
-        <v>109</v>
-      </c>
-      <c r="Q28" s="45" t="s">
+      <c r="R28" s="45" t="s">
         <v>214</v>
       </c>
-      <c r="R28" s="45" t="s">
+      <c r="S28" s="45" t="s">
         <v>215</v>
       </c>
-      <c r="S28" s="45" t="s">
-        <v>216</v>
-      </c>
       <c r="T28" s="45"/>
-      <c r="U28" s="44" t="s">
-        <v>131</v>
-      </c>
+      <c r="U28" s="44"/>
       <c r="V28" s="44"/>
       <c r="W28" s="44"/>
+    </row>
+    <row r="29" s="7" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="43" t="n">
+        <v>62132</v>
+      </c>
+      <c r="B29" s="44" t="n">
+        <v>1</v>
+      </c>
+      <c r="C29" s="45" t="s">
+        <v>216</v>
+      </c>
+      <c r="D29" s="45" t="s">
+        <v>217</v>
+      </c>
+      <c r="E29" s="45" t="s">
+        <v>131</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>218</v>
+      </c>
+      <c r="G29" s="44" t="s">
+        <v>219</v>
+      </c>
+      <c r="H29" s="46" t="n">
+        <v>41337</v>
+      </c>
+      <c r="I29" s="46" t="n">
+        <v>41337</v>
+      </c>
+      <c r="J29" s="46" t="n">
+        <v>43162</v>
+      </c>
+      <c r="K29" s="47" t="n">
+        <v>1</v>
+      </c>
+      <c r="L29" s="44" t="s">
+        <v>220</v>
+      </c>
+      <c r="M29" s="44" t="s">
+        <v>221</v>
+      </c>
+      <c r="N29" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="O29" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="P29" s="44" t="s">
+        <v>117</v>
+      </c>
+      <c r="Q29" s="45" t="s">
+        <v>222</v>
+      </c>
+      <c r="R29" s="45" t="s">
+        <v>223</v>
+      </c>
+      <c r="S29" s="45" t="s">
+        <v>224</v>
+      </c>
+      <c r="T29" s="45"/>
+      <c r="U29" s="44" t="s">
+        <v>139</v>
+      </c>
+      <c r="V29" s="44"/>
+      <c r="W29" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Add ATC-Code for products like priorix
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package.xlsx
+++ b/spec/data/swissmedic_package.xlsx
@@ -17,6 +17,7 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Titles_0_0_0_0_0" vbProcedure="false">'Zugelassene Packungen'!$5:$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="289">
   <si>
     <t xml:space="preserve">Zugelassene Packungen / Conditionnements autorisés</t>
   </si>
@@ -956,18 +957,38 @@
   <si>
     <t xml:space="preserve">Onkologikum</t>
   </si>
+  <si>
+    <t xml:space="preserve">Priorix-Tetra, Pulver und Lösungsmittel zur Herstellung einer Injektionslösung</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GlaxoSmithKline AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J07BD54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">virus morbilli vivus (Stamm: Schwarz), virus parotitis vivus (Stamm: RIT 4385), virus rubella vivus (Stamm: Wistar RA 27/3), virus varicellae vivus (Stamm: OKA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaccinum attenuatum: virus morbilli vivus (Stamm: Schwarz) min. 10^3 U., virus parotitis vivus (Stamm: RIT 4385) min.10^4.4 U., virus rubella vivus (Stamm: Wistar RA 27/3) min.10^3 U., virus varicellae vivus (Stamm: OKA) min.10^3.3 U., lactosum, sorbitolum, mannitolum, aminoacida, residui: neomycini sulfas nihil, pro praeparatione.
+Solvens: aqua ad iniectabilia q.s. ad suspensionem pro 0.5 ml.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">aktive Immunisierung gegen Masern, Mumps, Röteln und Varizellen, ab dem vollendeten 12. Lebensmonat</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="6">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="00000"/>
     <numFmt numFmtId="166" formatCode="DD/MM/YY;@"/>
     <numFmt numFmtId="167" formatCode="00"/>
     <numFmt numFmtId="168" formatCode="DD/MM/YYYY"/>
     <numFmt numFmtId="169" formatCode="000"/>
+    <numFmt numFmtId="170" formatCode="DD/MM/YYYY"/>
   </numFmts>
   <fonts count="13">
     <font>
@@ -1123,7 +1144,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="21">
+  <cellStyleXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1151,37 +1172,41 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="58">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1205,63 +1230,63 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="1" xfId="21" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1281,15 +1306,15 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1325,23 +1350,23 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="169" fontId="4" fillId="0" borderId="0" xfId="21" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1353,15 +1378,48 @@
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="2" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="12" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="3" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="170" fontId="12" fillId="0" borderId="4" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="12" fillId="0" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="8">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Excel Built-in Explanatory Text" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Standard 2" xfId="20" builtinId="53" customBuiltin="true"/>
+    <cellStyle name="Excel Built-in Explanatory Text" xfId="21" builtinId="53" customBuiltin="true"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -1437,9 +1495,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>444600</xdr:colOff>
+      <xdr:colOff>444240</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>37080</xdr:rowOff>
+      <xdr:rowOff>36720</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1453,7 +1511,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="36360" y="360"/>
-          <a:ext cx="1685160" cy="569880"/>
+          <a:ext cx="1684800" cy="569520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1473,12 +1531,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ40"/>
+  <dimension ref="A1:AMJ41"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A40" activeCellId="0" sqref="40:40"/>
+      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="41:41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19870,6 +19928,69 @@
       <c r="AMI40" s="0"/>
       <c r="AMJ40" s="0"/>
     </row>
+    <row r="41" s="57" customFormat="true" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="50" t="n">
+        <v>58158</v>
+      </c>
+      <c r="B41" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="C41" s="52" t="s">
+        <v>283</v>
+      </c>
+      <c r="D41" s="52" t="s">
+        <v>284</v>
+      </c>
+      <c r="E41" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="F41" s="53" t="s">
+        <v>214</v>
+      </c>
+      <c r="G41" s="53" t="s">
+        <v>285</v>
+      </c>
+      <c r="H41" s="54" t="n">
+        <v>39296</v>
+      </c>
+      <c r="I41" s="54" t="n">
+        <v>40027</v>
+      </c>
+      <c r="J41" s="55" t="n">
+        <v>44774</v>
+      </c>
+      <c r="K41" s="56" t="n">
+        <v>1</v>
+      </c>
+      <c r="L41" s="50" t="s">
+        <v>198</v>
+      </c>
+      <c r="M41" s="52" t="s">
+        <v>237</v>
+      </c>
+      <c r="N41" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="O41" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="P41" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q41" s="52" t="s">
+        <v>286</v>
+      </c>
+      <c r="R41" s="52" t="s">
+        <v>287</v>
+      </c>
+      <c r="S41" s="52" t="s">
+        <v>288</v>
+      </c>
+      <c r="T41" s="52"/>
+      <c r="U41" s="53"/>
+      <c r="V41" s="52"/>
+      <c r="W41" s="53"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>

</xml_diff>

<commit_message>
Ensure correct prodno for artikelstamm
</commit_message>
<xml_diff>
--- a/spec/data/swissmedic_package.xlsx
+++ b/spec/data/swissmedic_package.xlsx
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="301">
   <si>
     <t xml:space="preserve">Zugelassene Packungen / Conditionnements autorisés</t>
   </si>
@@ -975,6 +975,42 @@
   </si>
   <si>
     <t xml:space="preserve">aktive Immunisierung gegen Masern, Mumps, Röteln und Varizellen, ab dem vollendeten 12. Lebensmonat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lopresor Retard 200, Divitabs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daiichi Sankyo (Schweiz) AG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">02.03.0.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C07AB02</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metoprololi tartras (2:1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metoprololi tartras (2:1) 200 mg, excipiens pro compresso obducto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Betarezeptorenblocker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lopresor 100, Filmtabletten</t>
+  </si>
+  <si>
+    <t xml:space="preserve">metoprololi tartras (2:1) 100 mg, excipiens pro compresso obducto.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Beta-Rezeptorenblocker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200</t>
   </si>
 </sst>
 </file>
@@ -1531,12 +1567,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ41"/>
+  <dimension ref="A1:AMJ45"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="5" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="41:41"/>
+      <selection pane="bottomLeft" activeCell="A44" activeCellId="0" sqref="44:45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -17800,1070 +17836,70 @@
       <c r="AMI38" s="0"/>
       <c r="AMJ38" s="0"/>
     </row>
-    <row r="39" customFormat="false" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="36" t="n">
+    <row r="39" s="57" customFormat="true" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="50" t="n">
         <v>55561</v>
       </c>
-      <c r="B39" s="49" t="n">
+      <c r="B39" s="51" t="n">
         <v>2</v>
       </c>
-      <c r="C39" s="38" t="s">
+      <c r="C39" s="52" t="s">
         <v>265</v>
       </c>
-      <c r="D39" s="38" t="s">
+      <c r="D39" s="52" t="s">
         <v>266</v>
       </c>
-      <c r="E39" s="39" t="s">
+      <c r="E39" s="53" t="s">
         <v>39</v>
       </c>
-      <c r="F39" s="39" t="s">
+      <c r="F39" s="53" t="s">
         <v>267</v>
       </c>
-      <c r="G39" s="39" t="s">
+      <c r="G39" s="53" t="s">
         <v>268</v>
       </c>
-      <c r="H39" s="40" t="n">
+      <c r="H39" s="54" t="n">
         <v>37232</v>
       </c>
-      <c r="I39" s="40" t="n">
+      <c r="I39" s="54" t="n">
         <v>37232</v>
       </c>
-      <c r="J39" s="41" t="n">
+      <c r="J39" s="55" t="n">
         <v>43732</v>
       </c>
-      <c r="K39" s="48" t="n">
+      <c r="K39" s="56" t="n">
         <v>4</v>
       </c>
-      <c r="L39" s="36" t="s">
+      <c r="L39" s="50" t="s">
         <v>269</v>
       </c>
-      <c r="M39" s="38" t="s">
+      <c r="M39" s="52" t="s">
         <v>72</v>
       </c>
-      <c r="N39" s="39" t="s">
+      <c r="N39" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="O39" s="39" t="s">
+      <c r="O39" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="P39" s="39" t="s">
+      <c r="P39" s="53" t="s">
         <v>117</v>
       </c>
-      <c r="Q39" s="38" t="s">
+      <c r="Q39" s="52" t="s">
         <v>270</v>
       </c>
-      <c r="R39" s="38" t="s">
+      <c r="R39" s="52" t="s">
         <v>271</v>
       </c>
-      <c r="S39" s="38" t="s">
+      <c r="S39" s="52" t="s">
         <v>272</v>
       </c>
-      <c r="T39" s="38"/>
-      <c r="U39" s="39"/>
-      <c r="V39" s="38"/>
-      <c r="W39" s="39" t="s">
+      <c r="T39" s="52"/>
+      <c r="U39" s="53"/>
+      <c r="V39" s="52"/>
+      <c r="W39" s="53" t="s">
         <v>273</v>
       </c>
-      <c r="Y39" s="0"/>
-      <c r="Z39" s="0"/>
-      <c r="AA39" s="0"/>
-      <c r="AB39" s="0"/>
-      <c r="AC39" s="0"/>
-      <c r="AD39" s="0"/>
-      <c r="AE39" s="0"/>
-      <c r="AF39" s="0"/>
-      <c r="AG39" s="0"/>
-      <c r="AH39" s="0"/>
-      <c r="AI39" s="0"/>
-      <c r="AJ39" s="0"/>
-      <c r="AK39" s="0"/>
-      <c r="AL39" s="0"/>
-      <c r="AM39" s="0"/>
-      <c r="AN39" s="0"/>
-      <c r="AO39" s="0"/>
-      <c r="AP39" s="0"/>
-      <c r="AQ39" s="0"/>
-      <c r="AR39" s="0"/>
-      <c r="AS39" s="0"/>
-      <c r="AT39" s="0"/>
-      <c r="AU39" s="0"/>
-      <c r="AV39" s="0"/>
-      <c r="AW39" s="0"/>
-      <c r="AX39" s="0"/>
-      <c r="AY39" s="0"/>
-      <c r="AZ39" s="0"/>
-      <c r="BA39" s="0"/>
-      <c r="BB39" s="0"/>
-      <c r="BC39" s="0"/>
-      <c r="BD39" s="0"/>
-      <c r="BE39" s="0"/>
-      <c r="BF39" s="0"/>
-      <c r="BG39" s="0"/>
-      <c r="BH39" s="0"/>
-      <c r="BI39" s="0"/>
-      <c r="BJ39" s="0"/>
-      <c r="BK39" s="0"/>
-      <c r="BL39" s="0"/>
-      <c r="BM39" s="0"/>
-      <c r="BN39" s="0"/>
-      <c r="BO39" s="0"/>
-      <c r="BP39" s="0"/>
-      <c r="BQ39" s="0"/>
-      <c r="BR39" s="0"/>
-      <c r="BS39" s="0"/>
-      <c r="BT39" s="0"/>
-      <c r="BU39" s="0"/>
-      <c r="BV39" s="0"/>
-      <c r="BW39" s="0"/>
-      <c r="BX39" s="0"/>
-      <c r="BY39" s="0"/>
-      <c r="BZ39" s="0"/>
-      <c r="CA39" s="0"/>
-      <c r="CB39" s="0"/>
-      <c r="CC39" s="0"/>
-      <c r="CD39" s="0"/>
-      <c r="CE39" s="0"/>
-      <c r="CF39" s="0"/>
-      <c r="CG39" s="0"/>
-      <c r="CH39" s="0"/>
-      <c r="CI39" s="0"/>
-      <c r="CJ39" s="0"/>
-      <c r="CK39" s="0"/>
-      <c r="CL39" s="0"/>
-      <c r="CM39" s="0"/>
-      <c r="CN39" s="0"/>
-      <c r="CO39" s="0"/>
-      <c r="CP39" s="0"/>
-      <c r="CQ39" s="0"/>
-      <c r="CR39" s="0"/>
-      <c r="CS39" s="0"/>
-      <c r="CT39" s="0"/>
-      <c r="CU39" s="0"/>
-      <c r="CV39" s="0"/>
-      <c r="CW39" s="0"/>
-      <c r="CX39" s="0"/>
-      <c r="CY39" s="0"/>
-      <c r="CZ39" s="0"/>
-      <c r="DA39" s="0"/>
-      <c r="DB39" s="0"/>
-      <c r="DC39" s="0"/>
-      <c r="DD39" s="0"/>
-      <c r="DE39" s="0"/>
-      <c r="DF39" s="0"/>
-      <c r="DG39" s="0"/>
-      <c r="DH39" s="0"/>
-      <c r="DI39" s="0"/>
-      <c r="DJ39" s="0"/>
-      <c r="DK39" s="0"/>
-      <c r="DL39" s="0"/>
-      <c r="DM39" s="0"/>
-      <c r="DN39" s="0"/>
-      <c r="DO39" s="0"/>
-      <c r="DP39" s="0"/>
-      <c r="DQ39" s="0"/>
-      <c r="DR39" s="0"/>
-      <c r="DS39" s="0"/>
-      <c r="DT39" s="0"/>
-      <c r="DU39" s="0"/>
-      <c r="DV39" s="0"/>
-      <c r="DW39" s="0"/>
-      <c r="DX39" s="0"/>
-      <c r="DY39" s="0"/>
-      <c r="DZ39" s="0"/>
-      <c r="EA39" s="0"/>
-      <c r="EB39" s="0"/>
-      <c r="EC39" s="0"/>
-      <c r="ED39" s="0"/>
-      <c r="EE39" s="0"/>
-      <c r="EF39" s="0"/>
-      <c r="EG39" s="0"/>
-      <c r="EH39" s="0"/>
-      <c r="EI39" s="0"/>
-      <c r="EJ39" s="0"/>
-      <c r="EK39" s="0"/>
-      <c r="EL39" s="0"/>
-      <c r="EM39" s="0"/>
-      <c r="EN39" s="0"/>
-      <c r="EO39" s="0"/>
-      <c r="EP39" s="0"/>
-      <c r="EQ39" s="0"/>
-      <c r="ER39" s="0"/>
-      <c r="ES39" s="0"/>
-      <c r="ET39" s="0"/>
-      <c r="EU39" s="0"/>
-      <c r="EV39" s="0"/>
-      <c r="EW39" s="0"/>
-      <c r="EX39" s="0"/>
-      <c r="EY39" s="0"/>
-      <c r="EZ39" s="0"/>
-      <c r="FA39" s="0"/>
-      <c r="FB39" s="0"/>
-      <c r="FC39" s="0"/>
-      <c r="FD39" s="0"/>
-      <c r="FE39" s="0"/>
-      <c r="FF39" s="0"/>
-      <c r="FG39" s="0"/>
-      <c r="FH39" s="0"/>
-      <c r="FI39" s="0"/>
-      <c r="FJ39" s="0"/>
-      <c r="FK39" s="0"/>
-      <c r="FL39" s="0"/>
-      <c r="FM39" s="0"/>
-      <c r="FN39" s="0"/>
-      <c r="FO39" s="0"/>
-      <c r="FP39" s="0"/>
-      <c r="FQ39" s="0"/>
-      <c r="FR39" s="0"/>
-      <c r="FS39" s="0"/>
-      <c r="FT39" s="0"/>
-      <c r="FU39" s="0"/>
-      <c r="FV39" s="0"/>
-      <c r="FW39" s="0"/>
-      <c r="FX39" s="0"/>
-      <c r="FY39" s="0"/>
-      <c r="FZ39" s="0"/>
-      <c r="GA39" s="0"/>
-      <c r="GB39" s="0"/>
-      <c r="GC39" s="0"/>
-      <c r="GD39" s="0"/>
-      <c r="GE39" s="0"/>
-      <c r="GF39" s="0"/>
-      <c r="GG39" s="0"/>
-      <c r="GH39" s="0"/>
-      <c r="GI39" s="0"/>
-      <c r="GJ39" s="0"/>
-      <c r="GK39" s="0"/>
-      <c r="GL39" s="0"/>
-      <c r="GM39" s="0"/>
-      <c r="GN39" s="0"/>
-      <c r="GO39" s="0"/>
-      <c r="GP39" s="0"/>
-      <c r="GQ39" s="0"/>
-      <c r="GR39" s="0"/>
-      <c r="GS39" s="0"/>
-      <c r="GT39" s="0"/>
-      <c r="GU39" s="0"/>
-      <c r="GV39" s="0"/>
-      <c r="GW39" s="0"/>
-      <c r="GX39" s="0"/>
-      <c r="GY39" s="0"/>
-      <c r="GZ39" s="0"/>
-      <c r="HA39" s="0"/>
-      <c r="HB39" s="0"/>
-      <c r="HC39" s="0"/>
-      <c r="HD39" s="0"/>
-      <c r="HE39" s="0"/>
-      <c r="HF39" s="0"/>
-      <c r="HG39" s="0"/>
-      <c r="HH39" s="0"/>
-      <c r="HI39" s="0"/>
-      <c r="HJ39" s="0"/>
-      <c r="HK39" s="0"/>
-      <c r="HL39" s="0"/>
-      <c r="HM39" s="0"/>
-      <c r="HN39" s="0"/>
-      <c r="HO39" s="0"/>
-      <c r="HP39" s="0"/>
-      <c r="HQ39" s="0"/>
-      <c r="HR39" s="0"/>
-      <c r="HS39" s="0"/>
-      <c r="HT39" s="0"/>
-      <c r="HU39" s="0"/>
-      <c r="HV39" s="0"/>
-      <c r="HW39" s="0"/>
-      <c r="HX39" s="0"/>
-      <c r="HY39" s="0"/>
-      <c r="HZ39" s="0"/>
-      <c r="IA39" s="0"/>
-      <c r="IB39" s="0"/>
-      <c r="IC39" s="0"/>
-      <c r="ID39" s="0"/>
-      <c r="IE39" s="0"/>
-      <c r="IF39" s="0"/>
-      <c r="IG39" s="0"/>
-      <c r="IH39" s="0"/>
-      <c r="II39" s="0"/>
-      <c r="IJ39" s="0"/>
-      <c r="IK39" s="0"/>
-      <c r="IL39" s="0"/>
-      <c r="IM39" s="0"/>
-      <c r="IN39" s="0"/>
-      <c r="IO39" s="0"/>
-      <c r="IP39" s="0"/>
-      <c r="IQ39" s="0"/>
-      <c r="IR39" s="0"/>
-      <c r="IS39" s="0"/>
-      <c r="IT39" s="0"/>
-      <c r="IU39" s="0"/>
-      <c r="IV39" s="0"/>
-      <c r="IW39" s="0"/>
-      <c r="IX39" s="0"/>
-      <c r="IY39" s="0"/>
-      <c r="IZ39" s="0"/>
-      <c r="JA39" s="0"/>
-      <c r="JB39" s="0"/>
-      <c r="JC39" s="0"/>
-      <c r="JD39" s="0"/>
-      <c r="JE39" s="0"/>
-      <c r="JF39" s="0"/>
-      <c r="JG39" s="0"/>
-      <c r="JH39" s="0"/>
-      <c r="JI39" s="0"/>
-      <c r="JJ39" s="0"/>
-      <c r="JK39" s="0"/>
-      <c r="JL39" s="0"/>
-      <c r="JM39" s="0"/>
-      <c r="JN39" s="0"/>
-      <c r="JO39" s="0"/>
-      <c r="JP39" s="0"/>
-      <c r="JQ39" s="0"/>
-      <c r="JR39" s="0"/>
-      <c r="JS39" s="0"/>
-      <c r="JT39" s="0"/>
-      <c r="JU39" s="0"/>
-      <c r="JV39" s="0"/>
-      <c r="JW39" s="0"/>
-      <c r="JX39" s="0"/>
-      <c r="JY39" s="0"/>
-      <c r="JZ39" s="0"/>
-      <c r="KA39" s="0"/>
-      <c r="KB39" s="0"/>
-      <c r="KC39" s="0"/>
-      <c r="KD39" s="0"/>
-      <c r="KE39" s="0"/>
-      <c r="KF39" s="0"/>
-      <c r="KG39" s="0"/>
-      <c r="KH39" s="0"/>
-      <c r="KI39" s="0"/>
-      <c r="KJ39" s="0"/>
-      <c r="KK39" s="0"/>
-      <c r="KL39" s="0"/>
-      <c r="KM39" s="0"/>
-      <c r="KN39" s="0"/>
-      <c r="KO39" s="0"/>
-      <c r="KP39" s="0"/>
-      <c r="KQ39" s="0"/>
-      <c r="KR39" s="0"/>
-      <c r="KS39" s="0"/>
-      <c r="KT39" s="0"/>
-      <c r="KU39" s="0"/>
-      <c r="KV39" s="0"/>
-      <c r="KW39" s="0"/>
-      <c r="KX39" s="0"/>
-      <c r="KY39" s="0"/>
-      <c r="KZ39" s="0"/>
-      <c r="LA39" s="0"/>
-      <c r="LB39" s="0"/>
-      <c r="LC39" s="0"/>
-      <c r="LD39" s="0"/>
-      <c r="LE39" s="0"/>
-      <c r="LF39" s="0"/>
-      <c r="LG39" s="0"/>
-      <c r="LH39" s="0"/>
-      <c r="LI39" s="0"/>
-      <c r="LJ39" s="0"/>
-      <c r="LK39" s="0"/>
-      <c r="LL39" s="0"/>
-      <c r="LM39" s="0"/>
-      <c r="LN39" s="0"/>
-      <c r="LO39" s="0"/>
-      <c r="LP39" s="0"/>
-      <c r="LQ39" s="0"/>
-      <c r="LR39" s="0"/>
-      <c r="LS39" s="0"/>
-      <c r="LT39" s="0"/>
-      <c r="LU39" s="0"/>
-      <c r="LV39" s="0"/>
-      <c r="LW39" s="0"/>
-      <c r="LX39" s="0"/>
-      <c r="LY39" s="0"/>
-      <c r="LZ39" s="0"/>
-      <c r="MA39" s="0"/>
-      <c r="MB39" s="0"/>
-      <c r="MC39" s="0"/>
-      <c r="MD39" s="0"/>
-      <c r="ME39" s="0"/>
-      <c r="MF39" s="0"/>
-      <c r="MG39" s="0"/>
-      <c r="MH39" s="0"/>
-      <c r="MI39" s="0"/>
-      <c r="MJ39" s="0"/>
-      <c r="MK39" s="0"/>
-      <c r="ML39" s="0"/>
-      <c r="MM39" s="0"/>
-      <c r="MN39" s="0"/>
-      <c r="MO39" s="0"/>
-      <c r="MP39" s="0"/>
-      <c r="MQ39" s="0"/>
-      <c r="MR39" s="0"/>
-      <c r="MS39" s="0"/>
-      <c r="MT39" s="0"/>
-      <c r="MU39" s="0"/>
-      <c r="MV39" s="0"/>
-      <c r="MW39" s="0"/>
-      <c r="MX39" s="0"/>
-      <c r="MY39" s="0"/>
-      <c r="MZ39" s="0"/>
-      <c r="NA39" s="0"/>
-      <c r="NB39" s="0"/>
-      <c r="NC39" s="0"/>
-      <c r="ND39" s="0"/>
-      <c r="NE39" s="0"/>
-      <c r="NF39" s="0"/>
-      <c r="NG39" s="0"/>
-      <c r="NH39" s="0"/>
-      <c r="NI39" s="0"/>
-      <c r="NJ39" s="0"/>
-      <c r="NK39" s="0"/>
-      <c r="NL39" s="0"/>
-      <c r="NM39" s="0"/>
-      <c r="NN39" s="0"/>
-      <c r="NO39" s="0"/>
-      <c r="NP39" s="0"/>
-      <c r="NQ39" s="0"/>
-      <c r="NR39" s="0"/>
-      <c r="NS39" s="0"/>
-      <c r="NT39" s="0"/>
-      <c r="NU39" s="0"/>
-      <c r="NV39" s="0"/>
-      <c r="NW39" s="0"/>
-      <c r="NX39" s="0"/>
-      <c r="NY39" s="0"/>
-      <c r="NZ39" s="0"/>
-      <c r="OA39" s="0"/>
-      <c r="OB39" s="0"/>
-      <c r="OC39" s="0"/>
-      <c r="OD39" s="0"/>
-      <c r="OE39" s="0"/>
-      <c r="OF39" s="0"/>
-      <c r="OG39" s="0"/>
-      <c r="OH39" s="0"/>
-      <c r="OI39" s="0"/>
-      <c r="OJ39" s="0"/>
-      <c r="OK39" s="0"/>
-      <c r="OL39" s="0"/>
-      <c r="OM39" s="0"/>
-      <c r="ON39" s="0"/>
-      <c r="OO39" s="0"/>
-      <c r="OP39" s="0"/>
-      <c r="OQ39" s="0"/>
-      <c r="OR39" s="0"/>
-      <c r="OS39" s="0"/>
-      <c r="OT39" s="0"/>
-      <c r="OU39" s="0"/>
-      <c r="OV39" s="0"/>
-      <c r="OW39" s="0"/>
-      <c r="OX39" s="0"/>
-      <c r="OY39" s="0"/>
-      <c r="OZ39" s="0"/>
-      <c r="PA39" s="0"/>
-      <c r="PB39" s="0"/>
-      <c r="PC39" s="0"/>
-      <c r="PD39" s="0"/>
-      <c r="PE39" s="0"/>
-      <c r="PF39" s="0"/>
-      <c r="PG39" s="0"/>
-      <c r="PH39" s="0"/>
-      <c r="PI39" s="0"/>
-      <c r="PJ39" s="0"/>
-      <c r="PK39" s="0"/>
-      <c r="PL39" s="0"/>
-      <c r="PM39" s="0"/>
-      <c r="PN39" s="0"/>
-      <c r="PO39" s="0"/>
-      <c r="PP39" s="0"/>
-      <c r="PQ39" s="0"/>
-      <c r="PR39" s="0"/>
-      <c r="PS39" s="0"/>
-      <c r="PT39" s="0"/>
-      <c r="PU39" s="0"/>
-      <c r="PV39" s="0"/>
-      <c r="PW39" s="0"/>
-      <c r="PX39" s="0"/>
-      <c r="PY39" s="0"/>
-      <c r="PZ39" s="0"/>
-      <c r="QA39" s="0"/>
-      <c r="QB39" s="0"/>
-      <c r="QC39" s="0"/>
-      <c r="QD39" s="0"/>
-      <c r="QE39" s="0"/>
-      <c r="QF39" s="0"/>
-      <c r="QG39" s="0"/>
-      <c r="QH39" s="0"/>
-      <c r="QI39" s="0"/>
-      <c r="QJ39" s="0"/>
-      <c r="QK39" s="0"/>
-      <c r="QL39" s="0"/>
-      <c r="QM39" s="0"/>
-      <c r="QN39" s="0"/>
-      <c r="QO39" s="0"/>
-      <c r="QP39" s="0"/>
-      <c r="QQ39" s="0"/>
-      <c r="QR39" s="0"/>
-      <c r="QS39" s="0"/>
-      <c r="QT39" s="0"/>
-      <c r="QU39" s="0"/>
-      <c r="QV39" s="0"/>
-      <c r="QW39" s="0"/>
-      <c r="QX39" s="0"/>
-      <c r="QY39" s="0"/>
-      <c r="QZ39" s="0"/>
-      <c r="RA39" s="0"/>
-      <c r="RB39" s="0"/>
-      <c r="RC39" s="0"/>
-      <c r="RD39" s="0"/>
-      <c r="RE39" s="0"/>
-      <c r="RF39" s="0"/>
-      <c r="RG39" s="0"/>
-      <c r="RH39" s="0"/>
-      <c r="RI39" s="0"/>
-      <c r="RJ39" s="0"/>
-      <c r="RK39" s="0"/>
-      <c r="RL39" s="0"/>
-      <c r="RM39" s="0"/>
-      <c r="RN39" s="0"/>
-      <c r="RO39" s="0"/>
-      <c r="RP39" s="0"/>
-      <c r="RQ39" s="0"/>
-      <c r="RR39" s="0"/>
-      <c r="RS39" s="0"/>
-      <c r="RT39" s="0"/>
-      <c r="RU39" s="0"/>
-      <c r="RV39" s="0"/>
-      <c r="RW39" s="0"/>
-      <c r="RX39" s="0"/>
-      <c r="RY39" s="0"/>
-      <c r="RZ39" s="0"/>
-      <c r="SA39" s="0"/>
-      <c r="SB39" s="0"/>
-      <c r="SC39" s="0"/>
-      <c r="SD39" s="0"/>
-      <c r="SE39" s="0"/>
-      <c r="SF39" s="0"/>
-      <c r="SG39" s="0"/>
-      <c r="SH39" s="0"/>
-      <c r="SI39" s="0"/>
-      <c r="SJ39" s="0"/>
-      <c r="SK39" s="0"/>
-      <c r="SL39" s="0"/>
-      <c r="SM39" s="0"/>
-      <c r="SN39" s="0"/>
-      <c r="SO39" s="0"/>
-      <c r="SP39" s="0"/>
-      <c r="SQ39" s="0"/>
-      <c r="SR39" s="0"/>
-      <c r="SS39" s="0"/>
-      <c r="ST39" s="0"/>
-      <c r="SU39" s="0"/>
-      <c r="SV39" s="0"/>
-      <c r="SW39" s="0"/>
-      <c r="SX39" s="0"/>
-      <c r="SY39" s="0"/>
-      <c r="SZ39" s="0"/>
-      <c r="TA39" s="0"/>
-      <c r="TB39" s="0"/>
-      <c r="TC39" s="0"/>
-      <c r="TD39" s="0"/>
-      <c r="TE39" s="0"/>
-      <c r="TF39" s="0"/>
-      <c r="TG39" s="0"/>
-      <c r="TH39" s="0"/>
-      <c r="TI39" s="0"/>
-      <c r="TJ39" s="0"/>
-      <c r="TK39" s="0"/>
-      <c r="TL39" s="0"/>
-      <c r="TM39" s="0"/>
-      <c r="TN39" s="0"/>
-      <c r="TO39" s="0"/>
-      <c r="TP39" s="0"/>
-      <c r="TQ39" s="0"/>
-      <c r="TR39" s="0"/>
-      <c r="TS39" s="0"/>
-      <c r="TT39" s="0"/>
-      <c r="TU39" s="0"/>
-      <c r="TV39" s="0"/>
-      <c r="TW39" s="0"/>
-      <c r="TX39" s="0"/>
-      <c r="TY39" s="0"/>
-      <c r="TZ39" s="0"/>
-      <c r="UA39" s="0"/>
-      <c r="UB39" s="0"/>
-      <c r="UC39" s="0"/>
-      <c r="UD39" s="0"/>
-      <c r="UE39" s="0"/>
-      <c r="UF39" s="0"/>
-      <c r="UG39" s="0"/>
-      <c r="UH39" s="0"/>
-      <c r="UI39" s="0"/>
-      <c r="UJ39" s="0"/>
-      <c r="UK39" s="0"/>
-      <c r="UL39" s="0"/>
-      <c r="UM39" s="0"/>
-      <c r="UN39" s="0"/>
-      <c r="UO39" s="0"/>
-      <c r="UP39" s="0"/>
-      <c r="UQ39" s="0"/>
-      <c r="UR39" s="0"/>
-      <c r="US39" s="0"/>
-      <c r="UT39" s="0"/>
-      <c r="UU39" s="0"/>
-      <c r="UV39" s="0"/>
-      <c r="UW39" s="0"/>
-      <c r="UX39" s="0"/>
-      <c r="UY39" s="0"/>
-      <c r="UZ39" s="0"/>
-      <c r="VA39" s="0"/>
-      <c r="VB39" s="0"/>
-      <c r="VC39" s="0"/>
-      <c r="VD39" s="0"/>
-      <c r="VE39" s="0"/>
-      <c r="VF39" s="0"/>
-      <c r="VG39" s="0"/>
-      <c r="VH39" s="0"/>
-      <c r="VI39" s="0"/>
-      <c r="VJ39" s="0"/>
-      <c r="VK39" s="0"/>
-      <c r="VL39" s="0"/>
-      <c r="VM39" s="0"/>
-      <c r="VN39" s="0"/>
-      <c r="VO39" s="0"/>
-      <c r="VP39" s="0"/>
-      <c r="VQ39" s="0"/>
-      <c r="VR39" s="0"/>
-      <c r="VS39" s="0"/>
-      <c r="VT39" s="0"/>
-      <c r="VU39" s="0"/>
-      <c r="VV39" s="0"/>
-      <c r="VW39" s="0"/>
-      <c r="VX39" s="0"/>
-      <c r="VY39" s="0"/>
-      <c r="VZ39" s="0"/>
-      <c r="WA39" s="0"/>
-      <c r="WB39" s="0"/>
-      <c r="WC39" s="0"/>
-      <c r="WD39" s="0"/>
-      <c r="WE39" s="0"/>
-      <c r="WF39" s="0"/>
-      <c r="WG39" s="0"/>
-      <c r="WH39" s="0"/>
-      <c r="WI39" s="0"/>
-      <c r="WJ39" s="0"/>
-      <c r="WK39" s="0"/>
-      <c r="WL39" s="0"/>
-      <c r="WM39" s="0"/>
-      <c r="WN39" s="0"/>
-      <c r="WO39" s="0"/>
-      <c r="WP39" s="0"/>
-      <c r="WQ39" s="0"/>
-      <c r="WR39" s="0"/>
-      <c r="WS39" s="0"/>
-      <c r="WT39" s="0"/>
-      <c r="WU39" s="0"/>
-      <c r="WV39" s="0"/>
-      <c r="WW39" s="0"/>
-      <c r="WX39" s="0"/>
-      <c r="WY39" s="0"/>
-      <c r="WZ39" s="0"/>
-      <c r="XA39" s="0"/>
-      <c r="XB39" s="0"/>
-      <c r="XC39" s="0"/>
-      <c r="XD39" s="0"/>
-      <c r="XE39" s="0"/>
-      <c r="XF39" s="0"/>
-      <c r="XG39" s="0"/>
-      <c r="XH39" s="0"/>
-      <c r="XI39" s="0"/>
-      <c r="XJ39" s="0"/>
-      <c r="XK39" s="0"/>
-      <c r="XL39" s="0"/>
-      <c r="XM39" s="0"/>
-      <c r="XN39" s="0"/>
-      <c r="XO39" s="0"/>
-      <c r="XP39" s="0"/>
-      <c r="XQ39" s="0"/>
-      <c r="XR39" s="0"/>
-      <c r="XS39" s="0"/>
-      <c r="XT39" s="0"/>
-      <c r="XU39" s="0"/>
-      <c r="XV39" s="0"/>
-      <c r="XW39" s="0"/>
-      <c r="XX39" s="0"/>
-      <c r="XY39" s="0"/>
-      <c r="XZ39" s="0"/>
-      <c r="YA39" s="0"/>
-      <c r="YB39" s="0"/>
-      <c r="YC39" s="0"/>
-      <c r="YD39" s="0"/>
-      <c r="YE39" s="0"/>
-      <c r="YF39" s="0"/>
-      <c r="YG39" s="0"/>
-      <c r="YH39" s="0"/>
-      <c r="YI39" s="0"/>
-      <c r="YJ39" s="0"/>
-      <c r="YK39" s="0"/>
-      <c r="YL39" s="0"/>
-      <c r="YM39" s="0"/>
-      <c r="YN39" s="0"/>
-      <c r="YO39" s="0"/>
-      <c r="YP39" s="0"/>
-      <c r="YQ39" s="0"/>
-      <c r="YR39" s="0"/>
-      <c r="YS39" s="0"/>
-      <c r="YT39" s="0"/>
-      <c r="YU39" s="0"/>
-      <c r="YV39" s="0"/>
-      <c r="YW39" s="0"/>
-      <c r="YX39" s="0"/>
-      <c r="YY39" s="0"/>
-      <c r="YZ39" s="0"/>
-      <c r="ZA39" s="0"/>
-      <c r="ZB39" s="0"/>
-      <c r="ZC39" s="0"/>
-      <c r="ZD39" s="0"/>
-      <c r="ZE39" s="0"/>
-      <c r="ZF39" s="0"/>
-      <c r="ZG39" s="0"/>
-      <c r="ZH39" s="0"/>
-      <c r="ZI39" s="0"/>
-      <c r="ZJ39" s="0"/>
-      <c r="ZK39" s="0"/>
-      <c r="ZL39" s="0"/>
-      <c r="ZM39" s="0"/>
-      <c r="ZN39" s="0"/>
-      <c r="ZO39" s="0"/>
-      <c r="ZP39" s="0"/>
-      <c r="ZQ39" s="0"/>
-      <c r="ZR39" s="0"/>
-      <c r="ZS39" s="0"/>
-      <c r="ZT39" s="0"/>
-      <c r="ZU39" s="0"/>
-      <c r="ZV39" s="0"/>
-      <c r="ZW39" s="0"/>
-      <c r="ZX39" s="0"/>
-      <c r="ZY39" s="0"/>
-      <c r="ZZ39" s="0"/>
-      <c r="AAA39" s="0"/>
-      <c r="AAB39" s="0"/>
-      <c r="AAC39" s="0"/>
-      <c r="AAD39" s="0"/>
-      <c r="AAE39" s="0"/>
-      <c r="AAF39" s="0"/>
-      <c r="AAG39" s="0"/>
-      <c r="AAH39" s="0"/>
-      <c r="AAI39" s="0"/>
-      <c r="AAJ39" s="0"/>
-      <c r="AAK39" s="0"/>
-      <c r="AAL39" s="0"/>
-      <c r="AAM39" s="0"/>
-      <c r="AAN39" s="0"/>
-      <c r="AAO39" s="0"/>
-      <c r="AAP39" s="0"/>
-      <c r="AAQ39" s="0"/>
-      <c r="AAR39" s="0"/>
-      <c r="AAS39" s="0"/>
-      <c r="AAT39" s="0"/>
-      <c r="AAU39" s="0"/>
-      <c r="AAV39" s="0"/>
-      <c r="AAW39" s="0"/>
-      <c r="AAX39" s="0"/>
-      <c r="AAY39" s="0"/>
-      <c r="AAZ39" s="0"/>
-      <c r="ABA39" s="0"/>
-      <c r="ABB39" s="0"/>
-      <c r="ABC39" s="0"/>
-      <c r="ABD39" s="0"/>
-      <c r="ABE39" s="0"/>
-      <c r="ABF39" s="0"/>
-      <c r="ABG39" s="0"/>
-      <c r="ABH39" s="0"/>
-      <c r="ABI39" s="0"/>
-      <c r="ABJ39" s="0"/>
-      <c r="ABK39" s="0"/>
-      <c r="ABL39" s="0"/>
-      <c r="ABM39" s="0"/>
-      <c r="ABN39" s="0"/>
-      <c r="ABO39" s="0"/>
-      <c r="ABP39" s="0"/>
-      <c r="ABQ39" s="0"/>
-      <c r="ABR39" s="0"/>
-      <c r="ABS39" s="0"/>
-      <c r="ABT39" s="0"/>
-      <c r="ABU39" s="0"/>
-      <c r="ABV39" s="0"/>
-      <c r="ABW39" s="0"/>
-      <c r="ABX39" s="0"/>
-      <c r="ABY39" s="0"/>
-      <c r="ABZ39" s="0"/>
-      <c r="ACA39" s="0"/>
-      <c r="ACB39" s="0"/>
-      <c r="ACC39" s="0"/>
-      <c r="ACD39" s="0"/>
-      <c r="ACE39" s="0"/>
-      <c r="ACF39" s="0"/>
-      <c r="ACG39" s="0"/>
-      <c r="ACH39" s="0"/>
-      <c r="ACI39" s="0"/>
-      <c r="ACJ39" s="0"/>
-      <c r="ACK39" s="0"/>
-      <c r="ACL39" s="0"/>
-      <c r="ACM39" s="0"/>
-      <c r="ACN39" s="0"/>
-      <c r="ACO39" s="0"/>
-      <c r="ACP39" s="0"/>
-      <c r="ACQ39" s="0"/>
-      <c r="ACR39" s="0"/>
-      <c r="ACS39" s="0"/>
-      <c r="ACT39" s="0"/>
-      <c r="ACU39" s="0"/>
-      <c r="ACV39" s="0"/>
-      <c r="ACW39" s="0"/>
-      <c r="ACX39" s="0"/>
-      <c r="ACY39" s="0"/>
-      <c r="ACZ39" s="0"/>
-      <c r="ADA39" s="0"/>
-      <c r="ADB39" s="0"/>
-      <c r="ADC39" s="0"/>
-      <c r="ADD39" s="0"/>
-      <c r="ADE39" s="0"/>
-      <c r="ADF39" s="0"/>
-      <c r="ADG39" s="0"/>
-      <c r="ADH39" s="0"/>
-      <c r="ADI39" s="0"/>
-      <c r="ADJ39" s="0"/>
-      <c r="ADK39" s="0"/>
-      <c r="ADL39" s="0"/>
-      <c r="ADM39" s="0"/>
-      <c r="ADN39" s="0"/>
-      <c r="ADO39" s="0"/>
-      <c r="ADP39" s="0"/>
-      <c r="ADQ39" s="0"/>
-      <c r="ADR39" s="0"/>
-      <c r="ADS39" s="0"/>
-      <c r="ADT39" s="0"/>
-      <c r="ADU39" s="0"/>
-      <c r="ADV39" s="0"/>
-      <c r="ADW39" s="0"/>
-      <c r="ADX39" s="0"/>
-      <c r="ADY39" s="0"/>
-      <c r="ADZ39" s="0"/>
-      <c r="AEA39" s="0"/>
-      <c r="AEB39" s="0"/>
-      <c r="AEC39" s="0"/>
-      <c r="AED39" s="0"/>
-      <c r="AEE39" s="0"/>
-      <c r="AEF39" s="0"/>
-      <c r="AEG39" s="0"/>
-      <c r="AEH39" s="0"/>
-      <c r="AEI39" s="0"/>
-      <c r="AEJ39" s="0"/>
-      <c r="AEK39" s="0"/>
-      <c r="AEL39" s="0"/>
-      <c r="AEM39" s="0"/>
-      <c r="AEN39" s="0"/>
-      <c r="AEO39" s="0"/>
-      <c r="AEP39" s="0"/>
-      <c r="AEQ39" s="0"/>
-      <c r="AER39" s="0"/>
-      <c r="AES39" s="0"/>
-      <c r="AET39" s="0"/>
-      <c r="AEU39" s="0"/>
-      <c r="AEV39" s="0"/>
-      <c r="AEW39" s="0"/>
-      <c r="AEX39" s="0"/>
-      <c r="AEY39" s="0"/>
-      <c r="AEZ39" s="0"/>
-      <c r="AFA39" s="0"/>
-      <c r="AFB39" s="0"/>
-      <c r="AFC39" s="0"/>
-      <c r="AFD39" s="0"/>
-      <c r="AFE39" s="0"/>
-      <c r="AFF39" s="0"/>
-      <c r="AFG39" s="0"/>
-      <c r="AFH39" s="0"/>
-      <c r="AFI39" s="0"/>
-      <c r="AFJ39" s="0"/>
-      <c r="AFK39" s="0"/>
-      <c r="AFL39" s="0"/>
-      <c r="AFM39" s="0"/>
-      <c r="AFN39" s="0"/>
-      <c r="AFO39" s="0"/>
-      <c r="AFP39" s="0"/>
-      <c r="AFQ39" s="0"/>
-      <c r="AFR39" s="0"/>
-      <c r="AFS39" s="0"/>
-      <c r="AFT39" s="0"/>
-      <c r="AFU39" s="0"/>
-      <c r="AFV39" s="0"/>
-      <c r="AFW39" s="0"/>
-      <c r="AFX39" s="0"/>
-      <c r="AFY39" s="0"/>
-      <c r="AFZ39" s="0"/>
-      <c r="AGA39" s="0"/>
-      <c r="AGB39" s="0"/>
-      <c r="AGC39" s="0"/>
-      <c r="AGD39" s="0"/>
-      <c r="AGE39" s="0"/>
-      <c r="AGF39" s="0"/>
-      <c r="AGG39" s="0"/>
-      <c r="AGH39" s="0"/>
-      <c r="AGI39" s="0"/>
-      <c r="AGJ39" s="0"/>
-      <c r="AGK39" s="0"/>
-      <c r="AGL39" s="0"/>
-      <c r="AGM39" s="0"/>
-      <c r="AGN39" s="0"/>
-      <c r="AGO39" s="0"/>
-      <c r="AGP39" s="0"/>
-      <c r="AGQ39" s="0"/>
-      <c r="AGR39" s="0"/>
-      <c r="AGS39" s="0"/>
-      <c r="AGT39" s="0"/>
-      <c r="AGU39" s="0"/>
-      <c r="AGV39" s="0"/>
-      <c r="AGW39" s="0"/>
-      <c r="AGX39" s="0"/>
-      <c r="AGY39" s="0"/>
-      <c r="AGZ39" s="0"/>
-      <c r="AHA39" s="0"/>
-      <c r="AHB39" s="0"/>
-      <c r="AHC39" s="0"/>
-      <c r="AHD39" s="0"/>
-      <c r="AHE39" s="0"/>
-      <c r="AHF39" s="0"/>
-      <c r="AHG39" s="0"/>
-      <c r="AHH39" s="0"/>
-      <c r="AHI39" s="0"/>
-      <c r="AHJ39" s="0"/>
-      <c r="AHK39" s="0"/>
-      <c r="AHL39" s="0"/>
-      <c r="AHM39" s="0"/>
-      <c r="AHN39" s="0"/>
-      <c r="AHO39" s="0"/>
-      <c r="AHP39" s="0"/>
-      <c r="AHQ39" s="0"/>
-      <c r="AHR39" s="0"/>
-      <c r="AHS39" s="0"/>
-      <c r="AHT39" s="0"/>
-      <c r="AHU39" s="0"/>
-      <c r="AHV39" s="0"/>
-      <c r="AHW39" s="0"/>
-      <c r="AHX39" s="0"/>
-      <c r="AHY39" s="0"/>
-      <c r="AHZ39" s="0"/>
-      <c r="AIA39" s="0"/>
-      <c r="AIB39" s="0"/>
-      <c r="AIC39" s="0"/>
-      <c r="AID39" s="0"/>
-      <c r="AIE39" s="0"/>
-      <c r="AIF39" s="0"/>
-      <c r="AIG39" s="0"/>
-      <c r="AIH39" s="0"/>
-      <c r="AII39" s="0"/>
-      <c r="AIJ39" s="0"/>
-      <c r="AIK39" s="0"/>
-      <c r="AIL39" s="0"/>
-      <c r="AIM39" s="0"/>
-      <c r="AIN39" s="0"/>
-      <c r="AIO39" s="0"/>
-      <c r="AIP39" s="0"/>
-      <c r="AIQ39" s="0"/>
-      <c r="AIR39" s="0"/>
-      <c r="AIS39" s="0"/>
-      <c r="AIT39" s="0"/>
-      <c r="AIU39" s="0"/>
-      <c r="AIV39" s="0"/>
-      <c r="AIW39" s="0"/>
-      <c r="AIX39" s="0"/>
-      <c r="AIY39" s="0"/>
-      <c r="AIZ39" s="0"/>
-      <c r="AJA39" s="0"/>
-      <c r="AJB39" s="0"/>
-      <c r="AJC39" s="0"/>
-      <c r="AJD39" s="0"/>
-      <c r="AJE39" s="0"/>
-      <c r="AJF39" s="0"/>
-      <c r="AJG39" s="0"/>
-      <c r="AJH39" s="0"/>
-      <c r="AJI39" s="0"/>
-      <c r="AJJ39" s="0"/>
-      <c r="AJK39" s="0"/>
-      <c r="AJL39" s="0"/>
-      <c r="AJM39" s="0"/>
-      <c r="AJN39" s="0"/>
-      <c r="AJO39" s="0"/>
-      <c r="AJP39" s="0"/>
-      <c r="AJQ39" s="0"/>
-      <c r="AJR39" s="0"/>
-      <c r="AJS39" s="0"/>
-      <c r="AJT39" s="0"/>
-      <c r="AJU39" s="0"/>
-      <c r="AJV39" s="0"/>
-      <c r="AJW39" s="0"/>
-      <c r="AJX39" s="0"/>
-      <c r="AJY39" s="0"/>
-      <c r="AJZ39" s="0"/>
-      <c r="AKA39" s="0"/>
-      <c r="AKB39" s="0"/>
-      <c r="AKC39" s="0"/>
-      <c r="AKD39" s="0"/>
-      <c r="AKE39" s="0"/>
-      <c r="AKF39" s="0"/>
-      <c r="AKG39" s="0"/>
-      <c r="AKH39" s="0"/>
-      <c r="AKI39" s="0"/>
-      <c r="AKJ39" s="0"/>
-      <c r="AKK39" s="0"/>
-      <c r="AKL39" s="0"/>
-      <c r="AKM39" s="0"/>
-      <c r="AKN39" s="0"/>
-      <c r="AKO39" s="0"/>
-      <c r="AKP39" s="0"/>
-      <c r="AKQ39" s="0"/>
-      <c r="AKR39" s="0"/>
-      <c r="AKS39" s="0"/>
-      <c r="AKT39" s="0"/>
-      <c r="AKU39" s="0"/>
-      <c r="AKV39" s="0"/>
-      <c r="AKW39" s="0"/>
-      <c r="AKX39" s="0"/>
-      <c r="AKY39" s="0"/>
-      <c r="AKZ39" s="0"/>
-      <c r="ALA39" s="0"/>
-      <c r="ALB39" s="0"/>
-      <c r="ALC39" s="0"/>
-      <c r="ALD39" s="0"/>
-      <c r="ALE39" s="0"/>
-      <c r="ALF39" s="0"/>
-      <c r="ALG39" s="0"/>
-      <c r="ALH39" s="0"/>
-      <c r="ALI39" s="0"/>
-      <c r="ALJ39" s="0"/>
-      <c r="ALK39" s="0"/>
-      <c r="ALL39" s="0"/>
-      <c r="ALM39" s="0"/>
-      <c r="ALN39" s="0"/>
-      <c r="ALO39" s="0"/>
-      <c r="ALP39" s="0"/>
-      <c r="ALQ39" s="0"/>
-      <c r="ALR39" s="0"/>
-      <c r="ALS39" s="0"/>
-      <c r="ALT39" s="0"/>
-      <c r="ALU39" s="0"/>
-      <c r="ALV39" s="0"/>
-      <c r="ALW39" s="0"/>
-      <c r="ALX39" s="0"/>
-      <c r="ALY39" s="0"/>
-      <c r="ALZ39" s="0"/>
-      <c r="AMA39" s="0"/>
-      <c r="AMB39" s="0"/>
-      <c r="AMC39" s="0"/>
-      <c r="AMD39" s="0"/>
-      <c r="AME39" s="0"/>
-      <c r="AMF39" s="0"/>
-      <c r="AMG39" s="0"/>
-      <c r="AMH39" s="0"/>
-      <c r="AMI39" s="0"/>
-      <c r="AMJ39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -19991,6 +19027,258 @@
       <c r="V41" s="52"/>
       <c r="W41" s="53"/>
     </row>
+    <row r="42" s="57" customFormat="true" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="50" t="n">
+        <v>44447</v>
+      </c>
+      <c r="B42" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="C42" s="52" t="s">
+        <v>289</v>
+      </c>
+      <c r="D42" s="52" t="s">
+        <v>290</v>
+      </c>
+      <c r="E42" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F42" s="53" t="s">
+        <v>291</v>
+      </c>
+      <c r="G42" s="53" t="s">
+        <v>292</v>
+      </c>
+      <c r="H42" s="54" t="n">
+        <v>29980</v>
+      </c>
+      <c r="I42" s="54" t="n">
+        <v>29980</v>
+      </c>
+      <c r="J42" s="55" t="n">
+        <v>43821</v>
+      </c>
+      <c r="K42" s="56" t="n">
+        <v>29</v>
+      </c>
+      <c r="L42" s="50" t="s">
+        <v>293</v>
+      </c>
+      <c r="M42" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="N42" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="O42" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="P42" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q42" s="52" t="s">
+        <v>294</v>
+      </c>
+      <c r="R42" s="52" t="s">
+        <v>295</v>
+      </c>
+      <c r="S42" s="52" t="s">
+        <v>296</v>
+      </c>
+      <c r="T42" s="52"/>
+      <c r="U42" s="53"/>
+      <c r="V42" s="52"/>
+      <c r="W42" s="53"/>
+    </row>
+    <row r="43" s="57" customFormat="true" ht="15.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="50" t="n">
+        <v>15219</v>
+      </c>
+      <c r="B43" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="52" t="s">
+        <v>37</v>
+      </c>
+      <c r="D43" s="52" t="s">
+        <v>38</v>
+      </c>
+      <c r="E43" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F43" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="G43" s="53" t="s">
+        <v>41</v>
+      </c>
+      <c r="H43" s="54" t="n">
+        <v>18429</v>
+      </c>
+      <c r="I43" s="54" t="n">
+        <v>18429</v>
+      </c>
+      <c r="J43" s="55" t="n">
+        <v>44926</v>
+      </c>
+      <c r="K43" s="56" t="n">
+        <v>68</v>
+      </c>
+      <c r="L43" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="M43" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="N43" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="O43" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="P43" s="53" t="s">
+        <v>44</v>
+      </c>
+      <c r="Q43" s="52" t="s">
+        <v>45</v>
+      </c>
+      <c r="R43" s="52" t="s">
+        <v>46</v>
+      </c>
+      <c r="S43" s="52" t="s">
+        <v>47</v>
+      </c>
+      <c r="T43" s="52"/>
+      <c r="U43" s="53"/>
+      <c r="V43" s="52"/>
+      <c r="W43" s="53"/>
+    </row>
+    <row r="44" s="57" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="50" t="n">
+        <v>39252</v>
+      </c>
+      <c r="B44" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="52" t="s">
+        <v>297</v>
+      </c>
+      <c r="D44" s="52" t="s">
+        <v>290</v>
+      </c>
+      <c r="E44" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F44" s="53" t="s">
+        <v>291</v>
+      </c>
+      <c r="G44" s="53" t="s">
+        <v>292</v>
+      </c>
+      <c r="H44" s="54" t="n">
+        <v>27529</v>
+      </c>
+      <c r="I44" s="54" t="n">
+        <v>27529</v>
+      </c>
+      <c r="J44" s="55" t="n">
+        <v>43821</v>
+      </c>
+      <c r="K44" s="56" t="n">
+        <v>31</v>
+      </c>
+      <c r="L44" s="50" t="s">
+        <v>52</v>
+      </c>
+      <c r="M44" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="N44" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="O44" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="P44" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q44" s="52" t="s">
+        <v>294</v>
+      </c>
+      <c r="R44" s="52" t="s">
+        <v>298</v>
+      </c>
+      <c r="S44" s="52" t="s">
+        <v>299</v>
+      </c>
+      <c r="T44" s="52"/>
+      <c r="U44" s="53"/>
+      <c r="V44" s="52"/>
+      <c r="W44" s="53"/>
+    </row>
+    <row r="45" s="57" customFormat="true" ht="15.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="50" t="n">
+        <v>39252</v>
+      </c>
+      <c r="B45" s="51" t="n">
+        <v>1</v>
+      </c>
+      <c r="C45" s="52" t="s">
+        <v>297</v>
+      </c>
+      <c r="D45" s="52" t="s">
+        <v>290</v>
+      </c>
+      <c r="E45" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="F45" s="53" t="s">
+        <v>291</v>
+      </c>
+      <c r="G45" s="53" t="s">
+        <v>292</v>
+      </c>
+      <c r="H45" s="54" t="n">
+        <v>27529</v>
+      </c>
+      <c r="I45" s="54" t="n">
+        <v>27529</v>
+      </c>
+      <c r="J45" s="55" t="n">
+        <v>43821</v>
+      </c>
+      <c r="K45" s="56" t="n">
+        <v>58</v>
+      </c>
+      <c r="L45" s="50" t="s">
+        <v>300</v>
+      </c>
+      <c r="M45" s="52" t="s">
+        <v>43</v>
+      </c>
+      <c r="N45" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="O45" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="P45" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="Q45" s="52" t="s">
+        <v>294</v>
+      </c>
+      <c r="R45" s="52" t="s">
+        <v>298</v>
+      </c>
+      <c r="S45" s="52" t="s">
+        <v>299</v>
+      </c>
+      <c r="T45" s="52"/>
+      <c r="U45" s="53"/>
+      <c r="V45" s="52"/>
+      <c r="W45" s="53"/>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A4:O4"/>

</xml_diff>